<commit_message>
Haciendo registro de usuarios
He creado un paquete nuevo usuarios en sustitución de login, en el que pondremos las operaciones de registro, login y todo lo que tenga que ver con el usuario.
También he creado la clase Registro y sus tests, que todavía no funcionan.
</commit_message>
<xml_diff>
--- a/documentacion/Tareas.xlsx
+++ b/documentacion/Tareas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique/GitHubProjects/RecetApp/documentacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B190124A-6565-8F42-9FCF-BB934391F3E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A5A0FB-0CD2-6D41-89FD-3A8FF32BD4E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="460" windowWidth="28400" windowHeight="19040" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
+    <workbookView xWindow="3580" yWindow="460" windowWidth="28400" windowHeight="18980" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -517,7 +517,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -549,7 +549,7 @@
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="9"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
@@ -579,6 +579,7 @@
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="C8" s="8"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">

</xml_diff>

<commit_message>
Actualización de las tareas
</commit_message>
<xml_diff>
--- a/documentacion/Tareas.xlsx
+++ b/documentacion/Tareas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique/GitHubProjects/RecetApp/documentacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A5A0FB-0CD2-6D41-89FD-3A8FF32BD4E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE3608C-F558-EA45-A97C-02DADBDE5585}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3580" yWindow="460" windowWidth="28400" windowHeight="18980" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>CREACIÓN DE UNA CUENTA</t>
   </si>
@@ -105,6 +105,15 @@
   </si>
   <si>
     <t>PRIORIDAD</t>
+  </si>
+  <si>
+    <t>ENCARGADO</t>
+  </si>
+  <si>
+    <t>HECHO</t>
+  </si>
+  <si>
+    <t>REALIZADO POR</t>
   </si>
 </sst>
 </file>
@@ -135,7 +144,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -166,6 +175,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -179,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -199,7 +220,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,19 +540,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66436974-768D-9A40-9A43-2F0986DDE03B}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="7"/>
     <col min="2" max="2" width="116.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>23</v>
       </c>
@@ -536,123 +564,139 @@
       <c r="C1" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="7">
+      <c r="D1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="9"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
+      <c r="C6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="10">
         <v>1</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C7" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="8"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C9" s="8"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="7">
+      <c r="C11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="10">
         <v>1</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C13" s="8"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="7">
+      <c r="C17" s="8"/>
+    </row>
+    <row r="18" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="10">
         <v>1</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" s="8"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Actualización de las tareas de Enrique
</commit_message>
<xml_diff>
--- a/documentacion/Tareas.xlsx
+++ b/documentacion/Tareas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique/GitHubProjects/RecetApp/documentacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE3608C-F558-EA45-A97C-02DADBDE5585}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C30339E-1B47-F84D-9467-F3FB390133C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3580" yWindow="460" windowWidth="28400" windowHeight="18980" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>CREACIÓN DE UNA CUENTA</t>
   </si>
@@ -71,12 +71,6 @@
     <t>Diseñar una tabla en la base de datos donde guardar los alimentos</t>
   </si>
   <si>
-    <t>Buscar una base de datos con alimentos y volcarla en la base de datos</t>
-  </si>
-  <si>
-    <t>Crear una interfaz que le permita al usuario buscar y seleccionar ingredientes</t>
-  </si>
-  <si>
     <t>Guardar la selección de ingredientes en la base de datos</t>
   </si>
   <si>
@@ -89,15 +83,6 @@
     <t>Diseñar y crear tablas en la base de datos para guardar recetas</t>
   </si>
   <si>
-    <t>Guardar recetas. Buscar bbdd para volcarla en la nuestra</t>
-  </si>
-  <si>
-    <t>Programar una opción para buscar las coincidencias entre la tabla con los ingredientes del usuario y los de las recetas. Diseñar y escribir las consultas</t>
-  </si>
-  <si>
-    <t>Mostrar en pantalla las coincidencias</t>
-  </si>
-  <si>
     <t>TAREAS</t>
   </si>
   <si>
@@ -113,14 +98,56 @@
     <t>HECHO</t>
   </si>
   <si>
-    <t>REALIZADO POR</t>
+    <t>TIEMPO ESTIMADO</t>
+  </si>
+  <si>
+    <t>TIEMPO INVERTIDO</t>
+  </si>
+  <si>
+    <t>Enrique</t>
+  </si>
+  <si>
+    <t>Crear una interfaz que le permita al usuario buscar ingredientes</t>
+  </si>
+  <si>
+    <t>AGREGAR INGREDIENTES A LA BASE DE DATOS</t>
+  </si>
+  <si>
+    <t>Buscar una base de datos con alimentos</t>
+  </si>
+  <si>
+    <t>Volcar una bd con ingredientes en la nuestra / Agregarlos a mano</t>
+  </si>
+  <si>
+    <t>Crear una interfaz que permita al usuario indicar si quiere guardar el ingrediente buscado</t>
+  </si>
+  <si>
+    <t>GENERAR RECETAS</t>
+  </si>
+  <si>
+    <t>AÑADIR RECETAS A LA BASE DE DATOS</t>
+  </si>
+  <si>
+    <t>Buscar una base de datos con recetas</t>
+  </si>
+  <si>
+    <t>Guardar recetas volcando una bbdd o añadiendo a mano</t>
+  </si>
+  <si>
+    <t>Diseñar y escribir las consultas o algoritmo que permita buscar las coincidencias entre la tabla con los ingredientes del usuario y los de las recetas</t>
+  </si>
+  <si>
+    <t>Crear una opción en la interfaz de usuario para mostrar una lista de recetas con los ingredientes de que dispone el usuario</t>
+  </si>
+  <si>
+    <t>Mostrar la lista de recetas por pantalla</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -137,6 +164,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -200,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -226,6 +261,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66436974-768D-9A40-9A43-2F0986DDE03B}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -551,27 +592,31 @@
     <col min="1" max="1" width="10.83203125" style="7"/>
     <col min="2" max="2" width="116.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="F1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -579,30 +624,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="8"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="8"/>
     </row>
-    <row r="7" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="10">
         <v>1</v>
       </c>
@@ -610,95 +655,152 @@
         <v>5</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="8"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="8"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="8"/>
     </row>
-    <row r="12" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10">
         <v>1</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D12" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="8"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="C14" s="15"/>
+    </row>
+    <row r="15" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="10">
+        <v>1</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="8"/>
-    </row>
-    <row r="18" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10">
         <v>1</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C19" s="8"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="C20" s="15"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B22" s="2" t="s">
-        <v>20</v>
+        <v>12</v>
+      </c>
+      <c r="C21" s="15"/>
+    </row>
+    <row r="22" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="10">
+        <v>1</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="14"/>
+      <c r="B23" s="16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="14"/>
+      <c r="B24" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="14"/>
+      <c r="B25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="8"/>
+    </row>
+    <row r="26" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="10">
+        <v>1</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="8"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B28" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B29" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización de tareas de Enrique
</commit_message>
<xml_diff>
--- a/documentacion/Tareas.xlsx
+++ b/documentacion/Tareas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique/GitHubProjects/RecetApp/documentacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C30339E-1B47-F84D-9467-F3FB390133C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC01699-01C6-EC4B-B88F-AA2B6154BF59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3580" yWindow="460" windowWidth="28400" windowHeight="18980" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>CREACIÓN DE UNA CUENTA</t>
   </si>
@@ -119,9 +119,6 @@
     <t>Volcar una bd con ingredientes en la nuestra / Agregarlos a mano</t>
   </si>
   <si>
-    <t>Crear una interfaz que permita al usuario indicar si quiere guardar el ingrediente buscado</t>
-  </si>
-  <si>
     <t>GENERAR RECETAS</t>
   </si>
   <si>
@@ -141,6 +138,15 @@
   </si>
   <si>
     <t>Mostrar la lista de recetas por pantalla</t>
+  </si>
+  <si>
+    <t>1 hora</t>
+  </si>
+  <si>
+    <t>0,5 horas</t>
+  </si>
+  <si>
+    <t>2 horas</t>
   </si>
 </sst>
 </file>
@@ -581,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66436974-768D-9A40-9A43-2F0986DDE03B}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -689,8 +695,17 @@
       <c r="B12" s="11" t="s">
         <v>10</v>
       </c>
+      <c r="C12" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="D12" s="12" t="s">
         <v>23</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -703,7 +718,7 @@
       <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="15"/>
+      <c r="C14" s="8"/>
     </row>
     <row r="15" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="10">
@@ -718,89 +733,92 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10">
         <v>1</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>14</v>
       </c>
+      <c r="C18" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="D18" s="12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="8"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="15"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="15"/>
-    </row>
-    <row r="22" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="10">
+      <c r="C20" s="8"/>
+    </row>
+    <row r="21" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="10">
         <v>1</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B21" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="14"/>
+      <c r="B22" s="16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="14"/>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="14"/>
       <c r="B24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="8"/>
+    </row>
+    <row r="25" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="10">
+        <v>1</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B26" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="8"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B27" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="14"/>
-      <c r="B25" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="8"/>
-    </row>
-    <row r="26" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="10">
-        <v>1</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="2" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B28" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="C27" s="8"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B28" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualizando la tabla de tareas y escogiendo algunas
</commit_message>
<xml_diff>
--- a/documentacion/Tareas.xlsx
+++ b/documentacion/Tareas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique/GitHubProjects/RecetApp/documentacion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/481f6a27916b9a84/Documentos/RecetApp/documentacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC01699-01C6-EC4B-B88F-AA2B6154BF59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{0EC01699-01C6-EC4B-B88F-AA2B6154BF59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D281C823-C26A-4917-906E-6AD564762170}"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="460" windowWidth="28400" windowHeight="18980" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t>CREACIÓN DE UNA CUENTA</t>
   </si>
@@ -147,6 +147,12 @@
   </si>
   <si>
     <t>2 horas</t>
+  </si>
+  <si>
+    <t>Mario</t>
+  </si>
+  <si>
+    <t>20 min</t>
   </si>
 </sst>
 </file>
@@ -589,20 +595,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66436974-768D-9A40-9A43-2F0986DDE03B}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="7"/>
-    <col min="2" max="2" width="116.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.796875" style="7"/>
+    <col min="2" max="2" width="116.296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>18</v>
       </c>
@@ -622,7 +628,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -630,30 +636,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="8"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="8"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="8"/>
     </row>
-    <row r="7" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <v>1</v>
       </c>
@@ -664,31 +670,31 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="8"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="8"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="8"/>
     </row>
-    <row r="12" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
         <v>1</v>
       </c>
@@ -708,19 +714,19 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="8"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="8"/>
     </row>
-    <row r="15" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <v>1</v>
       </c>
@@ -728,17 +734,33 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C16" s="8"/>
+      <c r="D16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <v>1</v>
       </c>
@@ -758,19 +780,19 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="8"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="8"/>
     </row>
-    <row r="21" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10">
         <v>1</v>
       </c>
@@ -778,26 +800,26 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
       <c r="B24" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="8"/>
     </row>
-    <row r="25" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10">
         <v>1</v>
       </c>
@@ -805,18 +827,18 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C26" s="8"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
actualizando tracking y confirmando la realización de tareas de los registros de la tabla ingredientes
</commit_message>
<xml_diff>
--- a/documentacion/Tareas.xlsx
+++ b/documentacion/Tareas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/481f6a27916b9a84/Documentos/RecetApp/documentacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{0EC01699-01C6-EC4B-B88F-AA2B6154BF59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D281C823-C26A-4917-906E-6AD564762170}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{0EC01699-01C6-EC4B-B88F-AA2B6154BF59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9762F7ED-9406-4A08-8699-1BC2CA08ACB1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>CREACIÓN DE UNA CUENTA</t>
   </si>
@@ -596,7 +596,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -753,11 +753,15 @@
       <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="C17" s="8"/>
       <c r="D17" t="s">
         <v>38</v>
       </c>
       <c r="E17" t="s">
         <v>39</v>
+      </c>
+      <c r="F17" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Actualización encargados de tareas
</commit_message>
<xml_diff>
--- a/documentacion/Tareas.xlsx
+++ b/documentacion/Tareas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/481f6a27916b9a84/Documentos/RecetApp/documentacion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique/GitHubProjects/RecetApp/documentacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{0EC01699-01C6-EC4B-B88F-AA2B6154BF59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9762F7ED-9406-4A08-8699-1BC2CA08ACB1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06469AFD-3611-224C-95C3-ED3885AD121A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28160" windowHeight="16380" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
   <si>
     <t>CREACIÓN DE UNA CUENTA</t>
   </si>
@@ -153,13 +153,19 @@
   </si>
   <si>
     <t>20 min</t>
+  </si>
+  <si>
+    <t>José Manuel</t>
+  </si>
+  <si>
+    <t>Enrique, Mario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -186,6 +192,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -247,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -279,6 +292,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,20 +609,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66436974-768D-9A40-9A43-2F0986DDE03B}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.796875" style="7"/>
-    <col min="2" max="2" width="116.296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="7"/>
+    <col min="2" max="2" width="116.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>18</v>
       </c>
@@ -628,7 +642,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -636,30 +650,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="8"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="8"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="8"/>
-    </row>
-    <row r="7" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="10">
         <v>1</v>
       </c>
@@ -670,31 +693,43 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="8"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="8"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="8"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="8"/>
-    </row>
-    <row r="12" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10">
         <v>1</v>
       </c>
@@ -704,9 +739,6 @@
       <c r="C12" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="12" t="s">
-        <v>23</v>
-      </c>
       <c r="E12" s="12" t="s">
         <v>35</v>
       </c>
@@ -714,19 +746,25 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="8"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D13" s="17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="8"/>
-    </row>
-    <row r="15" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="10">
         <v>1</v>
       </c>
@@ -734,7 +772,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>26</v>
       </c>
@@ -749,7 +787,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
@@ -764,7 +802,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10">
         <v>1</v>
       </c>
@@ -774,9 +812,6 @@
       <c r="C18" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="12" t="s">
-        <v>23</v>
-      </c>
       <c r="E18" s="12" t="s">
         <v>35</v>
       </c>
@@ -784,19 +819,25 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="8"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="8"/>
-    </row>
-    <row r="21" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="10">
         <v>1</v>
       </c>
@@ -804,26 +845,29 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="14"/>
       <c r="B22" s="16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="14"/>
       <c r="B23" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="14"/>
       <c r="B24" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="8"/>
-    </row>
-    <row r="25" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D24" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10">
         <v>1</v>
       </c>
@@ -831,18 +875,21 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C26" s="8"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
Update de la hoja de planificación
</commit_message>
<xml_diff>
--- a/documentacion/Tareas.xlsx
+++ b/documentacion/Tareas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique/GitHubProjects/RecetApp/documentacion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Desktop\Universidad\4ºAño\ISO\RecetApp\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06469AFD-3611-224C-95C3-ED3885AD121A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D28585D-A86A-4F19-8209-2D31EE3AF892}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28160" windowHeight="16380" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="53">
   <si>
     <t>CREACIÓN DE UNA CUENTA</t>
   </si>
@@ -143,9 +143,6 @@
     <t>1 hora</t>
   </si>
   <si>
-    <t>0,5 horas</t>
-  </si>
-  <si>
     <t>2 horas</t>
   </si>
   <si>
@@ -159,15 +156,58 @@
   </si>
   <si>
     <t>Enrique, Mario</t>
+  </si>
+  <si>
+    <t>Búsqueda de información para conectar la base de datos a la aplicación</t>
+  </si>
+  <si>
+    <t>Enrique, Sergio</t>
+  </si>
+  <si>
+    <t>Escribir el código que permite conectar la base de datos a la aplicación</t>
+  </si>
+  <si>
+    <t>Búsqueda de información para realizar la tarea en el lenguaje GO</t>
+  </si>
+  <si>
+    <t>Enrique, Mario, Sergio, José Manuel, Elisa</t>
+  </si>
+  <si>
+    <t>Crear un dump que permita la creación de la tabla usuario</t>
+  </si>
+  <si>
+    <t>Crear un dump para crear la tabla de ingredientes</t>
+  </si>
+  <si>
+    <t>Crear un dump que cree la base de datos</t>
+  </si>
+  <si>
+    <t>Elisa</t>
+  </si>
+  <si>
+    <t>Sergio</t>
+  </si>
+  <si>
+    <t>Búsqueda de información para crear las consultas de las recetas</t>
+  </si>
+  <si>
+    <t>3 horas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -204,7 +244,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -247,6 +287,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -260,39 +306,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,22 +658,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66436974-768D-9A40-9A43-2F0986DDE03B}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="7"/>
-    <col min="2" max="2" width="116.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.796875" style="7"/>
+    <col min="2" max="2" width="116.296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.09765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>18</v>
       </c>
@@ -642,7 +693,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -650,248 +701,335 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="3" t="s">
-        <v>2</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="18" t="s">
+        <v>44</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B6" s="2" t="s">
-        <v>4</v>
+        <v>45</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="18" t="s">
+        <v>41</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="10">
-        <v>1</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="2" t="s">
-        <v>6</v>
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="18" t="s">
+        <v>46</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="8"/>
-      <c r="D11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="10">
+    <row r="11" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
         <v>1</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="12" t="s">
+      <c r="B11" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C13" s="8"/>
-      <c r="D13" s="17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="10">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10">
         <v>1</v>
       </c>
-      <c r="B15" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="8"/>
-      <c r="D16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" t="s">
-        <v>35</v>
-      </c>
-      <c r="F16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="C17" s="8"/>
-      <c r="D17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="10">
-        <v>1</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B19" s="2" t="s">
-        <v>13</v>
+      <c r="D17" s="17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B18" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B19" s="19" t="s">
+        <v>47</v>
       </c>
       <c r="C19" s="8"/>
-      <c r="D19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D19" s="17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10">
         <v>1</v>
       </c>
-      <c r="B21" s="13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
-      <c r="B22" s="16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="14"/>
+      <c r="B21" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="14"/>
-      <c r="B24" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="10">
+        <v>27</v>
+      </c>
+      <c r="C23" s="8"/>
+      <c r="D23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="10">
         <v>1</v>
       </c>
-      <c r="B25" s="13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B24" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="8"/>
+      <c r="D25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B27" s="2" t="s">
+    <row r="27" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="10">
+        <v>1</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="14"/>
+      <c r="B28" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="14"/>
+      <c r="B29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="14"/>
+      <c r="B30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="8"/>
+      <c r="D30" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="10">
+        <v>1</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B33" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="20"/>
+      <c r="D33" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B34" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B28" s="2" t="s">
+      <c r="D34" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B35" s="2" t="s">
         <v>34</v>
+      </c>
+      <c r="D35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E35" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update de las tareas
</commit_message>
<xml_diff>
--- a/documentacion/Tareas.xlsx
+++ b/documentacion/Tareas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Desktop\Universidad\4ºAño\ISO\RecetApp\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9326E9-0C30-41F1-BEF6-EE227FE153B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7B81A3-8BC2-429E-9BD9-6123171C26C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="62">
   <si>
     <t>CREACIÓN DE UNA CUENTA</t>
   </si>
@@ -198,15 +198,43 @@
   </si>
   <si>
     <t>1,5 horas</t>
+  </si>
+  <si>
+    <t>Validar que el dump creado se vuelca a la base de datos en distintos dispositivos</t>
+  </si>
+  <si>
+    <t>5 minutos</t>
+  </si>
+  <si>
+    <t>Validar que el login permite a un usuario ya creado acceder a la aplicación en distintos dispositivos</t>
+  </si>
+  <si>
+    <t>Validar que un usuario que ha accedido a la aplicación puede añadir ingresientes a su inventarop</t>
+  </si>
+  <si>
+    <t>Crear un dump para crear la tabla de guradado de ingredientes</t>
+  </si>
+  <si>
+    <t>Validar que se guardan los ingredientes en la base de datos</t>
+  </si>
+  <si>
+    <t>Validar que las consultas se realicen correctamente, de manera que, cuando un usuario introduzca sus ingredientes le salga la receta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -312,44 +340,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -664,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66436974-768D-9A40-9A43-2F0986DDE03B}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -780,57 +812,63 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="2" t="s">
-        <v>3</v>
+      <c r="B9" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10">
+      <c r="C11" s="8"/>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10">
         <v>1</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B12" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C12" s="12" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="8"/>
-      <c r="D12" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" t="s">
@@ -839,45 +877,51 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="10">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B17" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="10">
         <v>1</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B18" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C18" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="2" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="19" t="s">
-        <v>47</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="17" t="s">
@@ -885,53 +929,45 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="2" t="s">
-        <v>24</v>
+      <c r="B20" s="19" t="s">
+        <v>48</v>
       </c>
       <c r="C20" s="8"/>
-      <c r="D20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="10">
-        <v>1</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>20</v>
+      <c r="D20" s="17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B21" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="17" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="2" t="s">
-        <v>26</v>
+      <c r="B22" s="22" t="s">
+        <v>55</v>
       </c>
       <c r="C22" s="8"/>
-      <c r="D22" t="s">
-        <v>37</v>
+      <c r="D22" s="17" t="s">
+        <v>42</v>
       </c>
       <c r="E22" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="F22" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" t="s">
-        <v>37</v>
-      </c>
-      <c r="E23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F23" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -939,7 +975,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>20</v>
@@ -947,110 +983,217 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" t="s">
-        <v>23</v>
+        <v>37</v>
+      </c>
+      <c r="E25" t="s">
+        <v>35</v>
+      </c>
+      <c r="F25" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="10">
+        <v>37</v>
+      </c>
+      <c r="E26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B27" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="10">
         <v>1</v>
       </c>
-      <c r="B27" s="13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="14"/>
-      <c r="B28" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="14"/>
+      <c r="B28" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="14"/>
-      <c r="B30" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="C29" s="8"/>
+      <c r="D29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B30" s="22" t="s">
+        <v>59</v>
       </c>
       <c r="C30" s="8"/>
-      <c r="D30" s="17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="10">
-        <v>1</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>28</v>
+      <c r="D30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B31" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" t="s">
+        <v>56</v>
+      </c>
+      <c r="F31" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B32" s="2" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B33" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="C33" s="20"/>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B33" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="8"/>
       <c r="D33" t="s">
         <v>50</v>
       </c>
       <c r="E33" t="s">
+        <v>56</v>
+      </c>
+      <c r="F33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="10">
+        <v>1</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="14"/>
+      <c r="B35" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="14"/>
+      <c r="B36" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="14"/>
+      <c r="B37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="8"/>
+      <c r="D37" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="10">
+        <v>1</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B39" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" s="8"/>
+      <c r="D39" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B40" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="20"/>
+      <c r="D40" t="s">
+        <v>50</v>
+      </c>
+      <c r="E40" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B34" s="2" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B41" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D41" t="s">
         <v>50</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E41" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B35" s="2" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B42" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D42" t="s">
         <v>50</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E42" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B43" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D43" t="s">
+        <v>50</v>
+      </c>
+      <c r="E43" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
actualizando un poco más la información el tracking
</commit_message>
<xml_diff>
--- a/documentacion/Tareas.xlsx
+++ b/documentacion/Tareas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Desktop\Universidad\4ºAño\ISO\RecetApp\documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/481f6a27916b9a84/Documentos/RecetApp/documentacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7B81A3-8BC2-429E-9BD9-6123171C26C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="114_{FAFFA8FD-DE6D-4DF6-95A6-B25036B615AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E1327B53-49E0-4382-BC40-6963018E2393}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="63">
   <si>
     <t>CREACIÓN DE UNA CUENTA</t>
   </si>
@@ -209,9 +209,6 @@
     <t>Validar que el login permite a un usuario ya creado acceder a la aplicación en distintos dispositivos</t>
   </si>
   <si>
-    <t>Validar que un usuario que ha accedido a la aplicación puede añadir ingresientes a su inventarop</t>
-  </si>
-  <si>
     <t>Crear un dump para crear la tabla de guradado de ingredientes</t>
   </si>
   <si>
@@ -219,15 +216,28 @@
   </si>
   <si>
     <t>Validar que las consultas se realicen correctamente, de manera que, cuando un usuario introduzca sus ingredientes le salga la receta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 minutos </t>
+  </si>
+  <si>
+    <t>Validar que un usuario que ha accedido a la aplicación puede añadir ingredientes a su inventario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -340,47 +350,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -698,8 +709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66436974-768D-9A40-9A43-2F0986DDE03B}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1012,8 +1023,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B27" s="22" t="s">
-        <v>58</v>
+      <c r="B27" s="23" t="s">
+        <v>62</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" t="s">
@@ -1048,7 +1059,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B30" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" t="s">
@@ -1081,7 +1092,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B33" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" t="s">
@@ -1129,6 +1140,12 @@
       <c r="D37" s="17" t="s">
         <v>40</v>
       </c>
+      <c r="E37" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="38" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10">
@@ -1183,7 +1200,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B43" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D43" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
Archivo de texto para el dump de las recetas
</commit_message>
<xml_diff>
--- a/documentacion/Tareas.xlsx
+++ b/documentacion/Tareas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jose_manuel179/Desktop/RecetApp/documentacion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elisa\Desktop\Ingenieria\RecetApp\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0355CB6C-8908-214B-9637-FF1A243C9705}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36567F2-40F6-49AE-B2CD-A537CD6BF26C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="69">
   <si>
     <t>CREACIÓN DE UNA CUENTA</t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t>20 minutos</t>
+  </si>
+  <si>
+    <t>2 horas y media</t>
   </si>
 </sst>
 </file>
@@ -727,20 +730,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66436974-768D-9A40-9A43-2F0986DDE03B}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="7"/>
-    <col min="2" max="2" width="116.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.625" style="7"/>
+    <col min="2" max="2" width="116.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>17</v>
       </c>
@@ -760,7 +763,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -768,7 +771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
@@ -783,7 +786,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>43</v>
       </c>
@@ -798,7 +801,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -807,7 +810,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>40</v>
       </c>
@@ -822,7 +825,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
         <v>42</v>
       </c>
@@ -831,7 +834,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>45</v>
       </c>
@@ -840,7 +843,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="21" t="s">
         <v>54</v>
       </c>
@@ -855,7 +858,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="24" t="s">
         <v>65</v>
       </c>
@@ -866,7 +869,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="24" t="s">
         <v>63</v>
       </c>
@@ -877,7 +880,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="24" t="s">
         <v>64</v>
       </c>
@@ -888,7 +891,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>3</v>
       </c>
@@ -897,7 +900,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>1</v>
       </c>
@@ -908,7 +911,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>5</v>
       </c>
@@ -923,7 +926,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>6</v>
       </c>
@@ -932,7 +935,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>7</v>
       </c>
@@ -941,7 +944,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
@@ -950,7 +953,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" s="22" t="s">
         <v>56</v>
       </c>
@@ -965,7 +968,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>1</v>
       </c>
@@ -976,7 +979,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>10</v>
       </c>
@@ -985,7 +988,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="19" t="s">
         <v>47</v>
       </c>
@@ -994,7 +997,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="19" t="s">
         <v>46</v>
       </c>
@@ -1003,7 +1006,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" s="22" t="s">
         <v>54</v>
       </c>
@@ -1018,7 +1021,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>23</v>
       </c>
@@ -1027,7 +1030,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>1</v>
       </c>
@@ -1038,7 +1041,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>25</v>
       </c>
@@ -1053,7 +1056,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>26</v>
       </c>
@@ -1068,7 +1071,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" s="22" t="s">
         <v>57</v>
       </c>
@@ -1083,7 +1086,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>1</v>
       </c>
@@ -1094,7 +1097,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>12</v>
       </c>
@@ -1103,7 +1106,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32" s="23" t="s">
         <v>60</v>
       </c>
@@ -1112,7 +1115,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B33" s="22" t="s">
         <v>54</v>
       </c>
@@ -1127,7 +1130,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>11</v>
       </c>
@@ -1136,7 +1139,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B35" s="22" t="s">
         <v>58</v>
       </c>
@@ -1151,7 +1154,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <v>1</v>
       </c>
@@ -1159,11 +1162,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="16" t="s">
         <v>29</v>
       </c>
+      <c r="C37" s="8"/>
       <c r="D37" s="15" t="s">
         <v>48</v>
       </c>
@@ -1174,19 +1178,23 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="14"/>
       <c r="B38" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="C38" s="8"/>
       <c r="D38" s="15" t="s">
         <v>48</v>
       </c>
       <c r="E38" s="15" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F38" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="14"/>
       <c r="B39" s="2" t="s">
         <v>14</v>
@@ -1196,7 +1204,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
         <v>1</v>
       </c>
@@ -1204,7 +1212,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>32</v>
       </c>
@@ -1213,7 +1221,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B42" s="19" t="s">
         <v>50</v>
       </c>
@@ -1225,7 +1233,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>31</v>
       </c>
@@ -1236,7 +1244,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>33</v>
       </c>
@@ -1247,7 +1255,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B45" s="22" t="s">
         <v>59</v>
       </c>

</xml_diff>

<commit_message>
Añadido story/tareas para borrar ingredientes del inventario
</commit_message>
<xml_diff>
--- a/documentacion/Tareas.xlsx
+++ b/documentacion/Tareas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique/GitHubProjects/RecetApp/documentacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320AE38A-2D04-F741-9256-A1DDD6C7751D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9474564B-8E6B-8F4B-90C9-A2727A08B679}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18840" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="62">
   <si>
     <t>CREACIÓN DE UNA CUENTA</t>
   </si>
@@ -210,6 +210,15 @@
   </si>
   <si>
     <t>Validar que las consultas se realicen correctamente, de manera que, cuando un usuario introduzca sus ingredientes le salgan las receta</t>
+  </si>
+  <si>
+    <t>BORRAR INGREDIENTES</t>
+  </si>
+  <si>
+    <t>Crear una opción en el menú para que el usuario borre ingredientes de su inventario</t>
+  </si>
+  <si>
+    <t>Crear la consulta sql para borrar un ingrediente introducido por el usuario</t>
   </si>
 </sst>
 </file>
@@ -698,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66436974-768D-9A40-9A43-2F0986DDE03B}">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -740,6 +749,9 @@
       <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
+      <c r="C2" s="12" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
@@ -1207,6 +1219,9 @@
       </c>
       <c r="B36" s="13" t="s">
         <v>26</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
@@ -1322,6 +1337,36 @@
         <v>42</v>
       </c>
       <c r="E45">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="10">
+        <v>2</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B47" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D47" t="s">
+        <v>20</v>
+      </c>
+      <c r="E47">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B48" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D48" t="s">
+        <v>20</v>
+      </c>
+      <c r="E48">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update de las tareas (separadas las tareas conjuntas en tareas para una persona)
</commit_message>
<xml_diff>
--- a/documentacion/Tareas.xlsx
+++ b/documentacion/Tareas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique/GitHubProjects/RecetApp/documentacion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Desktop\Universidad\4ºAño\ISO\RecetApp\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9474564B-8E6B-8F4B-90C9-A2727A08B679}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C036DF-3C5F-4CF0-A7BC-F8FF13379CF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18840" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="58">
   <si>
     <t>CREACIÓN DE UNA CUENTA</t>
   </si>
@@ -137,24 +137,15 @@
     <t>José Manuel</t>
   </si>
   <si>
-    <t>Enrique, Mario</t>
-  </si>
-  <si>
     <t>Búsqueda de información para conectar la base de datos a la aplicación</t>
   </si>
   <si>
-    <t>Enrique, Sergio</t>
-  </si>
-  <si>
     <t>Escribir el código que permite conectar la base de datos a la aplicación</t>
   </si>
   <si>
     <t>Búsqueda de información para realizar la tarea en el lenguaje GO</t>
   </si>
   <si>
-    <t>Enrique, Mario, Sergio, José Manuel, Elisa</t>
-  </si>
-  <si>
     <t>Crear un dump que permita la creación de la tabla usuario</t>
   </si>
   <si>
@@ -180,9 +171,6 @@
   </si>
   <si>
     <t>Validar que se guardan los ingredientes en la base de datos</t>
-  </si>
-  <si>
-    <t>Enrique, Sergio, Elisa</t>
   </si>
   <si>
     <t>Modificar la función Insert() para que los usuarios puedan añadir sus intolerancias</t>
@@ -707,22 +695,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66436974-768D-9A40-9A43-2F0986DDE03B}">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="7"/>
-    <col min="2" max="2" width="116.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.69921875" style="7"/>
+    <col min="2" max="2" width="116.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.19921875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>17</v>
       </c>
@@ -736,13 +724,13 @@
         <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -753,13 +741,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -768,13 +756,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" s="18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -783,398 +771,406 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
-        <v>2</v>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="18" t="s">
+        <v>36</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E5">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" s="18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="18" t="s">
         <v>36</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="18" t="s">
-        <v>37</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" s="18" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="E8">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="21" t="s">
-        <v>45</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="E9">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F9">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B10" s="2" t="s">
-        <v>3</v>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" t="s">
         <v>20</v>
       </c>
       <c r="E10">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="10">
-        <v>1</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="24" t="s">
-        <v>51</v>
-      </c>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B12" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="8"/>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E12">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="24" t="s">
-        <v>50</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B13" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="8"/>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E13">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="24" t="s">
-        <v>56</v>
-      </c>
+        <v>0.5</v>
+      </c>
+      <c r="F13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B14" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="8"/>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E14">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="10">
-        <v>1</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.1</v>
+      </c>
+      <c r="F14">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B15" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15">
+        <v>0.1</v>
+      </c>
+      <c r="F15">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="E16">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="F16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="8"/>
-      <c r="D17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10">
+        <v>1</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B18" s="24" t="s">
+        <v>47</v>
+      </c>
       <c r="D18" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="E18">
-        <v>0.5</v>
-      </c>
-      <c r="F18">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="8"/>
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B19" s="24" t="s">
+        <v>46</v>
+      </c>
       <c r="D19" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="E19">
-        <v>0.5</v>
-      </c>
-      <c r="F19">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B20" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="8"/>
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B20" s="24" t="s">
+        <v>52</v>
+      </c>
       <c r="D20" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E20">
-        <v>0.1</v>
-      </c>
-      <c r="F20">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10">
         <v>1</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C22" s="8"/>
-      <c r="D22" s="17" t="s">
+      <c r="D22" t="s">
         <v>20</v>
       </c>
       <c r="E22">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="F22">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B23" s="23" t="s">
-        <v>53</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B23" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C23" s="8"/>
-      <c r="D23" s="17" t="s">
-        <v>34</v>
+      <c r="D23" t="s">
+        <v>39</v>
       </c>
       <c r="E23">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="F23">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B24" s="22" t="s">
-        <v>45</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B24" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C24" s="8"/>
-      <c r="D24" s="17" t="s">
-        <v>36</v>
+      <c r="D24" t="s">
+        <v>20</v>
       </c>
       <c r="E24">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="F24">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" t="s">
         <v>20</v>
       </c>
       <c r="E25">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="F25">
         <v>1.5</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="10">
-        <v>1</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B27" s="2" t="s">
-        <v>23</v>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="8"/>
+      <c r="D26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26">
+        <v>0.5</v>
+      </c>
+      <c r="F26">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B27" s="22" t="s">
+        <v>43</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="F27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B28" s="2" t="s">
-        <v>24</v>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B28" s="22" t="s">
+        <v>43</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28">
+        <v>0.1</v>
+      </c>
+      <c r="F28">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="10">
+        <v>1</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="8"/>
+      <c r="D30" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30">
+        <v>0.5</v>
+      </c>
+      <c r="F30">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B31" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31">
+        <v>0.5</v>
+      </c>
+      <c r="F31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B32" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E28">
-        <v>0.33</v>
-      </c>
-      <c r="F28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B29" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" s="8"/>
-      <c r="D29" t="s">
+      <c r="E32">
+        <v>0.5</v>
+      </c>
+      <c r="F32">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B33" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="E29">
-        <v>0.1</v>
-      </c>
-      <c r="F29">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="10">
-        <v>1</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B31" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" s="8"/>
-      <c r="D31" t="s">
-        <v>20</v>
-      </c>
-      <c r="E31">
-        <v>0.5</v>
-      </c>
-      <c r="F31">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B32" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="C32" s="8"/>
-      <c r="D32" t="s">
-        <v>20</v>
-      </c>
-      <c r="E32">
-        <v>0.1</v>
-      </c>
-      <c r="F32">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B33" s="22" t="s">
-        <v>45</v>
-      </c>
       <c r="C33" s="8"/>
-      <c r="D33" t="s">
-        <v>49</v>
+      <c r="D33" s="17" t="s">
+        <v>20</v>
       </c>
       <c r="E33">
         <v>0.1</v>
@@ -1183,190 +1179,378 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B34" s="2" t="s">
-        <v>11</v>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B34" s="22" t="s">
+        <v>42</v>
       </c>
       <c r="C34" s="8"/>
-      <c r="D34" t="s">
-        <v>20</v>
+      <c r="D34" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="E34">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="F34">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B35" s="22" t="s">
-        <v>48</v>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B35" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="E35">
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="F35">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10">
         <v>1</v>
       </c>
-      <c r="B36" s="13" t="s">
-        <v>26</v>
+      <c r="B36" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="C36" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="14"/>
-      <c r="B37" s="16" t="s">
-        <v>27</v>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B37" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="C37" s="8"/>
-      <c r="D37" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E37" s="15">
-        <v>1</v>
-      </c>
-      <c r="F37" s="15">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="14"/>
+      <c r="D37" t="s">
+        <v>32</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B38" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C38" s="8"/>
-      <c r="D38" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E38" s="15">
-        <v>3</v>
-      </c>
-      <c r="F38" s="15">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="14"/>
-      <c r="B39" s="2" t="s">
-        <v>14</v>
+      <c r="D38" t="s">
+        <v>32</v>
+      </c>
+      <c r="E38">
+        <v>0.33</v>
+      </c>
+      <c r="F38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B39" s="22" t="s">
+        <v>44</v>
       </c>
       <c r="C39" s="8"/>
-      <c r="D39" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="E39" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="F39" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>39</v>
+      </c>
+      <c r="E39">
+        <v>0.1</v>
+      </c>
+      <c r="F39">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="10">
         <v>1</v>
       </c>
-      <c r="B40" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B40" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B41" s="2" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" t="s">
         <v>20</v>
       </c>
-      <c r="E41" s="15">
-        <v>0.33</v>
+      <c r="E41">
+        <v>0.5</v>
       </c>
       <c r="F41">
         <v>0.33</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B42" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C42" s="20"/>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B42" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" s="8"/>
       <c r="D42" t="s">
+        <v>20</v>
+      </c>
+      <c r="E42">
+        <v>0.1</v>
+      </c>
+      <c r="F42">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B43" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="E42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B43" s="2" t="s">
+      <c r="C43" s="8"/>
+      <c r="D43" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43">
+        <v>0.1</v>
+      </c>
+      <c r="F43">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B44" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" s="8"/>
+      <c r="D44" t="s">
+        <v>39</v>
+      </c>
+      <c r="E44">
+        <v>0.1</v>
+      </c>
+      <c r="F44">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B45" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C45" s="8"/>
+      <c r="D45" t="s">
+        <v>38</v>
+      </c>
+      <c r="E45">
+        <v>0.1</v>
+      </c>
+      <c r="F45">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B46" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="8"/>
+      <c r="D46" t="s">
+        <v>20</v>
+      </c>
+      <c r="E46">
+        <v>0.5</v>
+      </c>
+      <c r="F46">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B47" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" s="8"/>
+      <c r="D47" t="s">
+        <v>39</v>
+      </c>
+      <c r="E47">
+        <v>0.1</v>
+      </c>
+      <c r="F47">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="10">
+        <v>1</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="14"/>
+      <c r="B49" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C49" s="8"/>
+      <c r="D49" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E49" s="15">
+        <v>1</v>
+      </c>
+      <c r="F49" s="15">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="14"/>
+      <c r="B50" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C50" s="8"/>
+      <c r="D50" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E50" s="15">
+        <v>3</v>
+      </c>
+      <c r="F50" s="15">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="14"/>
+      <c r="B51" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51" s="8"/>
+      <c r="D51" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E51" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F51" s="15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="14"/>
+      <c r="B52" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52" s="8"/>
+      <c r="D52" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E52" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F52" s="15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="10">
+        <v>1</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B54" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C54" s="8"/>
+      <c r="D54" t="s">
+        <v>20</v>
+      </c>
+      <c r="E54" s="15">
+        <v>0.33</v>
+      </c>
+      <c r="F54">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B55" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C55" s="20"/>
+      <c r="D55" t="s">
+        <v>39</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B56" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D43" t="s">
-        <v>42</v>
-      </c>
-      <c r="E43">
+      <c r="D56" t="s">
+        <v>39</v>
+      </c>
+      <c r="E56">
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B44" s="2" t="s">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B57" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D44" t="s">
-        <v>42</v>
-      </c>
-      <c r="E44">
+      <c r="D57" t="s">
+        <v>39</v>
+      </c>
+      <c r="E57">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B45" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="D45" t="s">
-        <v>42</v>
-      </c>
-      <c r="E45">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="10">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B58" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D58" t="s">
+        <v>39</v>
+      </c>
+      <c r="E58">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="10">
         <v>2</v>
       </c>
-      <c r="B46" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B47" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="D47" t="s">
-        <v>20</v>
-      </c>
-      <c r="E47">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B48" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="D48" t="s">
-        <v>20</v>
-      </c>
-      <c r="E48">
+      <c r="B59" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B60" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D60" t="s">
+        <v>20</v>
+      </c>
+      <c r="E60">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B61" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="D61" t="s">
+        <v>20</v>
+      </c>
+      <c r="E61">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Subida versión inicial de las consultas a la BBDD para las recetas
</commit_message>
<xml_diff>
--- a/documentacion/Tareas.xlsx
+++ b/documentacion/Tareas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Desktop\Universidad\4ºAño\ISO\RecetApp\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD98B7F-A179-4251-A681-F81D3963E3BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A32939-C499-49EC-AB41-8799B5E88082}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="61">
   <si>
     <t>CREACIÓN DE UNA CUENTA</t>
   </si>
@@ -214,15 +214,25 @@
   </si>
   <si>
     <t>Mostrar la lista de recetas por pantalla de la base de datos</t>
+  </si>
+  <si>
+    <t>Validar que la consulta sale por pantalla</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -287,7 +297,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -330,12 +340,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -351,50 +355,50 @@
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -710,9 +714,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66436974-768D-9A40-9A43-2F0986DDE03B}">
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
@@ -922,7 +926,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="20" t="s">
         <v>41</v>
       </c>
       <c r="C14" s="8"/>
@@ -937,7 +941,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="20" t="s">
         <v>41</v>
       </c>
       <c r="C15" s="8"/>
@@ -975,7 +979,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="23" t="s">
         <v>46</v>
       </c>
       <c r="D18" t="s">
@@ -986,7 +990,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="23" t="s">
         <v>45</v>
       </c>
       <c r="D19" t="s">
@@ -997,7 +1001,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="23" t="s">
         <v>51</v>
       </c>
       <c r="D20" t="s">
@@ -1094,7 +1098,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="21" t="s">
         <v>42</v>
       </c>
       <c r="C27" s="8"/>
@@ -1109,7 +1113,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="21" t="s">
         <v>42</v>
       </c>
       <c r="C28" s="8"/>
@@ -1150,7 +1154,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B31" s="23" t="s">
+      <c r="B31" s="22" t="s">
         <v>48</v>
       </c>
       <c r="C31" s="8"/>
@@ -1165,7 +1169,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B32" s="23" t="s">
+      <c r="B32" s="22" t="s">
         <v>48</v>
       </c>
       <c r="C32" s="8"/>
@@ -1180,7 +1184,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="21" t="s">
         <v>41</v>
       </c>
       <c r="C33" s="8"/>
@@ -1195,7 +1199,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="21" t="s">
         <v>41</v>
       </c>
       <c r="C34" s="8"/>
@@ -1266,7 +1270,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="21" t="s">
         <v>43</v>
       </c>
       <c r="C39" s="8"/>
@@ -1307,7 +1311,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B42" s="23" t="s">
+      <c r="B42" s="22" t="s">
         <v>49</v>
       </c>
       <c r="C42" s="8"/>
@@ -1322,7 +1326,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B43" s="22" t="s">
+      <c r="B43" s="21" t="s">
         <v>41</v>
       </c>
       <c r="C43" s="8"/>
@@ -1337,7 +1341,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B44" s="22" t="s">
+      <c r="B44" s="21" t="s">
         <v>41</v>
       </c>
       <c r="C44" s="8"/>
@@ -1352,7 +1356,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B45" s="22" t="s">
+      <c r="B45" s="21" t="s">
         <v>41</v>
       </c>
       <c r="C45" s="8"/>
@@ -1382,7 +1386,7 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B47" s="22" t="s">
+      <c r="B47" s="21" t="s">
         <v>44</v>
       </c>
       <c r="C47" s="8"/>
@@ -1498,7 +1502,7 @@
       <c r="B55" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C55" s="20"/>
+      <c r="C55" s="8"/>
       <c r="D55" t="s">
         <v>38</v>
       </c>
@@ -1506,8 +1510,8 @@
         <v>1</v>
       </c>
       <c r="F55">
-        <f>1+1</f>
-        <v>2</v>
+        <f>1+1+0.5</f>
+        <v>2.5</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -1520,91 +1524,106 @@
       <c r="E56">
         <v>2</v>
       </c>
+      <c r="F56">
+        <f>1+2</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B57" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D57" t="s">
+        <v>38</v>
+      </c>
+      <c r="E57">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B58" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="D57" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B58" s="25" t="s">
+      <c r="D58" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B59" s="24" t="s">
         <v>59</v>
-      </c>
-      <c r="C58" s="8"/>
-      <c r="D58" t="s">
-        <v>38</v>
-      </c>
-      <c r="E58">
-        <v>0.4</v>
-      </c>
-      <c r="F58">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B59" s="25" t="s">
-        <v>58</v>
       </c>
       <c r="C59" s="8"/>
       <c r="D59" t="s">
         <v>38</v>
       </c>
       <c r="E59">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="F59">
         <v>0.1</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B60" s="25" t="s">
+      <c r="B60" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C60" s="8"/>
+      <c r="D60" t="s">
+        <v>38</v>
+      </c>
+      <c r="E60">
+        <v>0.1</v>
+      </c>
+      <c r="F60">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B61" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="D60" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B61" s="23" t="s">
+      <c r="D61" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B62" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D62" t="s">
         <v>38</v>
       </c>
-      <c r="E61">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="10">
+      <c r="E62">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="10">
         <v>2</v>
       </c>
-      <c r="B62" s="13" t="s">
+      <c r="B63" s="13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B63" s="23" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B64" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D63" t="s">
-        <v>20</v>
-      </c>
-      <c r="E63">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B64" s="23" t="s">
+      <c r="D64" t="s">
+        <v>20</v>
+      </c>
+      <c r="E64">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B65" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="D64" t="s">
-        <v>20</v>
-      </c>
-      <c r="E64">
+      <c r="D65" t="s">
+        <v>20</v>
+      </c>
+      <c r="E65">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
resolviendo un conflicto propio entre versiones del repositorio
</commit_message>
<xml_diff>
--- a/documentacion/Tareas.xlsx
+++ b/documentacion/Tareas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique/GitHubProjects/RecetApp/documentacion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/481f6a27916b9a84/Documentos/RecetApp/documentacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320AE38A-2D04-F741-9256-A1DDD6C7751D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{72C9CACF-675C-41F3-87C2-98BAA62F15DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18840" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -704,16 +704,16 @@
       <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="7"/>
-    <col min="2" max="2" width="116.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.69921875" style="7"/>
+    <col min="2" max="2" width="116.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.19921875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>17</v>
       </c>
@@ -733,7 +733,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -741,7 +741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
@@ -756,7 +756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" s="18" t="s">
         <v>38</v>
       </c>
@@ -771,7 +771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -786,7 +786,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" s="18" t="s">
         <v>35</v>
       </c>
@@ -801,7 +801,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B7" s="18" t="s">
         <v>37</v>
       </c>
@@ -816,7 +816,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" s="18" t="s">
         <v>40</v>
       </c>
@@ -831,7 +831,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B9" s="21" t="s">
         <v>45</v>
       </c>
@@ -846,7 +846,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>3</v>
       </c>
@@ -861,7 +861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <v>1</v>
       </c>
@@ -869,7 +869,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" s="24" t="s">
         <v>51</v>
       </c>
@@ -880,7 +880,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" s="24" t="s">
         <v>50</v>
       </c>
@@ -891,7 +891,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" s="24" t="s">
         <v>56</v>
       </c>
@@ -902,7 +902,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <v>1</v>
       </c>
@@ -913,7 +913,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>5</v>
       </c>
@@ -928,7 +928,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>6</v>
       </c>
@@ -943,7 +943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>7</v>
       </c>
@@ -958,7 +958,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>8</v>
       </c>
@@ -973,7 +973,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B20" s="22" t="s">
         <v>46</v>
       </c>
@@ -988,7 +988,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10">
         <v>1</v>
       </c>
@@ -999,7 +999,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>10</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B23" s="23" t="s">
         <v>53</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B24" s="22" t="s">
         <v>45</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
         <v>21</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10">
         <v>1</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
         <v>23</v>
       </c>
@@ -1085,7 +1085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
         <v>24</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B29" s="22" t="s">
         <v>47</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10">
         <v>1</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
         <v>12</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B32" s="23" t="s">
         <v>54</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B33" s="22" t="s">
         <v>45</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B34" s="2" t="s">
         <v>11</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B35" s="22" t="s">
         <v>48</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10">
         <v>1</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="14"/>
       <c r="B37" s="16" t="s">
         <v>27</v>
@@ -1225,7 +1225,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="14"/>
       <c r="B38" s="2" t="s">
         <v>28</v>
@@ -1241,7 +1241,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="14"/>
       <c r="B39" s="2" t="s">
         <v>14</v>
@@ -1257,7 +1257,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="10">
         <v>1</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B41" s="2" t="s">
         <v>30</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B42" s="19" t="s">
         <v>43</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B43" s="2" t="s">
         <v>29</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B44" s="2" t="s">
         <v>31</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B45" s="23" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
Update de las tareas y añadida la opción que permite al usuario acceder al Login si se equivoca en el primer intento
</commit_message>
<xml_diff>
--- a/documentacion/Tareas.xlsx
+++ b/documentacion/Tareas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/481f6a27916b9a84/Documentos/RecetApp/documentacion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Desktop\Universidad\4ºAño\ISO\RecetApp\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="114_{A24F956D-6679-4309-8506-19D78EBC3C6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{707035F4-3740-4B16-A01D-4A13320F1327}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E43D111-46BC-46A0-B1ED-932D8AE19F50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="72">
   <si>
     <t>CREACIÓN DE UNA CUENTA</t>
   </si>
@@ -102,9 +102,6 @@
     <t>Crear una interfaz que le permita al usuario buscar ingredientes</t>
   </si>
   <si>
-    <t>AGREGAR INGREDIENTES A LA BASE DE DATOS</t>
-  </si>
-  <si>
     <t>Buscar una base de datos con alimentos</t>
   </si>
   <si>
@@ -229,6 +226,30 @@
   </si>
   <si>
     <t>Validar que un usuario que ha accedido a la aplicación puede añadir ingresientes a su inventario</t>
+  </si>
+  <si>
+    <t>Colocar en el código una condición que no permita introducir el mismo ingrediente más de una vez a un usuario</t>
+  </si>
+  <si>
+    <t>Validar que un usuario intentente introducir dos veces el mismo ingrediente y le salga un error</t>
+  </si>
+  <si>
+    <t>Pemitir al usuario poner esta información después de haber hecho login con su cuenta creada</t>
+  </si>
+  <si>
+    <t>AGREGAR INGREDIENTES A EL INVENTARIO DEL USUARIO</t>
+  </si>
+  <si>
+    <t>Validar que los ingredientes se guardan en la BBDD mediante la muestra de la lista de ingredientes seleccionados</t>
+  </si>
+  <si>
+    <t>Pemirit al usuario que se le muestren por pantalla todas las recetas</t>
+  </si>
+  <si>
+    <t>Validar que el usuario puede ver todas las recetas por pantalla</t>
+  </si>
+  <si>
+    <t>Validar que el login permite a un usuario que si se equivoca en el Login pueda volver a entrar</t>
   </si>
 </sst>
 </file>
@@ -273,7 +294,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -316,6 +337,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -329,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -370,6 +403,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,10 +724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66436974-768D-9A40-9A43-2F0986DDE03B}">
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -713,10 +753,10 @@
         <v>18</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -756,7 +796,7 @@
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E4" s="5">
         <v>1</v>
@@ -772,7 +812,7 @@
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" s="5">
         <v>1</v>
@@ -788,7 +828,7 @@
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6" s="5">
         <v>1</v>
@@ -800,7 +840,7 @@
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="5" t="s">
@@ -816,11 +856,11 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="5">
         <v>1</v>
@@ -832,11 +872,11 @@
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E9" s="5">
         <v>1</v>
@@ -848,11 +888,11 @@
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="5">
         <v>1</v>
@@ -864,11 +904,11 @@
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E11" s="5">
         <v>1</v>
@@ -896,7 +936,7 @@
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="5" t="s">
@@ -912,11 +952,11 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E14" s="5">
         <v>1</v>
@@ -928,7 +968,7 @@
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="5" t="s">
@@ -944,7 +984,7 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="5" t="s">
@@ -960,7 +1000,7 @@
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="5" t="s">
@@ -976,11 +1016,11 @@
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E18" s="5">
         <v>0.1</v>
@@ -991,7 +1031,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="22" t="s">
         <v>3</v>
       </c>
       <c r="C19" s="15"/>
@@ -1010,7 +1050,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
@@ -1020,7 +1060,7 @@
     <row r="21" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
@@ -1030,11 +1070,11 @@
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E22" s="5">
         <v>0.17</v>
@@ -1044,11 +1084,11 @@
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E23" s="5">
         <v>0.33</v>
@@ -1058,44 +1098,41 @@
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
       <c r="B24" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C24" s="15"/>
       <c r="D24" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E24" s="5">
         <v>0.33</v>
       </c>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="12">
-        <v>1</v>
-      </c>
-      <c r="B25" s="3" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="21">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="12">
+        <v>1</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="14"/>
-      <c r="B26" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="15"/>
-      <c r="D26" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E26" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="F26" s="5">
-        <v>2</v>
-      </c>
+      <c r="C26" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
@@ -1104,7 +1141,7 @@
       </c>
       <c r="C27" s="15"/>
       <c r="D27" s="5" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="E27" s="5">
         <v>1.5</v>
@@ -1116,39 +1153,39 @@
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
       <c r="B28" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C28" s="15"/>
       <c r="D28" s="5" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="E28" s="5">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="F28" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="B29" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C29" s="15"/>
       <c r="D29" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E29" s="5">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F29" s="5">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="14"/>
       <c r="B30" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C30" s="15"/>
       <c r="D30" s="5" t="s">
@@ -1158,107 +1195,111 @@
         <v>0.5</v>
       </c>
       <c r="F30" s="5">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="14"/>
       <c r="B31" s="5" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="C31" s="15"/>
       <c r="D31" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E31" s="5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F31" s="5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="14"/>
-      <c r="B32" s="5" t="s">
-        <v>40</v>
+      <c r="B32" s="19" t="s">
+        <v>62</v>
       </c>
       <c r="C32" s="15"/>
-      <c r="D32" s="5" t="s">
-        <v>37</v>
+      <c r="D32" s="21" t="s">
+        <v>36</v>
       </c>
       <c r="E32" s="5">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="F32" s="5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="14"/>
-      <c r="B33" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="C33" s="17"/>
-      <c r="D33" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-    </row>
-    <row r="34" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="12">
-        <v>1</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
+      <c r="B33" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="15"/>
+      <c r="D33" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F33" s="5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="14"/>
+      <c r="B34" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="15"/>
+      <c r="D34" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F34" s="5">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="14"/>
-      <c r="B35" s="5" t="s">
-        <v>10</v>
+      <c r="B35" s="23" t="s">
+        <v>71</v>
       </c>
       <c r="C35" s="15"/>
-      <c r="D35" s="18" t="s">
-        <v>20</v>
+      <c r="D35" s="21" t="s">
+        <v>36</v>
       </c>
       <c r="E35" s="5">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="F35" s="5">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="14"/>
-      <c r="B36" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C36" s="15"/>
-      <c r="D36" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="E36" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="F36" s="5">
-        <v>0.5</v>
-      </c>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="12">
+        <v>1</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="14"/>
       <c r="B37" s="5" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="C37" s="15"/>
       <c r="D37" s="18" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E37" s="5">
         <v>0.5</v>
@@ -1270,181 +1311,181 @@
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="14"/>
       <c r="B38" s="5" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C38" s="15"/>
       <c r="D38" s="18" t="s">
         <v>20</v>
       </c>
       <c r="E38" s="5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F38" s="5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="14"/>
       <c r="B39" s="5" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C39" s="15"/>
       <c r="D39" s="18" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E39" s="5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F39" s="5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="14"/>
       <c r="B40" s="5" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C40" s="15"/>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="18" t="s">
         <v>20</v>
       </c>
       <c r="E40" s="5">
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="F40" s="5">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="12">
-        <v>1</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C41" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="14"/>
+      <c r="B41" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" s="15"/>
+      <c r="D41" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E41" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F41" s="5">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="14"/>
       <c r="B42" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C42" s="15"/>
       <c r="D42" s="5" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E42" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F42" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="14"/>
-      <c r="B43" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E43" s="5">
-        <v>0.33</v>
-      </c>
-      <c r="F43" s="5">
-        <v>2</v>
-      </c>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="12">
+        <v>1</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="14"/>
       <c r="B44" s="5" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="C44" s="15"/>
       <c r="D44" s="5" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E44" s="5">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="F44" s="5">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="12">
-        <v>1</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="14"/>
+      <c r="B45" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45" s="15"/>
+      <c r="D45" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E45" s="5">
+        <v>0.33</v>
+      </c>
+      <c r="F45" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="14"/>
-      <c r="B46" s="5" t="s">
-        <v>12</v>
+      <c r="B46" s="22" t="s">
+        <v>63</v>
       </c>
       <c r="C46" s="15"/>
       <c r="D46" s="5" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="E46" s="5">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="F46" s="5">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="14"/>
-      <c r="B47" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C47" s="15"/>
-      <c r="D47" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E47" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="F47" s="5">
-        <v>0.1</v>
-      </c>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="12">
+        <v>1</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="14"/>
       <c r="B48" s="5" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="C48" s="15"/>
       <c r="D48" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E48" s="5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F48" s="5">
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="14"/>
       <c r="B49" s="5" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C49" s="15"/>
       <c r="D49" s="5" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="E49" s="5">
         <v>0.1</v>
@@ -1456,11 +1497,11 @@
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="14"/>
       <c r="B50" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C50" s="15"/>
       <c r="D50" s="5" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="E50" s="5">
         <v>0.1</v>
@@ -1472,340 +1513,429 @@
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="14"/>
       <c r="B51" s="5" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="C51" s="15"/>
       <c r="D51" s="5" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="E51" s="5">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="F51" s="5">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="16"/>
-      <c r="B52" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="C52" s="17"/>
-      <c r="D52" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E52" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="F52" s="17"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="14"/>
+      <c r="B52" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C52" s="15"/>
+      <c r="D52" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E52" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F52" s="5">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="14"/>
       <c r="B53" s="5" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="C53" s="15"/>
       <c r="D53" s="5" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="E53" s="5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F53" s="5">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="12">
-        <v>1</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C54" s="13" t="s">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="16"/>
+      <c r="B54" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54" s="17"/>
+      <c r="D54" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E54" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="F54" s="17"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="14"/>
+      <c r="B55" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C55" s="15"/>
+      <c r="D55" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E55" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F55" s="5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B56" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D56" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E56" s="21">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="12">
+        <v>1</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C57" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D54" s="13"/>
-      <c r="E54" s="13"/>
-      <c r="F54" s="13"/>
-    </row>
-    <row r="55" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="16"/>
-      <c r="B55" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C55" s="15"/>
-      <c r="D55" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E55" s="17">
-        <v>1</v>
-      </c>
-      <c r="F55" s="17">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="16"/>
-      <c r="B56" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C56" s="15"/>
-      <c r="D56" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E56" s="17">
-        <v>3</v>
-      </c>
-      <c r="F56" s="17">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="16"/>
-      <c r="B57" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C57" s="15"/>
-      <c r="D57" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="E57" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="F57" s="17">
-        <v>0.5</v>
-      </c>
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="13"/>
     </row>
     <row r="58" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="16"/>
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C58" s="15"/>
+      <c r="D58" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E58" s="17">
+        <v>1</v>
+      </c>
+      <c r="F58" s="17">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="16"/>
+      <c r="B59" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C59" s="15"/>
+      <c r="D59" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E59" s="17">
+        <v>3</v>
+      </c>
+      <c r="F59" s="17">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="16"/>
+      <c r="B60" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C58" s="15"/>
-      <c r="D58" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="E58" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="F58" s="17">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="12">
-        <v>1</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C59" s="13"/>
-      <c r="D59" s="13"/>
-      <c r="E59" s="13"/>
-      <c r="F59" s="13"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="14"/>
-      <c r="B60" s="5" t="s">
+      <c r="C60" s="15"/>
+      <c r="D60" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E60" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="F60" s="17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="16"/>
+      <c r="B61" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C61" s="15"/>
+      <c r="D61" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C60" s="15"/>
-      <c r="D60" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E60" s="17">
-        <v>0.33</v>
-      </c>
-      <c r="F60" s="5">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="14"/>
-      <c r="B61" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C61" s="15"/>
-      <c r="D61" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E61" s="5">
-        <v>1</v>
-      </c>
-      <c r="F61" s="5">
-        <f>1+1+0.5</f>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="14"/>
-      <c r="B62" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E62" s="5">
-        <v>2</v>
-      </c>
-      <c r="F62" s="5">
-        <f>1+2</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="14"/>
-      <c r="B63" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E63" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="F63" s="5"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="14"/>
-      <c r="B64" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E64" s="5">
-        <v>1</v>
-      </c>
-      <c r="F64" s="5"/>
+      <c r="E61" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="F61" s="17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="16"/>
+      <c r="B62" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="C62" s="25"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="17"/>
+      <c r="F62" s="17"/>
+    </row>
+    <row r="63" spans="1:6" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A63" s="24"/>
+      <c r="B63" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D63" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E63" s="21">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="12">
+        <v>1</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C64" s="13"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="13"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="14"/>
       <c r="B65" s="5" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="C65" s="15"/>
       <c r="D65" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E65" s="5">
-        <v>0.4</v>
+        <v>20</v>
+      </c>
+      <c r="E65" s="17">
+        <v>0.33</v>
       </c>
       <c r="F65" s="5">
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="14"/>
       <c r="B66" s="5" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="C66" s="15"/>
       <c r="D66" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E66" s="5">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="F66" s="5">
-        <v>0.1</v>
+        <f>1+1+0.5</f>
+        <v>2.5</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="14"/>
       <c r="B67" s="5" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="C67" s="5"/>
       <c r="D67" s="5" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="E67" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="F67" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="F67" s="5">
+        <f>1+2+2</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="14"/>
       <c r="B68" s="5" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E68" s="5">
         <v>0.1</v>
       </c>
       <c r="F68" s="5"/>
     </row>
-    <row r="69" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="12">
-        <v>2</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C69" s="13"/>
-      <c r="D69" s="13"/>
-      <c r="E69" s="13"/>
-      <c r="F69" s="13"/>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" s="14"/>
+      <c r="B69" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E69" s="5">
+        <v>1</v>
+      </c>
+      <c r="F69" s="5"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="14"/>
       <c r="B70" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C70" s="5"/>
+        <v>54</v>
+      </c>
+      <c r="C70" s="15"/>
       <c r="D70" s="5" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="E70" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="F70" s="5"/>
+        <v>0.4</v>
+      </c>
+      <c r="F70" s="5">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="14"/>
       <c r="B71" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C71" s="15"/>
+      <c r="D71" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E71" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F71" s="5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" s="14"/>
+      <c r="B72" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E71" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="F71" s="5"/>
-    </row>
-    <row r="72" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="12">
-        <v>1</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C72" s="13"/>
-      <c r="D72" s="13"/>
-      <c r="E72" s="13"/>
-      <c r="F72" s="13"/>
-    </row>
-    <row r="73" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="12">
-        <v>1</v>
-      </c>
-      <c r="B73" s="3" t="s">
+      <c r="C72" s="5"/>
+      <c r="D72" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E72" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="F72" s="5"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" s="14"/>
+      <c r="B73" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E73" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F73" s="5"/>
+    </row>
+    <row r="74" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="12">
+        <v>2</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C74" s="13"/>
+      <c r="D74" s="13"/>
+      <c r="E74" s="13"/>
+      <c r="F74" s="13"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" s="14"/>
+      <c r="B75" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E75" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="F75" s="5"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" s="14"/>
+      <c r="B76" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E76" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F76" s="5"/>
+    </row>
+    <row r="77" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="12">
+        <v>1</v>
+      </c>
+      <c r="B77" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C73" s="13"/>
-      <c r="D73" s="13"/>
-      <c r="E73" s="13"/>
-      <c r="F73" s="13"/>
+      <c r="C77" s="13"/>
+      <c r="D77" s="13"/>
+      <c r="E77" s="13"/>
+      <c r="F77" s="13"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78" s="14"/>
+      <c r="B78" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5"/>
+      <c r="F78" s="5"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" s="14"/>
+      <c r="B79" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C79" s="5"/>
+      <c r="D79" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E79" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F79" s="5"/>
+    </row>
+    <row r="80" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="12">
+        <v>1</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C80" s="13"/>
+      <c r="D80" s="13"/>
+      <c r="E80" s="13"/>
+      <c r="F80" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Mostrar selección de ingredientes del usuario
</commit_message>
<xml_diff>
--- a/documentacion/Tareas.xlsx
+++ b/documentacion/Tareas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Desktop\Universidad\4ºAño\ISO\RecetApp\documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique/GitHubProjects/RecetApp/documentacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E43D111-46BC-46A0-B1ED-932D8AE19F50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3016FC-7C21-004B-9185-038C999A4054}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33400" windowHeight="18960" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -726,20 +726,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66436974-768D-9A40-9A43-2F0986DDE03B}">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.69921875" style="1"/>
-    <col min="2" max="2" width="116.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="1"/>
+    <col min="2" max="2" width="116.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>17</v>
       </c>
@@ -759,7 +759,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -773,7 +773,7 @@
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="14"/>
       <c r="B3" s="6" t="s">
         <v>1</v>
@@ -789,7 +789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="14"/>
       <c r="B4" s="6" t="s">
         <v>1</v>
@@ -805,7 +805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
@@ -821,7 +821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="14"/>
       <c r="B6" s="6" t="s">
         <v>1</v>
@@ -837,7 +837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" s="6" t="s">
         <v>33</v>
@@ -853,7 +853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
       <c r="B8" s="6" t="s">
         <v>33</v>
@@ -869,7 +869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="14"/>
       <c r="B9" s="6" t="s">
         <v>33</v>
@@ -885,7 +885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="14"/>
       <c r="B10" s="6" t="s">
         <v>33</v>
@@ -901,7 +901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="14"/>
       <c r="B11" s="6" t="s">
         <v>33</v>
@@ -917,7 +917,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="14"/>
       <c r="B12" s="6" t="s">
         <v>2</v>
@@ -933,7 +933,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="14"/>
       <c r="B13" s="6" t="s">
         <v>31</v>
@@ -949,7 +949,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="14"/>
       <c r="B14" s="6" t="s">
         <v>31</v>
@@ -965,7 +965,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="14"/>
       <c r="B15" s="6" t="s">
         <v>32</v>
@@ -981,7 +981,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="14"/>
       <c r="B16" s="6" t="s">
         <v>34</v>
@@ -997,7 +997,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="14"/>
       <c r="B17" s="6" t="s">
         <v>38</v>
@@ -1013,7 +1013,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="14"/>
       <c r="B18" s="6" t="s">
         <v>38</v>
@@ -1029,7 +1029,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="14"/>
       <c r="B19" s="22" t="s">
         <v>3</v>
@@ -1045,7 +1045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12">
         <v>1</v>
       </c>
@@ -1057,7 +1057,7 @@
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
     </row>
-    <row r="21" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="16"/>
       <c r="B21" s="20" t="s">
         <v>56</v>
@@ -1067,7 +1067,7 @@
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="14"/>
       <c r="B22" s="6" t="s">
         <v>42</v>
@@ -1081,7 +1081,7 @@
       </c>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="14"/>
       <c r="B23" s="6" t="s">
         <v>41</v>
@@ -1095,7 +1095,7 @@
       </c>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="14"/>
       <c r="B24" s="6" t="s">
         <v>61</v>
@@ -1109,7 +1109,7 @@
       </c>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B25" s="23" t="s">
         <v>66</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="12">
         <v>1</v>
       </c>
@@ -1134,7 +1134,7 @@
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="14"/>
       <c r="B27" s="5" t="s">
         <v>5</v>
@@ -1150,7 +1150,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="14"/>
       <c r="B28" s="5" t="s">
         <v>5</v>
@@ -1166,7 +1166,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="14"/>
       <c r="B29" s="5" t="s">
         <v>6</v>
@@ -1182,7 +1182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="14"/>
       <c r="B30" s="5" t="s">
         <v>7</v>
@@ -1198,7 +1198,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="14"/>
       <c r="B31" s="5" t="s">
         <v>8</v>
@@ -1214,7 +1214,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="14"/>
       <c r="B32" s="19" t="s">
         <v>62</v>
@@ -1230,7 +1230,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="14"/>
       <c r="B33" s="22" t="s">
         <v>39</v>
@@ -1246,7 +1246,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="14"/>
       <c r="B34" s="22" t="s">
         <v>39</v>
@@ -1262,7 +1262,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="14"/>
       <c r="B35" s="23" t="s">
         <v>71</v>
@@ -1278,7 +1278,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="12">
         <v>1</v>
       </c>
@@ -1292,7 +1292,7 @@
       <c r="E36" s="13"/>
       <c r="F36" s="13"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="14"/>
       <c r="B37" s="5" t="s">
         <v>10</v>
@@ -1308,7 +1308,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="14"/>
       <c r="B38" s="5" t="s">
         <v>44</v>
@@ -1324,7 +1324,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="14"/>
       <c r="B39" s="5" t="s">
         <v>44</v>
@@ -1340,7 +1340,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="14"/>
       <c r="B40" s="5" t="s">
         <v>38</v>
@@ -1356,7 +1356,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="14"/>
       <c r="B41" s="5" t="s">
         <v>38</v>
@@ -1372,7 +1372,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="14"/>
       <c r="B42" s="5" t="s">
         <v>21</v>
@@ -1388,7 +1388,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="12">
         <v>1</v>
       </c>
@@ -1402,7 +1402,7 @@
       <c r="E43" s="13"/>
       <c r="F43" s="13"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="14"/>
       <c r="B44" s="5" t="s">
         <v>22</v>
@@ -1418,7 +1418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="14"/>
       <c r="B45" s="5" t="s">
         <v>23</v>
@@ -1434,7 +1434,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="14"/>
       <c r="B46" s="22" t="s">
         <v>63</v>
@@ -1450,7 +1450,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="12">
         <v>1</v>
       </c>
@@ -1462,7 +1462,7 @@
       <c r="E47" s="13"/>
       <c r="F47" s="13"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="14"/>
       <c r="B48" s="5" t="s">
         <v>12</v>
@@ -1478,7 +1478,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="14"/>
       <c r="B49" s="5" t="s">
         <v>45</v>
@@ -1494,7 +1494,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="14"/>
       <c r="B50" s="5" t="s">
         <v>38</v>
@@ -1510,7 +1510,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="14"/>
       <c r="B51" s="5" t="s">
         <v>38</v>
@@ -1526,7 +1526,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="14"/>
       <c r="B52" s="5" t="s">
         <v>38</v>
@@ -1542,7 +1542,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="14"/>
       <c r="B53" s="5" t="s">
         <v>11</v>
@@ -1558,21 +1558,23 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="16"/>
       <c r="B54" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="C54" s="17"/>
+      <c r="C54" s="15"/>
       <c r="D54" s="17" t="s">
         <v>20</v>
       </c>
       <c r="E54" s="17">
         <v>0.5</v>
       </c>
-      <c r="F54" s="17"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F54" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="14"/>
       <c r="B55" s="5" t="s">
         <v>40</v>
@@ -1588,7 +1590,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B56" s="23" t="s">
         <v>68</v>
       </c>
@@ -1599,7 +1601,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="57" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="12">
         <v>1</v>
       </c>
@@ -1613,7 +1615,7 @@
       <c r="E57" s="13"/>
       <c r="F57" s="13"/>
     </row>
-    <row r="58" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="16"/>
       <c r="B58" s="17" t="s">
         <v>25</v>
@@ -1629,7 +1631,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="59" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="16"/>
       <c r="B59" s="5" t="s">
         <v>26</v>
@@ -1645,7 +1647,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="60" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="16"/>
       <c r="B60" s="5" t="s">
         <v>14</v>
@@ -1661,7 +1663,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="61" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="16"/>
       <c r="B61" s="5" t="s">
         <v>14</v>
@@ -1677,7 +1679,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="62" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="16"/>
       <c r="B62" s="21" t="s">
         <v>69</v>
@@ -1687,7 +1689,7 @@
       <c r="E62" s="17"/>
       <c r="F62" s="17"/>
     </row>
-    <row r="63" spans="1:6" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="24"/>
       <c r="B63" s="23" t="s">
         <v>70</v>
@@ -1699,7 +1701,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="64" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="12">
         <v>1</v>
       </c>
@@ -1711,7 +1713,7 @@
       <c r="E64" s="13"/>
       <c r="F64" s="13"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="14"/>
       <c r="B65" s="5" t="s">
         <v>28</v>
@@ -1727,7 +1729,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="14"/>
       <c r="B66" s="5" t="s">
         <v>37</v>
@@ -1744,7 +1746,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="14"/>
       <c r="B67" s="5" t="s">
         <v>27</v>
@@ -1761,7 +1763,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="14"/>
       <c r="B68" s="5" t="s">
         <v>55</v>
@@ -1775,7 +1777,7 @@
       </c>
       <c r="F68" s="5"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="14"/>
       <c r="B69" s="5" t="s">
         <v>52</v>
@@ -1789,7 +1791,7 @@
       </c>
       <c r="F69" s="5"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="14"/>
       <c r="B70" s="5" t="s">
         <v>54</v>
@@ -1805,7 +1807,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="14"/>
       <c r="B71" s="5" t="s">
         <v>53</v>
@@ -1821,7 +1823,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="14"/>
       <c r="B72" s="5" t="s">
         <v>52</v>
@@ -1835,7 +1837,7 @@
       </c>
       <c r="F72" s="5"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="14"/>
       <c r="B73" s="22" t="s">
         <v>48</v>
@@ -1849,7 +1851,7 @@
       </c>
       <c r="F73" s="5"/>
     </row>
-    <row r="74" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="12">
         <v>2</v>
       </c>
@@ -1861,7 +1863,7 @@
       <c r="E74" s="13"/>
       <c r="F74" s="13"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="14"/>
       <c r="B75" s="5" t="s">
         <v>50</v>
@@ -1875,7 +1877,7 @@
       </c>
       <c r="F75" s="5"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="14"/>
       <c r="B76" s="5" t="s">
         <v>51</v>
@@ -1889,7 +1891,7 @@
       </c>
       <c r="F76" s="5"/>
     </row>
-    <row r="77" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="12">
         <v>1</v>
       </c>
@@ -1901,7 +1903,7 @@
       <c r="E77" s="13"/>
       <c r="F77" s="13"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="14"/>
       <c r="B78" s="21" t="s">
         <v>64</v>
@@ -1911,7 +1913,7 @@
       <c r="E78" s="5"/>
       <c r="F78" s="5"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="14"/>
       <c r="B79" s="23" t="s">
         <v>65</v>
@@ -1925,7 +1927,7 @@
       </c>
       <c r="F79" s="5"/>
     </row>
-    <row r="80" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="12">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Consultas para mostrar las recetas al usuario según sus ingredientes
</commit_message>
<xml_diff>
--- a/documentacion/Tareas.xlsx
+++ b/documentacion/Tareas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique/GitHubProjects/RecetApp/documentacion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Desktop\Universidad\4ºAño\ISO\RecetApp\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234A85E8-970E-A044-83E3-61F3BB53E58D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1847934-2AE1-458E-AAD7-42F122872E30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="33600" windowHeight="18840" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="72">
   <si>
     <t>CREACIÓN DE UNA CUENTA</t>
   </si>
@@ -195,9 +195,6 @@
     <t>Mostrar la lista de recetas por pantalla de la base de datos</t>
   </si>
   <si>
-    <t>Validar que la consulta sale por pantalla</t>
-  </si>
-  <si>
     <t>Crear opción de añadir estos parámetros fuera del registro</t>
   </si>
   <si>
@@ -247,15 +244,28 @@
   </si>
   <si>
     <t>Crear un fichero para insertar recetas</t>
+  </si>
+  <si>
+    <t>Validar que la consultas salen por pantalla</t>
+  </si>
+  <si>
+    <t>Implementar las consultas en el código.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -366,57 +376,58 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -733,20 +744,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66436974-768D-9A40-9A43-2F0986DDE03B}">
   <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="B58" zoomScale="88" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="1"/>
-    <col min="2" max="2" width="116.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.69921875" style="1"/>
+    <col min="2" max="2" width="116.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.19921875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>17</v>
       </c>
@@ -766,7 +777,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -780,7 +791,7 @@
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
       <c r="B3" s="6" t="s">
         <v>1</v>
@@ -796,7 +807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="14"/>
       <c r="B4" s="6" t="s">
         <v>1</v>
@@ -812,7 +823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
@@ -828,7 +839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="6" t="s">
         <v>1</v>
@@ -844,7 +855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="6" t="s">
         <v>31</v>
@@ -860,7 +871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="6" t="s">
         <v>31</v>
@@ -876,7 +887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="6" t="s">
         <v>31</v>
@@ -892,7 +903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="6" t="s">
         <v>31</v>
@@ -908,7 +919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="6" t="s">
         <v>31</v>
@@ -924,7 +935,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="6" t="s">
         <v>2</v>
@@ -940,7 +951,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="6" t="s">
         <v>29</v>
@@ -956,7 +967,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="6" t="s">
         <v>29</v>
@@ -972,7 +983,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="6" t="s">
         <v>30</v>
@@ -988,7 +999,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="6" t="s">
         <v>32</v>
@@ -1004,7 +1015,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="6" t="s">
         <v>36</v>
@@ -1020,7 +1031,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="6" t="s">
         <v>36</v>
@@ -1036,7 +1047,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="22" t="s">
         <v>3</v>
@@ -1052,7 +1063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>1</v>
       </c>
@@ -1064,10 +1075,10 @@
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
     </row>
-    <row r="21" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C21" s="17"/>
       <c r="D21" s="28" t="s">
@@ -1076,7 +1087,7 @@
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="6" t="s">
         <v>40</v>
@@ -1090,7 +1101,7 @@
       </c>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="6" t="s">
         <v>39</v>
@@ -1104,10 +1115,10 @@
       </c>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
       <c r="B24" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C24" s="15"/>
       <c r="D24" s="5" t="s">
@@ -1118,9 +1129,9 @@
       </c>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B25" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D25" s="21" t="s">
         <v>34</v>
@@ -1129,7 +1140,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>1</v>
       </c>
@@ -1143,7 +1154,7 @@
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
       <c r="B27" s="5" t="s">
         <v>5</v>
@@ -1159,7 +1170,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
       <c r="B28" s="5" t="s">
         <v>5</v>
@@ -1175,7 +1186,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="B29" s="5" t="s">
         <v>6</v>
@@ -1191,7 +1202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="14"/>
       <c r="B30" s="5" t="s">
         <v>7</v>
@@ -1207,7 +1218,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="14"/>
       <c r="B31" s="5" t="s">
         <v>8</v>
@@ -1223,10 +1234,10 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="14"/>
       <c r="B32" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C32" s="15"/>
       <c r="D32" s="21" t="s">
@@ -1239,7 +1250,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="14"/>
       <c r="B33" s="22" t="s">
         <v>37</v>
@@ -1255,7 +1266,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="14"/>
       <c r="B34" s="22" t="s">
         <v>37</v>
@@ -1271,10 +1282,10 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="14"/>
       <c r="B35" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C35" s="15"/>
       <c r="D35" s="21" t="s">
@@ -1287,7 +1298,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="12">
         <v>1</v>
       </c>
@@ -1301,7 +1312,7 @@
       <c r="E36" s="13"/>
       <c r="F36" s="13"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="14"/>
       <c r="B37" s="5" t="s">
         <v>10</v>
@@ -1317,7 +1328,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="14"/>
       <c r="B38" s="5" t="s">
         <v>42</v>
@@ -1333,7 +1344,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="14"/>
       <c r="B39" s="5" t="s">
         <v>42</v>
@@ -1349,7 +1360,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="14"/>
       <c r="B40" s="5" t="s">
         <v>36</v>
@@ -1365,7 +1376,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="14"/>
       <c r="B41" s="5" t="s">
         <v>36</v>
@@ -1381,7 +1392,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="14"/>
       <c r="B42" s="5" t="s">
         <v>21</v>
@@ -1397,12 +1408,12 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="12">
         <v>1</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C43" s="13" t="s">
         <v>19</v>
@@ -1411,7 +1422,7 @@
       <c r="E43" s="13"/>
       <c r="F43" s="13"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="14"/>
       <c r="B44" s="5" t="s">
         <v>22</v>
@@ -1427,7 +1438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="14"/>
       <c r="B45" s="5" t="s">
         <v>23</v>
@@ -1443,10 +1454,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="14"/>
       <c r="B46" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C46" s="15"/>
       <c r="D46" s="5" t="s">
@@ -1459,7 +1470,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="12">
         <v>1</v>
       </c>
@@ -1473,7 +1484,7 @@
       <c r="E47" s="13"/>
       <c r="F47" s="13"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="14"/>
       <c r="B48" s="5" t="s">
         <v>12</v>
@@ -1489,7 +1500,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="14"/>
       <c r="B49" s="5" t="s">
         <v>43</v>
@@ -1505,7 +1516,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="14"/>
       <c r="B50" s="5" t="s">
         <v>36</v>
@@ -1521,7 +1532,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="14"/>
       <c r="B51" s="5" t="s">
         <v>36</v>
@@ -1537,7 +1548,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="14"/>
       <c r="B52" s="5" t="s">
         <v>36</v>
@@ -1553,7 +1564,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="14"/>
       <c r="B53" s="5" t="s">
         <v>11</v>
@@ -1569,10 +1580,10 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="16"/>
       <c r="B54" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C54" s="15"/>
       <c r="D54" s="17" t="s">
@@ -1585,7 +1596,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="14"/>
       <c r="B55" s="5" t="s">
         <v>38</v>
@@ -1601,22 +1612,22 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="56" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="12">
         <v>1</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C56" s="13"/>
       <c r="D56" s="13"/>
       <c r="E56" s="13"/>
       <c r="F56" s="13"/>
     </row>
-    <row r="57" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="16"/>
       <c r="B57" s="28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C57" s="15"/>
       <c r="D57" s="17" t="s">
@@ -1629,10 +1640,10 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="58" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="16"/>
       <c r="B58" s="27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C58" s="15"/>
       <c r="D58" s="28" t="s">
@@ -1645,10 +1656,10 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="59" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="16"/>
       <c r="B59" s="27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C59" s="15"/>
       <c r="D59" s="28" t="s">
@@ -1661,7 +1672,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="60" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="16"/>
       <c r="B60" s="5" t="s">
         <v>14</v>
@@ -1677,7 +1688,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="61" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="16"/>
       <c r="B61" s="5" t="s">
         <v>14</v>
@@ -1693,10 +1704,10 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="62" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="16"/>
       <c r="B62" s="27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C62" s="25"/>
       <c r="D62" s="18" t="s">
@@ -1705,10 +1716,10 @@
       <c r="E62" s="17"/>
       <c r="F62" s="17"/>
     </row>
-    <row r="63" spans="1:6" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A63" s="24"/>
       <c r="B63" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D63" s="21" t="s">
         <v>34</v>
@@ -1717,7 +1728,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="64" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="12">
         <v>1</v>
       </c>
@@ -1729,7 +1740,7 @@
       <c r="E64" s="13"/>
       <c r="F64" s="13"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="14"/>
       <c r="B65" s="5" t="s">
         <v>26</v>
@@ -1745,7 +1756,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="14"/>
       <c r="B66" s="5" t="s">
         <v>35</v>
@@ -1762,12 +1773,12 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="14"/>
       <c r="B67" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C67" s="5"/>
+      <c r="C67" s="15"/>
       <c r="D67" s="5" t="s">
         <v>34</v>
       </c>
@@ -1775,28 +1786,30 @@
         <v>2</v>
       </c>
       <c r="F67" s="5">
-        <f>1+2+2</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+        <f>1+2+2+0.25</f>
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="14"/>
-      <c r="B68" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C68" s="5"/>
+      <c r="B68" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="C68" s="15"/>
       <c r="D68" s="5" t="s">
         <v>34</v>
       </c>
       <c r="E68" s="5">
         <v>0.1</v>
       </c>
-      <c r="F68" s="5"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F68" s="5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="14"/>
-      <c r="B69" s="5" t="s">
-        <v>50</v>
+      <c r="B69" s="30" t="s">
+        <v>71</v>
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="5" t="s">
@@ -1807,7 +1820,7 @@
       </c>
       <c r="F69" s="5"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="14"/>
       <c r="B70" s="5" t="s">
         <v>52</v>
@@ -1823,7 +1836,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="14"/>
       <c r="B71" s="5" t="s">
         <v>51</v>
@@ -1839,7 +1852,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="14"/>
       <c r="B72" s="5" t="s">
         <v>50</v>
@@ -1853,7 +1866,7 @@
       </c>
       <c r="F72" s="5"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="14"/>
       <c r="B73" s="22" t="s">
         <v>46</v>
@@ -1867,7 +1880,7 @@
       </c>
       <c r="F73" s="5"/>
     </row>
-    <row r="74" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="12">
         <v>2</v>
       </c>
@@ -1879,7 +1892,7 @@
       <c r="E74" s="13"/>
       <c r="F74" s="13"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="14"/>
       <c r="B75" s="5" t="s">
         <v>48</v>
@@ -1893,7 +1906,7 @@
       </c>
       <c r="F75" s="5"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="14"/>
       <c r="B76" s="27" t="s">
         <v>49</v>
@@ -1907,22 +1920,22 @@
       </c>
       <c r="F76" s="5"/>
     </row>
-    <row r="77" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="12">
         <v>1</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C77" s="13"/>
       <c r="D77" s="13"/>
       <c r="E77" s="13"/>
       <c r="F77" s="13"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="14"/>
       <c r="B78" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="27" t="s">
@@ -1931,10 +1944,10 @@
       <c r="E78" s="5"/>
       <c r="F78" s="5"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="14"/>
       <c r="B79" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="21" t="s">
@@ -1945,19 +1958,19 @@
       </c>
       <c r="F79" s="5"/>
     </row>
-    <row r="80" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="12">
         <v>1</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C80" s="13"/>
       <c r="D80" s="13"/>
       <c r="E80" s="13"/>
       <c r="F80" s="13"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B81" s="27"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualizando tracking, añadiendo nueva tarea de investigacion del framework echo
</commit_message>
<xml_diff>
--- a/documentacion/Tareas.xlsx
+++ b/documentacion/Tareas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique/GitHubProjects/RecetApp/documentacion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/481f6a27916b9a84/Documentos/RecetApp/documentacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{536C58A0-E532-D645-8810-69BDA572FE6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="114_{5E53CC85-8C94-4E51-A24A-B3ED43F82F48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E35AA343-F008-4F21-97DF-0AFB80E78528}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33280" windowHeight="18960" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="99">
   <si>
     <t>CREACIÓN DE UNA CUENTA</t>
   </si>
@@ -327,15 +327,25 @@
   </si>
   <si>
     <t>FECHA ENTREGA</t>
+  </si>
+  <si>
+    <t>Investigar funcionamiento de Echo (framework web de Go)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -489,73 +499,79 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -870,25 +886,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66436974-768D-9A40-9A43-2F0986DDE03B}">
-  <dimension ref="A1:G106"/>
+  <dimension ref="A1:G107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="B61" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="28"/>
-    <col min="2" max="2" width="116.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="14"/>
-    <col min="4" max="4" width="36.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.69921875" style="28"/>
+    <col min="2" max="2" width="116.19921875" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.796875" style="14"/>
+    <col min="4" max="4" width="36.19921875" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.19921875" style="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="14"/>
+    <col min="7" max="7" width="15.19921875" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.796875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>17</v>
       </c>
@@ -911,7 +927,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -928,7 +944,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="15"/>
       <c r="B3" s="16" t="s">
         <v>1</v>
@@ -944,7 +960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="15"/>
       <c r="B4" s="16" t="s">
         <v>1</v>
@@ -960,7 +976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="15"/>
       <c r="B5" s="16" t="s">
         <v>1</v>
@@ -976,7 +992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="15"/>
       <c r="B6" s="16" t="s">
         <v>1</v>
@@ -992,7 +1008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="15"/>
       <c r="B7" s="16" t="s">
         <v>31</v>
@@ -1008,7 +1024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="15"/>
       <c r="B8" s="16" t="s">
         <v>31</v>
@@ -1024,7 +1040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="15"/>
       <c r="B9" s="16" t="s">
         <v>31</v>
@@ -1040,7 +1056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="15"/>
       <c r="B10" s="16" t="s">
         <v>31</v>
@@ -1056,7 +1072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="15"/>
       <c r="B11" s="16" t="s">
         <v>31</v>
@@ -1072,7 +1088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="15"/>
       <c r="B12" s="16" t="s">
         <v>2</v>
@@ -1088,7 +1104,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="15"/>
       <c r="B13" s="16" t="s">
         <v>29</v>
@@ -1104,7 +1120,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="15"/>
       <c r="B14" s="16" t="s">
         <v>29</v>
@@ -1120,7 +1136,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="15"/>
       <c r="B15" s="20" t="s">
         <v>30</v>
@@ -1136,7 +1152,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="15"/>
       <c r="B16" s="16" t="s">
         <v>32</v>
@@ -1152,7 +1168,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="15"/>
       <c r="B17" s="16" t="s">
         <v>36</v>
@@ -1168,7 +1184,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="15"/>
       <c r="B18" s="16" t="s">
         <v>36</v>
@@ -1184,7 +1200,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="15"/>
       <c r="B19" s="21" t="s">
         <v>3</v>
@@ -1200,7 +1216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>1</v>
       </c>
@@ -1215,7 +1231,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
       <c r="B21" s="23" t="s">
         <v>52</v>
@@ -1228,7 +1244,7 @@
       <c r="F21" s="24"/>
       <c r="G21" s="26"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="15"/>
       <c r="B22" s="16" t="s">
         <v>40</v>
@@ -1242,7 +1258,7 @@
       </c>
       <c r="F22" s="18"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="15"/>
       <c r="B23" s="16" t="s">
         <v>39</v>
@@ -1256,7 +1272,7 @@
       </c>
       <c r="F23" s="18"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="15"/>
       <c r="B24" s="16" t="s">
         <v>57</v>
@@ -1270,7 +1286,7 @@
       </c>
       <c r="F24" s="18"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B25" s="29" t="s">
         <v>62</v>
       </c>
@@ -1281,7 +1297,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>1</v>
       </c>
@@ -1298,7 +1314,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="15"/>
       <c r="B27" s="18" t="s">
         <v>5</v>
@@ -1314,7 +1330,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="15"/>
       <c r="B28" s="18" t="s">
         <v>5</v>
@@ -1330,7 +1346,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="15"/>
       <c r="B29" s="18" t="s">
         <v>6</v>
@@ -1346,7 +1362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="15"/>
       <c r="B30" s="18" t="s">
         <v>7</v>
@@ -1362,7 +1378,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="15"/>
       <c r="B31" s="18" t="s">
         <v>8</v>
@@ -1378,7 +1394,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="15"/>
       <c r="B32" s="32" t="s">
         <v>58</v>
@@ -1394,7 +1410,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="15"/>
       <c r="B33" s="21" t="s">
         <v>37</v>
@@ -1410,7 +1426,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="15"/>
       <c r="B34" s="21" t="s">
         <v>37</v>
@@ -1426,7 +1442,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="15"/>
       <c r="B35" s="29" t="s">
         <v>65</v>
@@ -1442,7 +1458,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>1</v>
       </c>
@@ -1459,7 +1475,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="15"/>
       <c r="B37" s="18" t="s">
         <v>10</v>
@@ -1475,7 +1491,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="15"/>
       <c r="B38" s="18" t="s">
         <v>42</v>
@@ -1491,7 +1507,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="15"/>
       <c r="B39" s="18" t="s">
         <v>42</v>
@@ -1507,7 +1523,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="15"/>
       <c r="B40" s="18" t="s">
         <v>36</v>
@@ -1523,7 +1539,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="15"/>
       <c r="B41" s="18" t="s">
         <v>36</v>
@@ -1539,7 +1555,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="15"/>
       <c r="B42" s="18" t="s">
         <v>21</v>
@@ -1555,7 +1571,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>1</v>
       </c>
@@ -1572,7 +1588,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="15"/>
       <c r="B44" s="18" t="s">
         <v>22</v>
@@ -1588,7 +1604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="15"/>
       <c r="B45" s="18" t="s">
         <v>23</v>
@@ -1604,7 +1620,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="15"/>
       <c r="B46" s="21" t="s">
         <v>59</v>
@@ -1620,7 +1636,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>1</v>
       </c>
@@ -1637,7 +1653,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="15"/>
       <c r="B48" s="18" t="s">
         <v>12</v>
@@ -1653,7 +1669,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="15"/>
       <c r="B49" s="18" t="s">
         <v>43</v>
@@ -1669,7 +1685,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="15"/>
       <c r="B50" s="18" t="s">
         <v>36</v>
@@ -1685,7 +1701,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="15"/>
       <c r="B51" s="18" t="s">
         <v>36</v>
@@ -1701,7 +1717,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="15"/>
       <c r="B52" s="18" t="s">
         <v>36</v>
@@ -1717,7 +1733,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="15"/>
       <c r="B53" s="18" t="s">
         <v>11</v>
@@ -1733,7 +1749,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="54" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="22"/>
       <c r="B54" s="32" t="s">
         <v>53</v>
@@ -1750,7 +1766,7 @@
       </c>
       <c r="G54" s="26"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="15"/>
       <c r="B55" s="18" t="s">
         <v>38</v>
@@ -1766,7 +1782,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="56" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>1</v>
       </c>
@@ -1781,7 +1797,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="57" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="22"/>
       <c r="B57" s="25" t="s">
         <v>67</v>
@@ -1798,7 +1814,7 @@
       </c>
       <c r="G57" s="26"/>
     </row>
-    <row r="58" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="22"/>
       <c r="B58" s="35" t="s">
         <v>68</v>
@@ -1815,7 +1831,7 @@
       </c>
       <c r="G58" s="26"/>
     </row>
-    <row r="59" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="22"/>
       <c r="B59" s="35" t="s">
         <v>68</v>
@@ -1832,7 +1848,7 @@
       </c>
       <c r="G59" s="26"/>
     </row>
-    <row r="60" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="22"/>
       <c r="B60" s="18" t="s">
         <v>14</v>
@@ -1849,7 +1865,7 @@
       </c>
       <c r="G60" s="26"/>
     </row>
-    <row r="61" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="22"/>
       <c r="B61" s="18" t="s">
         <v>14</v>
@@ -1866,7 +1882,7 @@
       </c>
       <c r="G61" s="26"/>
     </row>
-    <row r="62" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="22"/>
       <c r="B62" s="35" t="s">
         <v>66</v>
@@ -1879,7 +1895,7 @@
       <c r="F62" s="24"/>
       <c r="G62" s="26"/>
     </row>
-    <row r="63" spans="1:7" s="30" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" s="30" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A63" s="37"/>
       <c r="B63" s="29" t="s">
         <v>64</v>
@@ -1892,7 +1908,7 @@
       </c>
       <c r="G63" s="38"/>
     </row>
-    <row r="64" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>1</v>
       </c>
@@ -1907,7 +1923,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="15"/>
       <c r="B65" s="18" t="s">
         <v>26</v>
@@ -1923,7 +1939,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="15"/>
       <c r="B66" s="18" t="s">
         <v>35</v>
@@ -1940,7 +1956,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="15"/>
       <c r="B67" s="18" t="s">
         <v>25</v>
@@ -1957,7 +1973,7 @@
         <v>5.25</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="15"/>
       <c r="B68" s="18" t="s">
         <v>25</v>
@@ -1973,7 +1989,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="15"/>
       <c r="B69" s="40" t="s">
         <v>69</v>
@@ -1989,7 +2005,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="15"/>
       <c r="B70" s="40" t="s">
         <v>70</v>
@@ -2003,7 +2019,7 @@
       </c>
       <c r="F70" s="18"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="15"/>
       <c r="B71" s="18" t="s">
         <v>51</v>
@@ -2019,7 +2035,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="15"/>
       <c r="B72" s="18" t="s">
         <v>50</v>
@@ -2035,7 +2051,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="15"/>
       <c r="B73" s="21" t="s">
         <v>46</v>
@@ -2049,7 +2065,7 @@
       </c>
       <c r="F73" s="18"/>
     </row>
-    <row r="74" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>2</v>
       </c>
@@ -2064,7 +2080,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="15"/>
       <c r="B75" s="18" t="s">
         <v>48</v>
@@ -2078,7 +2094,7 @@
       </c>
       <c r="F75" s="18"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="15"/>
       <c r="B76" s="35" t="s">
         <v>49</v>
@@ -2092,7 +2108,7 @@
       </c>
       <c r="F76" s="18"/>
     </row>
-    <row r="77" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>1</v>
       </c>
@@ -2107,7 +2123,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="15"/>
       <c r="B78" s="41" t="s">
         <v>60</v>
@@ -2119,7 +2135,7 @@
       <c r="E78" s="18"/>
       <c r="F78" s="18"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="15"/>
       <c r="B79" s="29" t="s">
         <v>61</v>
@@ -2133,7 +2149,7 @@
       </c>
       <c r="F79" s="18"/>
     </row>
-    <row r="80" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>1</v>
       </c>
@@ -2148,245 +2164,260 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="81" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="6">
-        <v>2</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G81" s="4"/>
-    </row>
-    <row r="82" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="42"/>
+      <c r="B81" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="C81" s="36"/>
+      <c r="D81" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="E81" s="36">
+        <v>10</v>
+      </c>
+      <c r="F81" s="36"/>
+      <c r="G81" s="43"/>
+    </row>
+    <row r="82" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="6">
         <v>2</v>
       </c>
-      <c r="B82" s="7" t="s">
-        <v>72</v>
+      <c r="B82" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="G82" s="4"/>
     </row>
-    <row r="83" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="6">
         <v>2</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G83" s="4"/>
     </row>
-    <row r="84" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="6">
         <v>2</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G84" s="4"/>
     </row>
-    <row r="85" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="6">
         <v>2</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G85" s="4"/>
     </row>
-    <row r="86" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="6">
         <v>2</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G86" s="4"/>
     </row>
-    <row r="87" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="6">
         <v>2</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G87" s="4">
-        <v>44155</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+      <c r="G87" s="4"/>
+    </row>
+    <row r="88" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="6">
         <v>2</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G88" s="4">
         <v>44155</v>
       </c>
     </row>
-    <row r="89" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="6">
         <v>2</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G89" s="4">
         <v>44155</v>
       </c>
     </row>
-    <row r="90" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="6">
         <v>2</v>
       </c>
       <c r="B90" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G90" s="4">
+        <v>44155</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="6">
+        <v>2</v>
+      </c>
+      <c r="B91" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="G90" s="4"/>
-    </row>
-    <row r="91" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="6">
-        <v>3</v>
-      </c>
-      <c r="B91" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="G91" s="4"/>
     </row>
-    <row r="92" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="6">
         <v>3</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G92" s="4"/>
     </row>
-    <row r="93" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="6">
         <v>3</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G93" s="4"/>
     </row>
-    <row r="94" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="6">
         <v>3</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G94" s="4"/>
     </row>
-    <row r="95" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="6">
         <v>3</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G95" s="4"/>
     </row>
-    <row r="96" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="6">
         <v>3</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G96" s="4"/>
     </row>
-    <row r="97" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="6">
         <v>3</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G97" s="4"/>
     </row>
-    <row r="98" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="6">
         <v>3</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G98" s="4"/>
     </row>
-    <row r="99" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="6">
         <v>3</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G99" s="4"/>
     </row>
-    <row r="100" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="6">
         <v>3</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G100" s="4"/>
     </row>
-    <row r="101" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="6">
         <v>3</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G101" s="4"/>
     </row>
-    <row r="102" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="6">
         <v>3</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G102" s="4"/>
     </row>
-    <row r="103" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="6">
         <v>3</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G103" s="4"/>
     </row>
-    <row r="104" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A104" s="6">
         <v>3</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G104" s="4"/>
     </row>
-    <row r="105" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A105" s="6">
         <v>3</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G105" s="4"/>
     </row>
-    <row r="106" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A106" s="6">
         <v>3</v>
       </c>
       <c r="B106" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G106" s="4"/>
+    </row>
+    <row r="107" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="6">
+        <v>3</v>
+      </c>
+      <c r="B107" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="G106" s="4"/>
+      <c r="G107" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
actualizando tracking y añadiendo algunas tareas más
</commit_message>
<xml_diff>
--- a/documentacion/Tareas.xlsx
+++ b/documentacion/Tareas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique/GitHubProjects/RecetApp/documentacion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/481f6a27916b9a84/Documentos/RecetApp/documentacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4CD5AF-0EBC-6A47-A01D-E0CA34031A16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="114_{25AB7519-D560-47BF-A0B3-B864C1AB14AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0F60A6AC-DBBB-4CF2-B05C-647F0D394ECA}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33380" windowHeight="19020" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="104">
   <si>
     <t>CREACIÓN DE UNA CUENTA</t>
   </si>
@@ -212,9 +212,6 @@
     <t>Permitir al usuario hacer un nuevo login al equivocarse sin salir de la aplicación</t>
   </si>
   <si>
-    <t>Validar que un usuario que ha accedido a la aplicación puede añadir ingresientes a su inventario</t>
-  </si>
-  <si>
     <t>Colocar en el código una condición que no permita introducir el mismo ingrediente más de una vez a un usuario</t>
   </si>
   <si>
@@ -333,15 +330,37 @@
   </si>
   <si>
     <t>Aprender a utilizar las herramientas de testing en Go (setup y teardown)</t>
+  </si>
+  <si>
+    <t>Validar que un usuario que ha accedido a la aplicación puede añadir ingredientes a su inventario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crear pantalla de login </t>
+  </si>
+  <si>
+    <t>Crear pantalla para introducir recetas</t>
+  </si>
+  <si>
+    <t>Crear pantalla para buscar ingredientes</t>
+  </si>
+  <si>
+    <t>Crear pantalla de registro de usuario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -407,6 +426,14 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -502,80 +529,83 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -890,25 +920,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66436974-768D-9A40-9A43-2F0986DDE03B}">
-  <dimension ref="A1:G108"/>
+  <dimension ref="A1:G112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="118" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="28"/>
-    <col min="2" max="2" width="116.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="14"/>
-    <col min="4" max="4" width="36.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.69921875" style="28"/>
+    <col min="2" max="2" width="116.19921875" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.796875" style="14"/>
+    <col min="4" max="4" width="36.19921875" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.19921875" style="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="14"/>
+    <col min="7" max="7" width="15.19921875" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.796875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>17</v>
       </c>
@@ -928,10 +958,10 @@
         <v>45</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -948,7 +978,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="15"/>
       <c r="B3" s="16" t="s">
         <v>1</v>
@@ -964,7 +994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="15"/>
       <c r="B4" s="16" t="s">
         <v>1</v>
@@ -980,7 +1010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="15"/>
       <c r="B5" s="16" t="s">
         <v>1</v>
@@ -996,7 +1026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="15"/>
       <c r="B6" s="16" t="s">
         <v>1</v>
@@ -1012,7 +1042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="15"/>
       <c r="B7" s="16" t="s">
         <v>31</v>
@@ -1028,7 +1058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="15"/>
       <c r="B8" s="16" t="s">
         <v>31</v>
@@ -1044,7 +1074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="15"/>
       <c r="B9" s="16" t="s">
         <v>31</v>
@@ -1060,7 +1090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="15"/>
       <c r="B10" s="16" t="s">
         <v>31</v>
@@ -1076,7 +1106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="15"/>
       <c r="B11" s="16" t="s">
         <v>31</v>
@@ -1092,7 +1122,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="15"/>
       <c r="B12" s="16" t="s">
         <v>2</v>
@@ -1108,7 +1138,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="15"/>
       <c r="B13" s="16" t="s">
         <v>29</v>
@@ -1124,7 +1154,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="15"/>
       <c r="B14" s="16" t="s">
         <v>29</v>
@@ -1140,7 +1170,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="15"/>
       <c r="B15" s="20" t="s">
         <v>30</v>
@@ -1156,7 +1186,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="15"/>
       <c r="B16" s="16" t="s">
         <v>32</v>
@@ -1172,7 +1202,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="15"/>
       <c r="B17" s="16" t="s">
         <v>36</v>
@@ -1188,7 +1218,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="15"/>
       <c r="B18" s="16" t="s">
         <v>36</v>
@@ -1204,7 +1234,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="15"/>
       <c r="B19" s="21" t="s">
         <v>3</v>
@@ -1220,7 +1250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>1</v>
       </c>
@@ -1235,7 +1265,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
       <c r="B21" s="23" t="s">
         <v>52</v>
@@ -1248,7 +1278,7 @@
       <c r="F21" s="24"/>
       <c r="G21" s="26"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="15"/>
       <c r="B22" s="16" t="s">
         <v>40</v>
@@ -1262,7 +1292,7 @@
       </c>
       <c r="F22" s="18"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="15"/>
       <c r="B23" s="16" t="s">
         <v>39</v>
@@ -1276,7 +1306,7 @@
       </c>
       <c r="F23" s="18"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="15"/>
       <c r="B24" s="16" t="s">
         <v>57</v>
@@ -1290,9 +1320,9 @@
       </c>
       <c r="F24" s="18"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B25" s="29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D25" s="30" t="s">
         <v>34</v>
@@ -1301,7 +1331,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>1</v>
       </c>
@@ -1318,7 +1348,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="15"/>
       <c r="B27" s="18" t="s">
         <v>5</v>
@@ -1334,7 +1364,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="15"/>
       <c r="B28" s="18" t="s">
         <v>5</v>
@@ -1350,7 +1380,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="15"/>
       <c r="B29" s="18" t="s">
         <v>6</v>
@@ -1366,7 +1396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="15"/>
       <c r="B30" s="18" t="s">
         <v>7</v>
@@ -1382,7 +1412,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="15"/>
       <c r="B31" s="18" t="s">
         <v>8</v>
@@ -1398,7 +1428,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="15"/>
       <c r="B32" s="32" t="s">
         <v>58</v>
@@ -1414,7 +1444,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="15"/>
       <c r="B33" s="21" t="s">
         <v>37</v>
@@ -1430,7 +1460,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="15"/>
       <c r="B34" s="21" t="s">
         <v>37</v>
@@ -1446,10 +1476,10 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="15"/>
       <c r="B35" s="29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C35" s="17"/>
       <c r="D35" s="30" t="s">
@@ -1462,7 +1492,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>1</v>
       </c>
@@ -1479,7 +1509,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="15"/>
       <c r="B37" s="18" t="s">
         <v>10</v>
@@ -1495,7 +1525,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="15"/>
       <c r="B38" s="18" t="s">
         <v>42</v>
@@ -1511,7 +1541,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="15"/>
       <c r="B39" s="18" t="s">
         <v>42</v>
@@ -1527,7 +1557,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="15"/>
       <c r="B40" s="18" t="s">
         <v>36</v>
@@ -1543,7 +1573,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="15"/>
       <c r="B41" s="18" t="s">
         <v>36</v>
@@ -1559,7 +1589,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="15"/>
       <c r="B42" s="18" t="s">
         <v>21</v>
@@ -1575,12 +1605,12 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>1</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>19</v>
@@ -1592,7 +1622,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="15"/>
       <c r="B44" s="18" t="s">
         <v>22</v>
@@ -1608,7 +1638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="15"/>
       <c r="B45" s="18" t="s">
         <v>23</v>
@@ -1624,10 +1654,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="15"/>
-      <c r="B46" s="21" t="s">
-        <v>59</v>
+      <c r="B46" s="48" t="s">
+        <v>99</v>
       </c>
       <c r="C46" s="17"/>
       <c r="D46" s="18" t="s">
@@ -1640,7 +1670,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>1</v>
       </c>
@@ -1657,7 +1687,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="15"/>
       <c r="B48" s="18" t="s">
         <v>12</v>
@@ -1673,7 +1703,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="15"/>
       <c r="B49" s="18" t="s">
         <v>43</v>
@@ -1689,7 +1719,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="15"/>
       <c r="B50" s="18" t="s">
         <v>36</v>
@@ -1705,7 +1735,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="15"/>
       <c r="B51" s="18" t="s">
         <v>36</v>
@@ -1721,7 +1751,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="15"/>
       <c r="B52" s="18" t="s">
         <v>36</v>
@@ -1737,7 +1767,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="15"/>
       <c r="B53" s="18" t="s">
         <v>11</v>
@@ -1753,7 +1783,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="54" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="22"/>
       <c r="B54" s="32" t="s">
         <v>53</v>
@@ -1770,7 +1800,7 @@
       </c>
       <c r="G54" s="26"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="15"/>
       <c r="B55" s="18" t="s">
         <v>38</v>
@@ -1786,7 +1816,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="56" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>1</v>
       </c>
@@ -1801,10 +1831,10 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="57" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="22"/>
       <c r="B57" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C57" s="17"/>
       <c r="D57" s="24" t="s">
@@ -1818,10 +1848,10 @@
       </c>
       <c r="G57" s="26"/>
     </row>
-    <row r="58" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="22"/>
       <c r="B58" s="35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C58" s="17"/>
       <c r="D58" s="25" t="s">
@@ -1835,10 +1865,10 @@
       </c>
       <c r="G58" s="26"/>
     </row>
-    <row r="59" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="22"/>
       <c r="B59" s="35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C59" s="17"/>
       <c r="D59" s="25" t="s">
@@ -1852,7 +1882,7 @@
       </c>
       <c r="G59" s="26"/>
     </row>
-    <row r="60" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="22"/>
       <c r="B60" s="18" t="s">
         <v>14</v>
@@ -1869,7 +1899,7 @@
       </c>
       <c r="G60" s="26"/>
     </row>
-    <row r="61" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="22"/>
       <c r="B61" s="18" t="s">
         <v>14</v>
@@ -1886,10 +1916,10 @@
       </c>
       <c r="G61" s="26"/>
     </row>
-    <row r="62" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="22"/>
       <c r="B62" s="35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C62" s="36"/>
       <c r="D62" s="33" t="s">
@@ -1899,10 +1929,10 @@
       <c r="F62" s="24"/>
       <c r="G62" s="26"/>
     </row>
-    <row r="63" spans="1:7" s="30" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" s="30" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A63" s="37"/>
       <c r="B63" s="29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D63" s="30" t="s">
         <v>34</v>
@@ -1912,7 +1942,7 @@
       </c>
       <c r="G63" s="38"/>
     </row>
-    <row r="64" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>1</v>
       </c>
@@ -1927,7 +1957,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="15"/>
       <c r="B65" s="18" t="s">
         <v>26</v>
@@ -1943,7 +1973,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="15"/>
       <c r="B66" s="18" t="s">
         <v>35</v>
@@ -1960,7 +1990,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="15"/>
       <c r="B67" s="18" t="s">
         <v>25</v>
@@ -1977,7 +2007,7 @@
         <v>5.25</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="15"/>
       <c r="B68" s="18" t="s">
         <v>25</v>
@@ -1993,10 +2023,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="15"/>
       <c r="B69" s="40" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C69" s="17"/>
       <c r="D69" s="18" t="s">
@@ -2009,10 +2039,10 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="15"/>
       <c r="B70" s="40" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C70" s="18"/>
       <c r="D70" s="18" t="s">
@@ -2023,7 +2053,7 @@
       </c>
       <c r="F70" s="18"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="15"/>
       <c r="B71" s="18" t="s">
         <v>51</v>
@@ -2039,7 +2069,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="15"/>
       <c r="B72" s="18" t="s">
         <v>50</v>
@@ -2055,7 +2085,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="15"/>
       <c r="B73" s="21" t="s">
         <v>46</v>
@@ -2069,7 +2099,7 @@
       </c>
       <c r="F73" s="18"/>
     </row>
-    <row r="74" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>2</v>
       </c>
@@ -2084,10 +2114,10 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="75" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="22"/>
       <c r="B75" s="46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C75" s="24"/>
       <c r="D75" s="46" t="s">
@@ -2101,7 +2131,7 @@
       </c>
       <c r="G75" s="26"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="15"/>
       <c r="B76" s="18" t="s">
         <v>48</v>
@@ -2115,7 +2145,7 @@
       </c>
       <c r="F76" s="18"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="15"/>
       <c r="B77" s="35" t="s">
         <v>49</v>
@@ -2129,7 +2159,7 @@
       </c>
       <c r="F77" s="18"/>
     </row>
-    <row r="78" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>1</v>
       </c>
@@ -2144,10 +2174,10 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="15"/>
       <c r="B79" s="41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C79" s="18"/>
       <c r="D79" s="35" t="s">
@@ -2156,10 +2186,10 @@
       <c r="E79" s="18"/>
       <c r="F79" s="18"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="15"/>
       <c r="B80" s="29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C80" s="18"/>
       <c r="D80" s="30" t="s">
@@ -2170,7 +2200,7 @@
       </c>
       <c r="F80" s="18"/>
     </row>
-    <row r="81" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>1</v>
       </c>
@@ -2185,10 +2215,10 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="82" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="42"/>
       <c r="B82" s="45" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C82" s="36"/>
       <c r="D82" s="45" t="s">
@@ -2200,245 +2230,293 @@
       <c r="F82" s="36"/>
       <c r="G82" s="43"/>
     </row>
-    <row r="83" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="6">
-        <v>2</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G83" s="4"/>
-    </row>
-    <row r="84" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="6">
-        <v>2</v>
-      </c>
-      <c r="B84" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="G84" s="4"/>
-    </row>
-    <row r="85" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="6">
-        <v>2</v>
-      </c>
-      <c r="B85" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="G85" s="4"/>
-    </row>
-    <row r="86" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="6">
-        <v>2</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="G86" s="4"/>
-    </row>
-    <row r="87" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="42"/>
+      <c r="B83" s="47" t="s">
+        <v>100</v>
+      </c>
+      <c r="C83" s="36"/>
+      <c r="D83" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="E83" s="36">
+        <v>3</v>
+      </c>
+      <c r="F83" s="36"/>
+      <c r="G83" s="43"/>
+    </row>
+    <row r="84" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="42"/>
+      <c r="B84" s="47" t="s">
+        <v>103</v>
+      </c>
+      <c r="C84" s="36"/>
+      <c r="D84" s="47"/>
+      <c r="E84" s="36"/>
+      <c r="F84" s="36"/>
+      <c r="G84" s="43"/>
+    </row>
+    <row r="85" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="42"/>
+      <c r="B85" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="C85" s="36"/>
+      <c r="D85" s="45"/>
+      <c r="E85" s="36"/>
+      <c r="F85" s="36"/>
+      <c r="G85" s="43"/>
+    </row>
+    <row r="86" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="42"/>
+      <c r="B86" s="47" t="s">
+        <v>102</v>
+      </c>
+      <c r="C86" s="36"/>
+      <c r="D86" s="45"/>
+      <c r="E86" s="36"/>
+      <c r="F86" s="36"/>
+      <c r="G86" s="43"/>
+    </row>
+    <row r="87" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="6">
         <v>2</v>
       </c>
-      <c r="B87" s="7" t="s">
-        <v>75</v>
+      <c r="B87" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="G87" s="4"/>
     </row>
-    <row r="88" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="6">
         <v>2</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G88" s="4"/>
     </row>
-    <row r="89" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="6">
         <v>2</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G89" s="4">
-        <v>44155</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+      <c r="G89" s="4"/>
+    </row>
+    <row r="90" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="6">
         <v>2</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="G90" s="4">
-        <v>44155</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="G90" s="4"/>
+    </row>
+    <row r="91" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="6">
         <v>2</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G91" s="4">
-        <v>44155</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+      <c r="G91" s="4"/>
+    </row>
+    <row r="92" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="6">
         <v>2</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G92" s="4"/>
     </row>
-    <row r="93" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G93" s="4"/>
-    </row>
-    <row r="94" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+      <c r="G93" s="4">
+        <v>44155</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="G94" s="4"/>
-    </row>
-    <row r="95" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+      <c r="G94" s="4">
+        <v>44155</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="G95" s="4"/>
-    </row>
-    <row r="96" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="G95" s="4">
+        <v>44155</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G96" s="4"/>
     </row>
-    <row r="97" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="6">
         <v>3</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G97" s="4"/>
     </row>
-    <row r="98" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="6">
         <v>3</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G98" s="4"/>
     </row>
-    <row r="99" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="6">
         <v>3</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G99" s="4"/>
     </row>
-    <row r="100" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="6">
         <v>3</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G100" s="4"/>
     </row>
-    <row r="101" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="6">
         <v>3</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G101" s="4"/>
     </row>
-    <row r="102" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="6">
         <v>3</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G102" s="4"/>
     </row>
-    <row r="103" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="6">
         <v>3</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G103" s="4"/>
     </row>
-    <row r="104" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A104" s="6">
         <v>3</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G104" s="4"/>
     </row>
-    <row r="105" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A105" s="6">
         <v>3</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="G105" s="4"/>
     </row>
-    <row r="106" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A106" s="6">
         <v>3</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="G106" s="4"/>
     </row>
-    <row r="107" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A107" s="6">
         <v>3</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G107" s="4"/>
     </row>
-    <row r="108" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" s="6">
         <v>3</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="G108" s="4"/>
+    </row>
+    <row r="109" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="6">
+        <v>3</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G109" s="4"/>
+    </row>
+    <row r="110" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="6">
+        <v>3</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G110" s="4"/>
+    </row>
+    <row r="111" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="6">
+        <v>3</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G111" s="4"/>
+    </row>
+    <row r="112" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="6">
+        <v>3</v>
+      </c>
+      <c r="B112" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G112" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Actualizando tracking y escogiendo tarea de interfaz gráfica
</commit_message>
<xml_diff>
--- a/documentacion/Tareas.xlsx
+++ b/documentacion/Tareas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique/GitHubProjects/RecetApp/documentacion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/481f6a27916b9a84/Documentos/RecetApp/documentacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457F57BC-E7D6-B348-8A04-ABEF9F755BCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="114_{C94F985D-CB23-4A4C-A087-98E54B70A58C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3B3ECE03-0235-4D07-817D-06700470994D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18840" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="107">
   <si>
     <t>CREACIÓN DE UNA CUENTA</t>
   </si>
@@ -360,9 +360,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -544,94 +551,95 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -948,23 +956,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66436974-768D-9A40-9A43-2F0986DDE03B}">
   <dimension ref="A1:G126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="116" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F84" sqref="F84"/>
+    <sheetView tabSelected="1" topLeftCell="C62" zoomScale="116" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="25"/>
-    <col min="2" max="2" width="116.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="11"/>
-    <col min="4" max="4" width="36.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.69921875" style="25"/>
+    <col min="2" max="2" width="116.19921875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.796875" style="11"/>
+    <col min="4" max="4" width="36.19921875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.19921875" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="11"/>
+    <col min="7" max="7" width="15.19921875" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.796875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
@@ -987,7 +995,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="45">
         <v>1</v>
       </c>
@@ -1004,7 +1012,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="12"/>
       <c r="B3" s="13" t="s">
         <v>1</v>
@@ -1020,7 +1028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="12"/>
       <c r="B4" s="13" t="s">
         <v>1</v>
@@ -1036,7 +1044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
       <c r="B5" s="13" t="s">
         <v>1</v>
@@ -1052,7 +1060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="12"/>
       <c r="B6" s="13" t="s">
         <v>1</v>
@@ -1068,7 +1076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="12"/>
       <c r="B7" s="13" t="s">
         <v>31</v>
@@ -1084,7 +1092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="12"/>
       <c r="B8" s="13" t="s">
         <v>31</v>
@@ -1100,7 +1108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
       <c r="B9" s="13" t="s">
         <v>31</v>
@@ -1116,7 +1124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="12"/>
       <c r="B10" s="13" t="s">
         <v>31</v>
@@ -1132,7 +1140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="12"/>
       <c r="B11" s="13" t="s">
         <v>31</v>
@@ -1148,7 +1156,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="12"/>
       <c r="B12" s="13" t="s">
         <v>2</v>
@@ -1164,7 +1172,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="12"/>
       <c r="B13" s="13" t="s">
         <v>29</v>
@@ -1180,7 +1188,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
       <c r="B14" s="13" t="s">
         <v>29</v>
@@ -1196,7 +1204,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="12"/>
       <c r="B15" s="17" t="s">
         <v>30</v>
@@ -1212,7 +1220,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="12"/>
       <c r="B16" s="13" t="s">
         <v>32</v>
@@ -1228,7 +1236,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="12"/>
       <c r="B17" s="13" t="s">
         <v>36</v>
@@ -1244,7 +1252,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="12"/>
       <c r="B18" s="13" t="s">
         <v>36</v>
@@ -1260,7 +1268,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="12"/>
       <c r="B19" s="18" t="s">
         <v>3</v>
@@ -1276,7 +1284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="45">
         <v>1</v>
       </c>
@@ -1291,7 +1299,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="19"/>
       <c r="B21" s="20" t="s">
         <v>52</v>
@@ -1304,7 +1312,7 @@
       <c r="F21" s="21"/>
       <c r="G21" s="23"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="12"/>
       <c r="B22" s="13" t="s">
         <v>40</v>
@@ -1318,7 +1326,7 @@
       </c>
       <c r="F22" s="15"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="12"/>
       <c r="B23" s="13" t="s">
         <v>39</v>
@@ -1332,7 +1340,7 @@
       </c>
       <c r="F23" s="15"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="12"/>
       <c r="B24" s="13" t="s">
         <v>57</v>
@@ -1346,7 +1354,7 @@
       </c>
       <c r="F24" s="15"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B25" s="26" t="s">
         <v>61</v>
       </c>
@@ -1357,7 +1365,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="45">
         <v>1</v>
       </c>
@@ -1374,7 +1382,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="12"/>
       <c r="B27" s="15" t="s">
         <v>5</v>
@@ -1390,7 +1398,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="12"/>
       <c r="B28" s="15" t="s">
         <v>5</v>
@@ -1406,7 +1414,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="12"/>
       <c r="B29" s="15" t="s">
         <v>6</v>
@@ -1422,7 +1430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="12"/>
       <c r="B30" s="15" t="s">
         <v>7</v>
@@ -1438,7 +1446,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="12"/>
       <c r="B31" s="15" t="s">
         <v>8</v>
@@ -1454,7 +1462,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="12"/>
       <c r="B32" s="28" t="s">
         <v>58</v>
@@ -1470,7 +1478,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="12"/>
       <c r="B33" s="18" t="s">
         <v>37</v>
@@ -1486,7 +1494,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="12"/>
       <c r="B34" s="18" t="s">
         <v>37</v>
@@ -1502,7 +1510,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="12"/>
       <c r="B35" s="26" t="s">
         <v>64</v>
@@ -1518,7 +1526,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="45">
         <v>1</v>
       </c>
@@ -1535,7 +1543,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="12"/>
       <c r="B37" s="15" t="s">
         <v>10</v>
@@ -1551,7 +1559,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="12"/>
       <c r="B38" s="15" t="s">
         <v>42</v>
@@ -1567,7 +1575,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="12"/>
       <c r="B39" s="15" t="s">
         <v>42</v>
@@ -1583,7 +1591,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="12"/>
       <c r="B40" s="15" t="s">
         <v>36</v>
@@ -1599,7 +1607,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="12"/>
       <c r="B41" s="15" t="s">
         <v>36</v>
@@ -1615,7 +1623,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="12"/>
       <c r="B42" s="15" t="s">
         <v>21</v>
@@ -1631,7 +1639,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="45">
         <v>1</v>
       </c>
@@ -1648,7 +1656,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="12"/>
       <c r="B44" s="15" t="s">
         <v>22</v>
@@ -1664,7 +1672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="12"/>
       <c r="B45" s="15" t="s">
         <v>23</v>
@@ -1680,7 +1688,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="12"/>
       <c r="B46" s="43" t="s">
         <v>98</v>
@@ -1696,7 +1704,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="45">
         <v>1</v>
       </c>
@@ -1713,7 +1721,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="12"/>
       <c r="B48" s="15" t="s">
         <v>12</v>
@@ -1729,7 +1737,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="12"/>
       <c r="B49" s="15" t="s">
         <v>43</v>
@@ -1745,7 +1753,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="12"/>
       <c r="B50" s="15" t="s">
         <v>36</v>
@@ -1761,7 +1769,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="12"/>
       <c r="B51" s="15" t="s">
         <v>36</v>
@@ -1777,7 +1785,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="12"/>
       <c r="B52" s="15" t="s">
         <v>36</v>
@@ -1793,7 +1801,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="12"/>
       <c r="B53" s="15" t="s">
         <v>11</v>
@@ -1809,7 +1817,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="54" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="19"/>
       <c r="B54" s="28" t="s">
         <v>53</v>
@@ -1826,7 +1834,7 @@
       </c>
       <c r="G54" s="23"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="12"/>
       <c r="B55" s="15" t="s">
         <v>38</v>
@@ -1842,7 +1850,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="56" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="45">
         <v>1</v>
       </c>
@@ -1857,7 +1865,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="57" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="19"/>
       <c r="B57" s="22" t="s">
         <v>66</v>
@@ -1874,7 +1882,7 @@
       </c>
       <c r="G57" s="23"/>
     </row>
-    <row r="58" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="19"/>
       <c r="B58" s="30" t="s">
         <v>67</v>
@@ -1891,7 +1899,7 @@
       </c>
       <c r="G58" s="23"/>
     </row>
-    <row r="59" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="19"/>
       <c r="B59" s="30" t="s">
         <v>67</v>
@@ -1908,7 +1916,7 @@
       </c>
       <c r="G59" s="23"/>
     </row>
-    <row r="60" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="19"/>
       <c r="B60" s="15" t="s">
         <v>14</v>
@@ -1925,7 +1933,7 @@
       </c>
       <c r="G60" s="23"/>
     </row>
-    <row r="61" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="19"/>
       <c r="B61" s="15" t="s">
         <v>14</v>
@@ -1942,7 +1950,7 @@
       </c>
       <c r="G61" s="23"/>
     </row>
-    <row r="62" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="19"/>
       <c r="B62" s="30" t="s">
         <v>65</v>
@@ -1955,7 +1963,7 @@
       <c r="F62" s="21"/>
       <c r="G62" s="23"/>
     </row>
-    <row r="63" spans="1:7" s="27" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" s="27" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A63" s="32"/>
       <c r="B63" s="26" t="s">
         <v>63</v>
@@ -1968,7 +1976,7 @@
       </c>
       <c r="G63" s="33"/>
     </row>
-    <row r="64" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="45">
         <v>1</v>
       </c>
@@ -1983,7 +1991,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="12"/>
       <c r="B65" s="15" t="s">
         <v>26</v>
@@ -1999,7 +2007,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="12"/>
       <c r="B66" s="15" t="s">
         <v>35</v>
@@ -2016,7 +2024,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="12"/>
       <c r="B67" s="15" t="s">
         <v>25</v>
@@ -2033,7 +2041,7 @@
         <v>5.25</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="12"/>
       <c r="B68" s="15" t="s">
         <v>25</v>
@@ -2049,7 +2057,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="12"/>
       <c r="B69" s="35" t="s">
         <v>68</v>
@@ -2065,7 +2073,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="12"/>
       <c r="B70" s="35" t="s">
         <v>69</v>
@@ -2079,7 +2087,7 @@
       </c>
       <c r="F70" s="15"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="12"/>
       <c r="B71" s="15" t="s">
         <v>51</v>
@@ -2095,7 +2103,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="12"/>
       <c r="B72" s="15" t="s">
         <v>50</v>
@@ -2111,7 +2119,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="12"/>
       <c r="B73" s="18" t="s">
         <v>46</v>
@@ -2125,7 +2133,7 @@
       </c>
       <c r="F73" s="15"/>
     </row>
-    <row r="74" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="45">
         <v>2</v>
       </c>
@@ -2140,7 +2148,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="75" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="19"/>
       <c r="B75" s="41" t="s">
         <v>97</v>
@@ -2157,7 +2165,7 @@
       </c>
       <c r="G75" s="23"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="12"/>
       <c r="B76" s="15" t="s">
         <v>48</v>
@@ -2173,7 +2181,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="12"/>
       <c r="B77" s="30" t="s">
         <v>49</v>
@@ -2189,7 +2197,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="78" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="45">
         <v>1</v>
       </c>
@@ -2204,7 +2212,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="12"/>
       <c r="B79" s="36" t="s">
         <v>59</v>
@@ -2216,7 +2224,7 @@
       <c r="E79" s="15"/>
       <c r="F79" s="15"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="12"/>
       <c r="B80" s="26" t="s">
         <v>60</v>
@@ -2230,7 +2238,7 @@
       </c>
       <c r="F80" s="15"/>
     </row>
-    <row r="81" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="45">
         <v>1</v>
       </c>
@@ -2245,7 +2253,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="82" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="37"/>
       <c r="B82" s="40" t="s">
         <v>96</v>
@@ -2260,7 +2268,7 @@
       <c r="F82" s="31"/>
       <c r="G82" s="38"/>
     </row>
-    <row r="83" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="37"/>
       <c r="B83" s="42" t="s">
         <v>106</v>
@@ -2277,7 +2285,7 @@
       </c>
       <c r="G83" s="38"/>
     </row>
-    <row r="84" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="37"/>
       <c r="B84" s="42" t="s">
         <v>99</v>
@@ -2292,18 +2300,22 @@
       <c r="F84" s="31"/>
       <c r="G84" s="38"/>
     </row>
-    <row r="85" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="37"/>
       <c r="B85" s="42" t="s">
         <v>102</v>
       </c>
       <c r="C85" s="31"/>
-      <c r="D85" s="42"/>
-      <c r="E85" s="31"/>
+      <c r="D85" s="57" t="s">
+        <v>27</v>
+      </c>
+      <c r="E85" s="31">
+        <v>5</v>
+      </c>
       <c r="F85" s="31"/>
       <c r="G85" s="38"/>
     </row>
-    <row r="86" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="37"/>
       <c r="B86" s="44" t="s">
         <v>100</v>
@@ -2314,7 +2326,7 @@
       <c r="F86" s="31"/>
       <c r="G86" s="38"/>
     </row>
-    <row r="87" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="37"/>
       <c r="B87" s="42" t="s">
         <v>101</v>
@@ -2325,7 +2337,7 @@
       <c r="F87" s="31"/>
       <c r="G87" s="38"/>
     </row>
-    <row r="88" spans="1:7" s="56" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" s="56" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="55">
         <v>2</v>
       </c>
@@ -2336,7 +2348,7 @@
         <v>44187</v>
       </c>
     </row>
-    <row r="89" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="45">
         <v>2</v>
       </c>
@@ -2351,7 +2363,7 @@
         <v>44187</v>
       </c>
     </row>
-    <row r="90" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="52">
         <v>2</v>
       </c>
@@ -2362,7 +2374,7 @@
         <v>44187</v>
       </c>
     </row>
-    <row r="91" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="52">
         <v>2</v>
       </c>
@@ -2373,7 +2385,7 @@
         <v>44187</v>
       </c>
     </row>
-    <row r="92" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="52">
         <v>2</v>
       </c>
@@ -2384,7 +2396,7 @@
         <v>44187</v>
       </c>
     </row>
-    <row r="93" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="52">
         <v>2</v>
       </c>
@@ -2395,7 +2407,7 @@
         <v>44187</v>
       </c>
     </row>
-    <row r="94" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="52">
         <v>3</v>
       </c>
@@ -2406,7 +2418,7 @@
         <v>44187</v>
       </c>
     </row>
-    <row r="95" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="52">
         <v>3</v>
       </c>
@@ -2417,7 +2429,7 @@
         <v>44187</v>
       </c>
     </row>
-    <row r="96" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="52">
         <v>3</v>
       </c>
@@ -2428,7 +2440,7 @@
         <v>44187</v>
       </c>
     </row>
-    <row r="108" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" s="3">
         <v>2</v>
       </c>
@@ -2437,7 +2449,7 @@
       </c>
       <c r="G108" s="1"/>
     </row>
-    <row r="109" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" s="3">
         <v>2</v>
       </c>
@@ -2446,7 +2458,7 @@
       </c>
       <c r="G109" s="1"/>
     </row>
-    <row r="110" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A110" s="3">
         <v>2</v>
       </c>
@@ -2455,7 +2467,7 @@
       </c>
       <c r="G110" s="1"/>
     </row>
-    <row r="111" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A111" s="3">
         <v>2</v>
       </c>
@@ -2464,7 +2476,7 @@
       </c>
       <c r="G111" s="1"/>
     </row>
-    <row r="112" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" s="3">
         <v>2</v>
       </c>
@@ -2473,7 +2485,7 @@
       </c>
       <c r="G112" s="1"/>
     </row>
-    <row r="113" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113" s="3">
         <v>3</v>
       </c>
@@ -2482,7 +2494,7 @@
       </c>
       <c r="G113" s="1"/>
     </row>
-    <row r="114" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A114" s="3">
         <v>3</v>
       </c>
@@ -2491,7 +2503,7 @@
       </c>
       <c r="G114" s="1"/>
     </row>
-    <row r="115" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A115" s="3">
         <v>3</v>
       </c>
@@ -2500,7 +2512,7 @@
       </c>
       <c r="G115" s="1"/>
     </row>
-    <row r="116" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A116" s="3">
         <v>3</v>
       </c>
@@ -2509,7 +2521,7 @@
       </c>
       <c r="G116" s="1"/>
     </row>
-    <row r="117" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A117" s="3">
         <v>3</v>
       </c>
@@ -2518,7 +2530,7 @@
       </c>
       <c r="G117" s="1"/>
     </row>
-    <row r="118" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A118" s="3">
         <v>3</v>
       </c>
@@ -2527,7 +2539,7 @@
       </c>
       <c r="G118" s="1"/>
     </row>
-    <row r="119" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A119" s="3">
         <v>3</v>
       </c>
@@ -2536,7 +2548,7 @@
       </c>
       <c r="G119" s="1"/>
     </row>
-    <row r="120" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A120" s="3">
         <v>3</v>
       </c>
@@ -2545,7 +2557,7 @@
       </c>
       <c r="G120" s="1"/>
     </row>
-    <row r="121" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A121" s="3">
         <v>3</v>
       </c>
@@ -2554,7 +2566,7 @@
       </c>
       <c r="G121" s="1"/>
     </row>
-    <row r="122" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A122" s="3">
         <v>3</v>
       </c>
@@ -2563,7 +2575,7 @@
       </c>
       <c r="G122" s="1"/>
     </row>
-    <row r="123" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A123" s="3">
         <v>3</v>
       </c>
@@ -2572,7 +2584,7 @@
       </c>
       <c r="G123" s="1"/>
     </row>
-    <row r="124" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A124" s="3">
         <v>3</v>
       </c>
@@ -2581,7 +2593,7 @@
       </c>
       <c r="G124" s="1"/>
     </row>
-    <row r="125" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A125" s="3">
         <v>3</v>
       </c>
@@ -2590,7 +2602,7 @@
       </c>
       <c r="G125" s="1"/>
     </row>
-    <row r="126" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A126" s="3">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Tutorial de sesiones y cookies
</commit_message>
<xml_diff>
--- a/documentacion/Tareas.xlsx
+++ b/documentacion/Tareas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique/GitHubProjects/RecetApp/documentacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1A4646-50BC-5F4C-87CE-C4D68ACCA502}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150D1376-D376-7B4D-832B-65D51BB38F75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26680" windowHeight="17620" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
   </bookViews>
@@ -962,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66436974-768D-9A40-9A43-2F0986DDE03B}">
   <dimension ref="A1:G129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B67" zoomScale="116" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F91" sqref="F91"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="116" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2303,7 +2303,9 @@
       <c r="E84" s="31">
         <v>3</v>
       </c>
-      <c r="F84" s="31"/>
+      <c r="F84" s="31">
+        <v>1.5</v>
+      </c>
       <c r="G84" s="38"/>
     </row>
     <row r="85" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
actualizando tracking, quitando tarea de echo que al final no se va a hacer
</commit_message>
<xml_diff>
--- a/documentacion/Tareas.xlsx
+++ b/documentacion/Tareas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique/GitHubProjects/RecetApp/documentacion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/481f6a27916b9a84/Documentos/RecetApp/documentacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150D1376-D376-7B4D-832B-65D51BB38F75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="114_{946D7391-A773-4F77-9886-C4BE819E556F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{725B0B73-B719-4217-AA7A-8BC9EEE3265B}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="26680" windowHeight="17620" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="108">
   <si>
     <t>CREACIÓN DE UNA CUENTA</t>
   </si>
@@ -321,9 +321,6 @@
   </si>
   <si>
     <t>FECHA ENTREGA</t>
-  </si>
-  <si>
-    <t>Investigar funcionamiento de Echo (framework web de Go)</t>
   </si>
   <si>
     <t>Aprender a utilizar las herramientas de testing en Go (setup y teardown)</t>
@@ -960,25 +957,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66436974-768D-9A40-9A43-2F0986DDE03B}">
-  <dimension ref="A1:G129"/>
+  <dimension ref="A1:G128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="116" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F83" sqref="F83"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="116" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="25"/>
-    <col min="2" max="2" width="116.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="11"/>
-    <col min="4" max="4" width="36.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.69921875" style="25"/>
+    <col min="2" max="2" width="116.19921875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.796875" style="11"/>
+    <col min="4" max="4" width="36.19921875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.19921875" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="11"/>
+    <col min="7" max="7" width="15.19921875" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.796875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
@@ -1001,7 +998,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="45">
         <v>1</v>
       </c>
@@ -1018,7 +1015,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="12"/>
       <c r="B3" s="13" t="s">
         <v>1</v>
@@ -1034,7 +1031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="12"/>
       <c r="B4" s="13" t="s">
         <v>1</v>
@@ -1050,7 +1047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
       <c r="B5" s="13" t="s">
         <v>1</v>
@@ -1066,7 +1063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="12"/>
       <c r="B6" s="13" t="s">
         <v>1</v>
@@ -1082,7 +1079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="12"/>
       <c r="B7" s="13" t="s">
         <v>31</v>
@@ -1098,7 +1095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="12"/>
       <c r="B8" s="13" t="s">
         <v>31</v>
@@ -1114,7 +1111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
       <c r="B9" s="13" t="s">
         <v>31</v>
@@ -1130,7 +1127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="12"/>
       <c r="B10" s="13" t="s">
         <v>31</v>
@@ -1146,7 +1143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="12"/>
       <c r="B11" s="13" t="s">
         <v>31</v>
@@ -1162,7 +1159,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="12"/>
       <c r="B12" s="13" t="s">
         <v>2</v>
@@ -1178,7 +1175,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="12"/>
       <c r="B13" s="13" t="s">
         <v>29</v>
@@ -1194,7 +1191,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
       <c r="B14" s="13" t="s">
         <v>29</v>
@@ -1210,7 +1207,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="12"/>
       <c r="B15" s="17" t="s">
         <v>30</v>
@@ -1226,7 +1223,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="12"/>
       <c r="B16" s="13" t="s">
         <v>32</v>
@@ -1242,7 +1239,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="12"/>
       <c r="B17" s="13" t="s">
         <v>36</v>
@@ -1258,7 +1255,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="12"/>
       <c r="B18" s="13" t="s">
         <v>36</v>
@@ -1274,7 +1271,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="12"/>
       <c r="B19" s="18" t="s">
         <v>3</v>
@@ -1290,7 +1287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="45">
         <v>1</v>
       </c>
@@ -1305,7 +1302,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="19"/>
       <c r="B21" s="20" t="s">
         <v>52</v>
@@ -1318,7 +1315,7 @@
       <c r="F21" s="21"/>
       <c r="G21" s="23"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="12"/>
       <c r="B22" s="13" t="s">
         <v>40</v>
@@ -1332,7 +1329,7 @@
       </c>
       <c r="F22" s="15"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="12"/>
       <c r="B23" s="13" t="s">
         <v>39</v>
@@ -1346,7 +1343,7 @@
       </c>
       <c r="F23" s="15"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="12"/>
       <c r="B24" s="13" t="s">
         <v>57</v>
@@ -1360,7 +1357,7 @@
       </c>
       <c r="F24" s="15"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B25" s="26" t="s">
         <v>61</v>
       </c>
@@ -1371,7 +1368,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="45">
         <v>1</v>
       </c>
@@ -1388,7 +1385,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="12"/>
       <c r="B27" s="15" t="s">
         <v>5</v>
@@ -1404,7 +1401,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="12"/>
       <c r="B28" s="15" t="s">
         <v>5</v>
@@ -1420,7 +1417,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="12"/>
       <c r="B29" s="15" t="s">
         <v>6</v>
@@ -1436,7 +1433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="12"/>
       <c r="B30" s="15" t="s">
         <v>7</v>
@@ -1452,7 +1449,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="12"/>
       <c r="B31" s="15" t="s">
         <v>8</v>
@@ -1468,7 +1465,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="12"/>
       <c r="B32" s="28" t="s">
         <v>58</v>
@@ -1484,7 +1481,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="12"/>
       <c r="B33" s="18" t="s">
         <v>37</v>
@@ -1500,7 +1497,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="12"/>
       <c r="B34" s="18" t="s">
         <v>37</v>
@@ -1516,7 +1513,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="12"/>
       <c r="B35" s="26" t="s">
         <v>64</v>
@@ -1532,7 +1529,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="45">
         <v>1</v>
       </c>
@@ -1549,7 +1546,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="12"/>
       <c r="B37" s="15" t="s">
         <v>10</v>
@@ -1565,7 +1562,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="12"/>
       <c r="B38" s="15" t="s">
         <v>42</v>
@@ -1581,7 +1578,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="12"/>
       <c r="B39" s="15" t="s">
         <v>42</v>
@@ -1597,7 +1594,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="12"/>
       <c r="B40" s="15" t="s">
         <v>36</v>
@@ -1613,7 +1610,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="12"/>
       <c r="B41" s="15" t="s">
         <v>36</v>
@@ -1629,7 +1626,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="12"/>
       <c r="B42" s="15" t="s">
         <v>21</v>
@@ -1645,7 +1642,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="45">
         <v>1</v>
       </c>
@@ -1662,7 +1659,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="12"/>
       <c r="B44" s="15" t="s">
         <v>22</v>
@@ -1678,7 +1675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="12"/>
       <c r="B45" s="15" t="s">
         <v>23</v>
@@ -1694,10 +1691,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="12"/>
       <c r="B46" s="43" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C46" s="14"/>
       <c r="D46" s="15" t="s">
@@ -1710,7 +1707,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="45">
         <v>1</v>
       </c>
@@ -1727,7 +1724,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="12"/>
       <c r="B48" s="15" t="s">
         <v>12</v>
@@ -1743,7 +1740,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="12"/>
       <c r="B49" s="15" t="s">
         <v>43</v>
@@ -1759,7 +1756,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="12"/>
       <c r="B50" s="15" t="s">
         <v>36</v>
@@ -1775,7 +1772,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="12"/>
       <c r="B51" s="15" t="s">
         <v>36</v>
@@ -1791,7 +1788,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="12"/>
       <c r="B52" s="15" t="s">
         <v>36</v>
@@ -1807,7 +1804,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="12"/>
       <c r="B53" s="15" t="s">
         <v>11</v>
@@ -1823,7 +1820,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="54" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="19"/>
       <c r="B54" s="28" t="s">
         <v>53</v>
@@ -1840,7 +1837,7 @@
       </c>
       <c r="G54" s="23"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="12"/>
       <c r="B55" s="15" t="s">
         <v>38</v>
@@ -1856,7 +1853,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="56" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="45">
         <v>1</v>
       </c>
@@ -1871,7 +1868,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="57" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="19"/>
       <c r="B57" s="22" t="s">
         <v>66</v>
@@ -1888,7 +1885,7 @@
       </c>
       <c r="G57" s="23"/>
     </row>
-    <row r="58" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="19"/>
       <c r="B58" s="30" t="s">
         <v>67</v>
@@ -1905,7 +1902,7 @@
       </c>
       <c r="G58" s="23"/>
     </row>
-    <row r="59" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="19"/>
       <c r="B59" s="30" t="s">
         <v>67</v>
@@ -1922,7 +1919,7 @@
       </c>
       <c r="G59" s="23"/>
     </row>
-    <row r="60" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="19"/>
       <c r="B60" s="15" t="s">
         <v>14</v>
@@ -1939,7 +1936,7 @@
       </c>
       <c r="G60" s="23"/>
     </row>
-    <row r="61" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="19"/>
       <c r="B61" s="15" t="s">
         <v>14</v>
@@ -1956,7 +1953,7 @@
       </c>
       <c r="G61" s="23"/>
     </row>
-    <row r="62" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="19"/>
       <c r="B62" s="30" t="s">
         <v>65</v>
@@ -1969,7 +1966,7 @@
       <c r="F62" s="21"/>
       <c r="G62" s="23"/>
     </row>
-    <row r="63" spans="1:7" s="27" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" s="27" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A63" s="32"/>
       <c r="B63" s="26" t="s">
         <v>63</v>
@@ -1982,7 +1979,7 @@
       </c>
       <c r="G63" s="33"/>
     </row>
-    <row r="64" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="45">
         <v>1</v>
       </c>
@@ -1997,7 +1994,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="12"/>
       <c r="B65" s="15" t="s">
         <v>26</v>
@@ -2013,7 +2010,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="12"/>
       <c r="B66" s="15" t="s">
         <v>35</v>
@@ -2030,7 +2027,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="12"/>
       <c r="B67" s="15" t="s">
         <v>25</v>
@@ -2047,7 +2044,7 @@
         <v>5.25</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="12"/>
       <c r="B68" s="15" t="s">
         <v>25</v>
@@ -2063,7 +2060,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="12"/>
       <c r="B69" s="35" t="s">
         <v>68</v>
@@ -2079,7 +2076,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="12"/>
       <c r="B70" s="35" t="s">
         <v>69</v>
@@ -2093,7 +2090,7 @@
       </c>
       <c r="F70" s="15"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="12"/>
       <c r="B71" s="15" t="s">
         <v>51</v>
@@ -2109,7 +2106,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="12"/>
       <c r="B72" s="15" t="s">
         <v>50</v>
@@ -2125,7 +2122,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="12"/>
       <c r="B73" s="18" t="s">
         <v>46</v>
@@ -2139,7 +2136,7 @@
       </c>
       <c r="F73" s="15"/>
     </row>
-    <row r="74" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="45">
         <v>2</v>
       </c>
@@ -2154,10 +2151,10 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="75" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="19"/>
       <c r="B75" s="41" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C75" s="21"/>
       <c r="D75" s="41" t="s">
@@ -2171,7 +2168,7 @@
       </c>
       <c r="G75" s="23"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="12"/>
       <c r="B76" s="15" t="s">
         <v>48</v>
@@ -2187,7 +2184,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="12"/>
       <c r="B77" s="30" t="s">
         <v>49</v>
@@ -2203,7 +2200,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="78" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="45">
         <v>1</v>
       </c>
@@ -2218,7 +2215,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="12"/>
       <c r="B79" s="36" t="s">
         <v>59</v>
@@ -2230,7 +2227,7 @@
       <c r="E79" s="15"/>
       <c r="F79" s="15"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="12"/>
       <c r="B80" s="26" t="s">
         <v>60</v>
@@ -2244,7 +2241,7 @@
       </c>
       <c r="F80" s="15"/>
     </row>
-    <row r="81" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="45">
         <v>1</v>
       </c>
@@ -2259,420 +2256,405 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="82" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="37"/>
-      <c r="B82" s="40" t="s">
-        <v>96</v>
+      <c r="B82" s="42" t="s">
+        <v>104</v>
       </c>
       <c r="C82" s="31"/>
-      <c r="D82" s="40" t="s">
+      <c r="D82" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="E82" s="31">
+        <v>4</v>
+      </c>
+      <c r="F82" s="31">
+        <v>14</v>
+      </c>
+      <c r="G82" s="38"/>
+    </row>
+    <row r="83" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="37"/>
+      <c r="B83" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="C83" s="31"/>
+      <c r="D83" s="57" t="s">
+        <v>20</v>
+      </c>
+      <c r="E83" s="31">
+        <v>3</v>
+      </c>
+      <c r="F83" s="31">
+        <v>1.5</v>
+      </c>
+      <c r="G83" s="38"/>
+    </row>
+    <row r="84" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="37"/>
+      <c r="B84" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="C84" s="31"/>
+      <c r="D84" s="42" t="s">
         <v>27</v>
-      </c>
-      <c r="E82" s="31">
-        <v>10</v>
-      </c>
-      <c r="F82" s="31"/>
-      <c r="G82" s="38"/>
-    </row>
-    <row r="83" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="37"/>
-      <c r="B83" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="C83" s="31"/>
-      <c r="D83" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="E83" s="31">
-        <v>4</v>
-      </c>
-      <c r="F83" s="31">
-        <v>14</v>
-      </c>
-      <c r="G83" s="38"/>
-    </row>
-    <row r="84" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="37"/>
-      <c r="B84" s="57" t="s">
-        <v>108</v>
-      </c>
-      <c r="C84" s="31"/>
-      <c r="D84" s="57" t="s">
-        <v>20</v>
       </c>
       <c r="E84" s="31">
         <v>3</v>
       </c>
-      <c r="F84" s="31">
-        <v>1.5</v>
-      </c>
+      <c r="F84" s="31"/>
       <c r="G84" s="38"/>
     </row>
-    <row r="85" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="37"/>
       <c r="B85" s="42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C85" s="31"/>
-      <c r="D85" s="42" t="s">
-        <v>27</v>
+      <c r="D85" s="57" t="s">
+        <v>20</v>
       </c>
       <c r="E85" s="31">
-        <v>3</v>
-      </c>
-      <c r="F85" s="31"/>
+        <v>5</v>
+      </c>
+      <c r="F85" s="31">
+        <v>4</v>
+      </c>
       <c r="G85" s="38"/>
     </row>
-    <row r="86" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="37"/>
       <c r="B86" s="42" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C86" s="31"/>
       <c r="D86" s="57" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E86" s="31">
         <v>5</v>
       </c>
-      <c r="F86" s="31">
-        <v>4</v>
-      </c>
+      <c r="F86" s="31"/>
       <c r="G86" s="38"/>
     </row>
-    <row r="87" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="37"/>
-      <c r="B87" s="42" t="s">
-        <v>101</v>
+      <c r="B87" s="57" t="s">
+        <v>105</v>
       </c>
       <c r="C87" s="31"/>
       <c r="D87" s="57" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E87" s="31">
-        <v>5</v>
-      </c>
-      <c r="F87" s="31"/>
+        <v>3</v>
+      </c>
+      <c r="F87" s="31">
+        <v>2</v>
+      </c>
       <c r="G87" s="38"/>
     </row>
-    <row r="88" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="37"/>
-      <c r="B88" s="57" t="s">
+      <c r="B88" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="C88" s="31"/>
+      <c r="D88" s="40"/>
+      <c r="E88" s="31"/>
+      <c r="F88" s="31"/>
+      <c r="G88" s="38"/>
+    </row>
+    <row r="89" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="37"/>
+      <c r="B89" s="57" t="s">
         <v>106</v>
       </c>
-      <c r="C88" s="31"/>
-      <c r="D88" s="57" t="s">
-        <v>20</v>
-      </c>
-      <c r="E88" s="31">
-        <v>3</v>
-      </c>
-      <c r="F88" s="31">
+      <c r="C89" s="31"/>
+      <c r="D89" s="57" t="s">
+        <v>20</v>
+      </c>
+      <c r="E89" s="31">
+        <v>4</v>
+      </c>
+      <c r="F89" s="31">
+        <v>1.5</v>
+      </c>
+      <c r="G89" s="38"/>
+    </row>
+    <row r="90" spans="1:7" s="56" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="55">
         <v>2</v>
       </c>
-      <c r="G88" s="38"/>
-    </row>
-    <row r="89" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="37"/>
-      <c r="B89" s="44" t="s">
-        <v>100</v>
-      </c>
-      <c r="C89" s="31"/>
-      <c r="D89" s="40"/>
-      <c r="E89" s="31"/>
-      <c r="F89" s="31"/>
-      <c r="G89" s="38"/>
-    </row>
-    <row r="90" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="37"/>
-      <c r="B90" s="57" t="s">
-        <v>107</v>
-      </c>
-      <c r="C90" s="31"/>
-      <c r="D90" s="57" t="s">
-        <v>20</v>
-      </c>
-      <c r="E90" s="31">
-        <v>4</v>
-      </c>
-      <c r="F90" s="31">
-        <v>1.5</v>
-      </c>
-      <c r="G90" s="38"/>
-    </row>
-    <row r="91" spans="1:7" s="56" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="55">
+      <c r="B90" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="G90" s="48">
+        <v>44187</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="45">
         <v>2</v>
       </c>
       <c r="B91" s="53" t="s">
-        <v>103</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="C91" s="47"/>
+      <c r="D91" s="54"/>
+      <c r="E91" s="47"/>
+      <c r="F91" s="47"/>
       <c r="G91" s="48">
         <v>44187</v>
       </c>
     </row>
-    <row r="92" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="45">
+    <row r="92" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="52">
         <v>2</v>
       </c>
       <c r="B92" s="53" t="s">
-        <v>102</v>
-      </c>
-      <c r="C92" s="47"/>
-      <c r="D92" s="54"/>
-      <c r="E92" s="47"/>
-      <c r="F92" s="47"/>
+        <v>76</v>
+      </c>
       <c r="G92" s="48">
         <v>44187</v>
       </c>
     </row>
-    <row r="93" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="52">
         <v>2</v>
       </c>
       <c r="B93" s="53" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G93" s="48">
         <v>44187</v>
       </c>
     </row>
-    <row r="94" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="52">
         <v>2</v>
       </c>
       <c r="B94" s="53" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="G94" s="48">
         <v>44187</v>
       </c>
     </row>
-    <row r="95" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="52">
         <v>2</v>
       </c>
       <c r="B95" s="53" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="G95" s="48">
         <v>44187</v>
       </c>
     </row>
-    <row r="96" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="52">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B96" s="53" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="G96" s="48">
         <v>44187</v>
       </c>
     </row>
-    <row r="97" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="52">
         <v>3</v>
       </c>
       <c r="B97" s="53" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="G97" s="48">
         <v>44187</v>
       </c>
     </row>
-    <row r="98" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="52">
         <v>3</v>
       </c>
       <c r="B98" s="53" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="G98" s="48">
         <v>44187</v>
       </c>
     </row>
-    <row r="99" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="52">
-        <v>3</v>
-      </c>
-      <c r="B99" s="53" t="s">
-        <v>81</v>
-      </c>
-      <c r="G99" s="48">
-        <v>44187</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="3">
+        <v>2</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G110" s="1"/>
+    </row>
+    <row r="111" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A111" s="3">
         <v>2</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G111" s="1"/>
     </row>
-    <row r="112" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" s="3">
         <v>2</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G112" s="1"/>
     </row>
-    <row r="113" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113" s="3">
         <v>2</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G113" s="1"/>
     </row>
-    <row r="114" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A114" s="3">
         <v>2</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="G114" s="1"/>
     </row>
-    <row r="115" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A115" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G115" s="1"/>
     </row>
-    <row r="116" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A116" s="3">
         <v>3</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G116" s="1"/>
     </row>
-    <row r="117" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A117" s="3">
         <v>3</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G117" s="1"/>
     </row>
-    <row r="118" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A118" s="3">
         <v>3</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G118" s="1"/>
     </row>
-    <row r="119" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A119" s="3">
         <v>3</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G119" s="1"/>
     </row>
-    <row r="120" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A120" s="3">
         <v>3</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G120" s="1"/>
     </row>
-    <row r="121" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A121" s="3">
         <v>3</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G121" s="1"/>
     </row>
-    <row r="122" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A122" s="3">
         <v>3</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G122" s="1"/>
     </row>
-    <row r="123" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A123" s="3">
         <v>3</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G123" s="1"/>
     </row>
-    <row r="124" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A124" s="3">
         <v>3</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G124" s="1"/>
     </row>
-    <row r="125" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A125" s="3">
         <v>3</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G125" s="1"/>
     </row>
-    <row r="126" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A126" s="3">
         <v>3</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G126" s="1"/>
     </row>
-    <row r="127" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A127" s="3">
         <v>3</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G127" s="1"/>
     </row>
-    <row r="128" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A128" s="3">
         <v>3</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G128" s="1"/>
-    </row>
-    <row r="129" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="3">
-        <v>3</v>
-      </c>
-      <c r="B129" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G129" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Conseguido que se muestren todas las recetas existentes por pantalla, falta adaptar el html para que se pueda visualizar correctamente y descubierto un conflicto con htlmParser (no se puede redirigir dos veces a la misma clase
</commit_message>
<xml_diff>
--- a/documentacion/Tareas.xlsx
+++ b/documentacion/Tareas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Desktop\Universidad\4ºAño\ISO\RecetApp\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3507F87-821B-402C-A29D-1895DBB0CDDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6462EE-56F6-4241-8E00-5897EE452A57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
   </bookViews>
@@ -1008,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66436974-768D-9A40-9A43-2F0986DDE03B}">
   <dimension ref="A1:G136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="116" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D98" sqref="D98"/>
+    <sheetView tabSelected="1" topLeftCell="B86" zoomScale="116" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2028,7 +2028,9 @@
       <c r="E63" s="21">
         <v>0.5</v>
       </c>
-      <c r="F63" s="21"/>
+      <c r="F63" s="21">
+        <v>0.75</v>
+      </c>
       <c r="G63" s="23"/>
     </row>
     <row r="64" spans="1:7" s="27" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -2488,14 +2490,16 @@
       <c r="B93" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="C93" s="21"/>
+      <c r="C93" s="14"/>
       <c r="D93" s="63" t="s">
         <v>34</v>
       </c>
       <c r="E93" s="31">
         <v>0.1</v>
       </c>
-      <c r="F93" s="31"/>
+      <c r="F93" s="31">
+        <v>0.4</v>
+      </c>
       <c r="G93" s="38"/>
     </row>
     <row r="94" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solucionado el problema de htmlParser, ya se ven todas las recetas existentes por pantalla, solo falta mejorar el html para que se pueda ver todo bien
</commit_message>
<xml_diff>
--- a/documentacion/Tareas.xlsx
+++ b/documentacion/Tareas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Desktop\Universidad\4ºAño\ISO\RecetApp\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6462EE-56F6-4241-8E00-5897EE452A57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D508A9-3068-49B2-8D8F-E9C3CD49F845}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
   </bookViews>
@@ -1008,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66436974-768D-9A40-9A43-2F0986DDE03B}">
   <dimension ref="A1:G136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B86" zoomScale="116" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="116" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2021,7 +2021,7 @@
       <c r="B63" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="C63" s="31"/>
+      <c r="C63" s="14"/>
       <c r="D63" s="29" t="s">
         <v>34</v>
       </c>
@@ -2029,7 +2029,8 @@
         <v>0.5</v>
       </c>
       <c r="F63" s="21">
-        <v>0.75</v>
+        <f>0.75+0.75</f>
+        <v>1.5</v>
       </c>
       <c r="G63" s="23"/>
     </row>
@@ -2490,7 +2491,7 @@
       <c r="B93" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="C93" s="14"/>
+      <c r="C93" s="21"/>
       <c r="D93" s="63" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
Update de tareas, el html funciona, pero hay que adaptar el css para que se vean bien las recetas
</commit_message>
<xml_diff>
--- a/documentacion/Tareas.xlsx
+++ b/documentacion/Tareas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Desktop\Universidad\4ºAño\ISO\RecetApp\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D508A9-3068-49B2-8D8F-E9C3CD49F845}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7C427F-A21F-4B54-A7E1-09ACB2E46882}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="117">
   <si>
     <t>CREACIÓN DE UNA CUENTA</t>
   </si>
@@ -594,7 +594,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -659,7 +659,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1008,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66436974-768D-9A40-9A43-2F0986DDE03B}">
   <dimension ref="A1:G136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="116" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" topLeftCell="B67" zoomScale="116" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1047,20 +1046,20 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="44">
-        <v>1</v>
-      </c>
-      <c r="B2" s="45" t="s">
+    <row r="2" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="43">
+        <v>1</v>
+      </c>
+      <c r="B2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="47">
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="46">
         <v>44155</v>
       </c>
     </row>
@@ -1336,18 +1335,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="44">
-        <v>1</v>
-      </c>
-      <c r="B20" s="45" t="s">
+    <row r="20" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="43">
+        <v>1</v>
+      </c>
+      <c r="B20" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="47">
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="46">
         <v>44155</v>
       </c>
     </row>
@@ -1417,20 +1416,20 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="44">
-        <v>1</v>
-      </c>
-      <c r="B26" s="45" t="s">
+    <row r="26" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="43">
+        <v>1</v>
+      </c>
+      <c r="B26" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="49" t="s">
+      <c r="C26" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="47">
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="46">
         <v>44155</v>
       </c>
     </row>
@@ -1532,11 +1531,11 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="12"/>
-      <c r="B33" s="58" t="s">
+      <c r="B33" s="57" t="s">
         <v>108</v>
       </c>
       <c r="C33" s="21"/>
-      <c r="D33" s="57" t="s">
+      <c r="D33" s="56" t="s">
         <v>109</v>
       </c>
       <c r="E33" s="15"/>
@@ -1592,20 +1591,20 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="44">
-        <v>1</v>
-      </c>
-      <c r="B37" s="45" t="s">
+    <row r="37" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="43">
+        <v>1</v>
+      </c>
+      <c r="B37" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C37" s="46" t="s">
+      <c r="C37" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="D37" s="46"/>
-      <c r="E37" s="46"/>
-      <c r="F37" s="46"/>
-      <c r="G37" s="47">
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="46">
         <v>44155</v>
       </c>
     </row>
@@ -1705,20 +1704,20 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="44">
-        <v>1</v>
-      </c>
-      <c r="B44" s="45" t="s">
+    <row r="44" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="43">
+        <v>1</v>
+      </c>
+      <c r="B44" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="C44" s="46" t="s">
+      <c r="C44" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="D44" s="46"/>
-      <c r="E44" s="46"/>
-      <c r="F44" s="46"/>
-      <c r="G44" s="47">
+      <c r="D44" s="45"/>
+      <c r="E44" s="45"/>
+      <c r="F44" s="45"/>
+      <c r="G44" s="46">
         <v>44155</v>
       </c>
     </row>
@@ -1756,7 +1755,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="12"/>
-      <c r="B47" s="43" t="s">
+      <c r="B47" s="42" t="s">
         <v>97</v>
       </c>
       <c r="C47" s="14"/>
@@ -1770,20 +1769,20 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="44">
-        <v>1</v>
-      </c>
-      <c r="B48" s="45" t="s">
+    <row r="48" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="43">
+        <v>1</v>
+      </c>
+      <c r="B48" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="C48" s="50" t="s">
+      <c r="C48" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="D48" s="46"/>
-      <c r="E48" s="46"/>
-      <c r="F48" s="46"/>
-      <c r="G48" s="47">
+      <c r="D48" s="45"/>
+      <c r="E48" s="45"/>
+      <c r="F48" s="45"/>
+      <c r="G48" s="46">
         <v>44155</v>
       </c>
     </row>
@@ -1916,18 +1915,18 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="57" spans="1:7" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="44">
-        <v>1</v>
-      </c>
-      <c r="B57" s="45" t="s">
+    <row r="57" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="43">
+        <v>1</v>
+      </c>
+      <c r="B57" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="C57" s="46"/>
-      <c r="D57" s="46"/>
-      <c r="E57" s="46"/>
-      <c r="F57" s="46"/>
-      <c r="G57" s="47">
+      <c r="C57" s="45"/>
+      <c r="D57" s="45"/>
+      <c r="E57" s="45"/>
+      <c r="F57" s="45"/>
+      <c r="G57" s="46">
         <v>44155</v>
       </c>
     </row>
@@ -2047,18 +2046,18 @@
       </c>
       <c r="G64" s="33"/>
     </row>
-    <row r="65" spans="1:7" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="44">
-        <v>1</v>
-      </c>
-      <c r="B65" s="45" t="s">
+    <row r="65" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="43">
+        <v>1</v>
+      </c>
+      <c r="B65" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="C65" s="46"/>
-      <c r="D65" s="46"/>
-      <c r="E65" s="46"/>
-      <c r="F65" s="46"/>
-      <c r="G65" s="47">
+      <c r="C65" s="45"/>
+      <c r="D65" s="45"/>
+      <c r="E65" s="45"/>
+      <c r="F65" s="45"/>
+      <c r="G65" s="46">
         <v>44155</v>
       </c>
     </row>
@@ -2195,37 +2194,39 @@
       <c r="B74" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C74" s="15"/>
+      <c r="C74" s="14"/>
       <c r="D74" s="15" t="s">
         <v>34</v>
       </c>
       <c r="E74" s="15">
         <v>0.1</v>
       </c>
-      <c r="F74" s="15"/>
-    </row>
-    <row r="75" spans="1:7" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="44">
+      <c r="F74" s="15">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="43">
         <v>2</v>
       </c>
-      <c r="B75" s="45" t="s">
+      <c r="B75" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C75" s="46"/>
-      <c r="D75" s="46"/>
-      <c r="E75" s="46"/>
-      <c r="F75" s="46"/>
-      <c r="G75" s="47">
+      <c r="C75" s="45"/>
+      <c r="D75" s="45"/>
+      <c r="E75" s="45"/>
+      <c r="F75" s="45"/>
+      <c r="G75" s="46">
         <v>44155</v>
       </c>
     </row>
     <row r="76" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="19"/>
-      <c r="B76" s="41" t="s">
+      <c r="B76" s="40" t="s">
         <v>96</v>
       </c>
       <c r="C76" s="21"/>
-      <c r="D76" s="41" t="s">
+      <c r="D76" s="40" t="s">
         <v>20</v>
       </c>
       <c r="E76" s="21">
@@ -2268,18 +2269,18 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="79" spans="1:7" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="44">
-        <v>1</v>
-      </c>
-      <c r="B79" s="45" t="s">
+    <row r="79" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="43">
+        <v>1</v>
+      </c>
+      <c r="B79" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="C79" s="46"/>
-      <c r="D79" s="46"/>
-      <c r="E79" s="46"/>
-      <c r="F79" s="46"/>
-      <c r="G79" s="47">
+      <c r="C79" s="45"/>
+      <c r="D79" s="45"/>
+      <c r="E79" s="45"/>
+      <c r="F79" s="45"/>
+      <c r="G79" s="46">
         <v>44155</v>
       </c>
     </row>
@@ -2309,28 +2310,28 @@
       </c>
       <c r="F81" s="15"/>
     </row>
-    <row r="82" spans="1:7" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="44">
-        <v>1</v>
-      </c>
-      <c r="B82" s="45" t="s">
+    <row r="82" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="43">
+        <v>1</v>
+      </c>
+      <c r="B82" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="C82" s="46"/>
-      <c r="D82" s="46"/>
-      <c r="E82" s="46"/>
-      <c r="F82" s="46"/>
-      <c r="G82" s="47">
+      <c r="C82" s="45"/>
+      <c r="D82" s="45"/>
+      <c r="E82" s="45"/>
+      <c r="F82" s="45"/>
+      <c r="G82" s="46">
         <v>44155</v>
       </c>
     </row>
     <row r="83" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="37"/>
-      <c r="B83" s="42" t="s">
+      <c r="B83" s="41" t="s">
         <v>104</v>
       </c>
       <c r="C83" s="14"/>
-      <c r="D83" s="42" t="s">
+      <c r="D83" s="41" t="s">
         <v>20</v>
       </c>
       <c r="E83" s="31">
@@ -2343,11 +2344,11 @@
     </row>
     <row r="84" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="37"/>
-      <c r="B84" s="56" t="s">
+      <c r="B84" s="55" t="s">
         <v>107</v>
       </c>
       <c r="C84" s="14"/>
-      <c r="D84" s="56" t="s">
+      <c r="D84" s="55" t="s">
         <v>20</v>
       </c>
       <c r="E84" s="31">
@@ -2360,11 +2361,11 @@
     </row>
     <row r="85" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="37"/>
-      <c r="B85" s="42" t="s">
+      <c r="B85" s="41" t="s">
         <v>98</v>
       </c>
       <c r="C85" s="14"/>
-      <c r="D85" s="42" t="s">
+      <c r="D85" s="41" t="s">
         <v>27</v>
       </c>
       <c r="E85" s="31">
@@ -2375,11 +2376,11 @@
     </row>
     <row r="86" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="37"/>
-      <c r="B86" s="42" t="s">
+      <c r="B86" s="41" t="s">
         <v>98</v>
       </c>
       <c r="C86" s="14"/>
-      <c r="D86" s="56" t="s">
+      <c r="D86" s="55" t="s">
         <v>20</v>
       </c>
       <c r="E86" s="31">
@@ -2392,11 +2393,11 @@
     </row>
     <row r="87" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="37"/>
-      <c r="B87" s="42" t="s">
+      <c r="B87" s="41" t="s">
         <v>100</v>
       </c>
       <c r="C87" s="14"/>
-      <c r="D87" s="56" t="s">
+      <c r="D87" s="55" t="s">
         <v>27</v>
       </c>
       <c r="E87" s="31">
@@ -2409,11 +2410,11 @@
     </row>
     <row r="88" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="37"/>
-      <c r="B88" s="56" t="s">
+      <c r="B88" s="55" t="s">
         <v>105</v>
       </c>
       <c r="C88" s="14"/>
-      <c r="D88" s="56" t="s">
+      <c r="D88" s="55" t="s">
         <v>20</v>
       </c>
       <c r="E88" s="31">
@@ -2426,22 +2427,28 @@
     </row>
     <row r="89" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="37"/>
-      <c r="B89" s="59" t="s">
+      <c r="B89" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="C89" s="31"/>
-      <c r="D89" s="40"/>
-      <c r="E89" s="31"/>
-      <c r="F89" s="31"/>
+      <c r="C89" s="14"/>
+      <c r="D89" s="62" t="s">
+        <v>27</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0.2</v>
+      </c>
+      <c r="F89" s="31">
+        <v>0.5</v>
+      </c>
       <c r="G89" s="38"/>
     </row>
     <row r="90" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="37"/>
-      <c r="B90" s="59" t="s">
+      <c r="B90" s="58" t="s">
         <v>110</v>
       </c>
       <c r="C90" s="14"/>
-      <c r="D90" s="59" t="s">
+      <c r="D90" s="58" t="s">
         <v>20</v>
       </c>
       <c r="E90" s="31">
@@ -2454,11 +2461,11 @@
     </row>
     <row r="91" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="37"/>
-      <c r="B91" s="60" t="s">
+      <c r="B91" s="59" t="s">
         <v>111</v>
       </c>
       <c r="C91" s="14"/>
-      <c r="D91" s="60" t="s">
+      <c r="D91" s="59" t="s">
         <v>27</v>
       </c>
       <c r="E91" s="31">
@@ -2471,11 +2478,11 @@
     </row>
     <row r="92" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="37"/>
-      <c r="B92" s="56" t="s">
+      <c r="B92" s="55" t="s">
         <v>106</v>
       </c>
       <c r="C92" s="14"/>
-      <c r="D92" s="56" t="s">
+      <c r="D92" s="55" t="s">
         <v>20</v>
       </c>
       <c r="E92" s="31">
@@ -2488,28 +2495,29 @@
     </row>
     <row r="93" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="37"/>
-      <c r="B93" s="63" t="s">
+      <c r="B93" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="C93" s="21"/>
-      <c r="D93" s="63" t="s">
+      <c r="C93" s="14"/>
+      <c r="D93" s="62" t="s">
         <v>34</v>
       </c>
       <c r="E93" s="31">
         <v>0.1</v>
       </c>
       <c r="F93" s="31">
-        <v>0.4</v>
+        <f>0.4+0.2</f>
+        <v>0.60000000000000009</v>
       </c>
       <c r="G93" s="38"/>
     </row>
     <row r="94" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="37"/>
-      <c r="B94" s="63" t="s">
+      <c r="B94" s="62" t="s">
         <v>113</v>
       </c>
       <c r="C94" s="21"/>
-      <c r="D94" s="63" t="s">
+      <c r="D94" s="62" t="s">
         <v>34</v>
       </c>
       <c r="E94" s="31">
@@ -2518,145 +2526,145 @@
       <c r="F94" s="31"/>
       <c r="G94" s="38"/>
     </row>
-    <row r="95" spans="1:7" s="55" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="54">
+    <row r="95" spans="1:7" s="54" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="53">
         <v>2</v>
       </c>
-      <c r="B95" s="52" t="s">
+      <c r="B95" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="G95" s="47">
+      <c r="G95" s="46">
         <v>44187</v>
       </c>
     </row>
-    <row r="96" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="61"/>
-      <c r="B96" s="64" t="s">
+    <row r="96" spans="1:7" s="61" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="60"/>
+      <c r="B96" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="D96" s="64" t="s">
+      <c r="D96" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="E96" s="64">
+      <c r="E96" s="63">
         <v>0.5</v>
       </c>
       <c r="G96" s="23"/>
     </row>
-    <row r="97" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="61"/>
-      <c r="B97" s="64" t="s">
+    <row r="97" spans="1:7" s="61" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="60"/>
+      <c r="B97" s="63" t="s">
         <v>115</v>
       </c>
-      <c r="D97" s="64" t="s">
+      <c r="D97" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="E97" s="64">
+      <c r="E97" s="63">
         <v>0.5</v>
       </c>
       <c r="G97" s="23"/>
     </row>
-    <row r="98" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="61"/>
-      <c r="B98" s="64" t="s">
+    <row r="98" spans="1:7" s="61" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="60"/>
+      <c r="B98" s="63" t="s">
         <v>116</v>
       </c>
-      <c r="D98" s="64" t="s">
+      <c r="D98" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="E98" s="64">
+      <c r="E98" s="63">
         <v>0.1</v>
       </c>
       <c r="G98" s="23"/>
     </row>
-    <row r="99" spans="1:7" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="44">
+    <row r="99" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="43">
         <v>2</v>
       </c>
-      <c r="B99" s="52" t="s">
+      <c r="B99" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="C99" s="46"/>
-      <c r="D99" s="53"/>
-      <c r="E99" s="46"/>
-      <c r="F99" s="46"/>
-      <c r="G99" s="47">
+      <c r="C99" s="45"/>
+      <c r="D99" s="52"/>
+      <c r="E99" s="45"/>
+      <c r="F99" s="45"/>
+      <c r="G99" s="46">
         <v>44187</v>
       </c>
     </row>
-    <row r="100" spans="1:7" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="51">
+    <row r="100" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="50">
         <v>2</v>
       </c>
-      <c r="B100" s="52" t="s">
+      <c r="B100" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="G100" s="47">
+      <c r="G100" s="46">
         <v>44187</v>
       </c>
     </row>
-    <row r="101" spans="1:7" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="51">
+    <row r="101" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="50">
         <v>2</v>
       </c>
-      <c r="B101" s="52" t="s">
+      <c r="B101" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="G101" s="47">
+      <c r="G101" s="46">
         <v>44187</v>
       </c>
     </row>
-    <row r="102" spans="1:7" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="51">
+    <row r="102" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="50">
         <v>2</v>
       </c>
-      <c r="B102" s="52" t="s">
+      <c r="B102" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="G102" s="47">
+      <c r="G102" s="46">
         <v>44187</v>
       </c>
     </row>
-    <row r="103" spans="1:7" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="51">
+    <row r="103" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="50">
         <v>2</v>
       </c>
-      <c r="B103" s="52" t="s">
+      <c r="B103" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="G103" s="47">
+      <c r="G103" s="46">
         <v>44187</v>
       </c>
     </row>
-    <row r="104" spans="1:7" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="51">
+    <row r="104" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="50">
         <v>3</v>
       </c>
-      <c r="B104" s="52" t="s">
+      <c r="B104" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="G104" s="47">
+      <c r="G104" s="46">
         <v>44187</v>
       </c>
     </row>
-    <row r="105" spans="1:7" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="51">
+    <row r="105" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="50">
         <v>3</v>
       </c>
-      <c r="B105" s="52" t="s">
+      <c r="B105" s="51" t="s">
         <v>90</v>
       </c>
-      <c r="G105" s="47">
+      <c r="G105" s="46">
         <v>44187</v>
       </c>
     </row>
-    <row r="106" spans="1:7" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="51">
+    <row r="106" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="50">
         <v>3</v>
       </c>
-      <c r="B106" s="52" t="s">
+      <c r="B106" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="G106" s="47">
+      <c r="G106" s="46">
         <v>44187</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ya se muestran los ingredientes por pantalla
</commit_message>
<xml_diff>
--- a/documentacion/Tareas.xlsx
+++ b/documentacion/Tareas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Desktop\Universidad\4ºAño\ISO\RecetApp\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7C427F-A21F-4B54-A7E1-09ACB2E46882}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F8463F-0184-4905-B2FB-410ABBEDA31E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
   </bookViews>
@@ -390,9 +390,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -594,103 +601,106 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1007,8 +1017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66436974-768D-9A40-9A43-2F0986DDE03B}">
   <dimension ref="A1:G136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B67" zoomScale="116" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F75" sqref="F75"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="116" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1534,11 +1544,13 @@
       <c r="B33" s="57" t="s">
         <v>108</v>
       </c>
-      <c r="C33" s="21"/>
+      <c r="C33" s="14"/>
       <c r="D33" s="56" t="s">
         <v>109</v>
       </c>
-      <c r="E33" s="15"/>
+      <c r="E33" s="15">
+        <v>0.5</v>
+      </c>
       <c r="F33" s="15">
         <v>2</v>
       </c>
@@ -2038,10 +2050,14 @@
       <c r="B64" s="26" t="s">
         <v>63</v>
       </c>
+      <c r="C64" s="66"/>
       <c r="D64" s="27" t="s">
         <v>34</v>
       </c>
       <c r="E64" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="F64" s="27">
         <v>0.1</v>
       </c>
       <c r="G64" s="33"/>
@@ -2516,14 +2532,16 @@
       <c r="B94" s="62" t="s">
         <v>113</v>
       </c>
-      <c r="C94" s="21"/>
+      <c r="C94" s="14"/>
       <c r="D94" s="62" t="s">
         <v>34</v>
       </c>
       <c r="E94" s="31">
         <v>0.1</v>
       </c>
-      <c r="F94" s="31"/>
+      <c r="F94" s="31">
+        <v>0.5</v>
+      </c>
       <c r="G94" s="38"/>
     </row>
     <row r="95" spans="1:7" s="54" customFormat="1" x14ac:dyDescent="0.3">
@@ -2542,11 +2560,15 @@
       <c r="B96" s="63" t="s">
         <v>114</v>
       </c>
+      <c r="C96" s="65"/>
       <c r="D96" s="63" t="s">
         <v>34</v>
       </c>
       <c r="E96" s="63">
         <v>0.5</v>
+      </c>
+      <c r="F96" s="64">
+        <v>1.5</v>
       </c>
       <c r="G96" s="23"/>
     </row>
@@ -2555,11 +2577,15 @@
       <c r="B97" s="63" t="s">
         <v>115</v>
       </c>
+      <c r="C97" s="65"/>
       <c r="D97" s="63" t="s">
         <v>34</v>
       </c>
       <c r="E97" s="63">
         <v>0.5</v>
+      </c>
+      <c r="F97" s="64">
+        <v>1</v>
       </c>
       <c r="G97" s="23"/>
     </row>

</xml_diff>

<commit_message>
Eliminada clase de mis ingredientes y metido el código dentro de la clase Ingredientes, sigue funcionando que se puedan ver los ingredientes que tiene el usuario, y logout parece funcionar sin problemas
</commit_message>
<xml_diff>
--- a/documentacion/Tareas.xlsx
+++ b/documentacion/Tareas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Desktop\Universidad\4ºAño\ISO\RecetApp\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F8463F-0184-4905-B2FB-410ABBEDA31E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5076F01-8A50-4E85-A89B-EDF93FA9EA22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
   </bookViews>
@@ -1017,8 +1017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66436974-768D-9A40-9A43-2F0986DDE03B}">
   <dimension ref="A1:G136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="116" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F98" sqref="F98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2594,10 +2594,14 @@
       <c r="B98" s="63" t="s">
         <v>116</v>
       </c>
+      <c r="C98" s="65"/>
       <c r="D98" s="63" t="s">
         <v>34</v>
       </c>
       <c r="E98" s="63">
+        <v>0.1</v>
+      </c>
+      <c r="F98" s="64">
         <v>0.1</v>
       </c>
       <c r="G98" s="23"/>

</xml_diff>

<commit_message>
Añadido método para borrar ingredientes y update de las tareas
</commit_message>
<xml_diff>
--- a/documentacion/Tareas.xlsx
+++ b/documentacion/Tareas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique/GitHubProjects/RecetApp/documentacion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Desktop\Universidad\4ºAño\ISO\RecetApp\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DF3767-6FFB-B84B-99A4-6DB85E3749CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225D8A3B-13BB-4C9E-B5DD-3B24CEEB0AE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="26240" windowHeight="18220" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5D545327-A097-4A48-844A-5C1BE78BE98A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="117">
   <si>
     <t>CREACIÓN DE UNA CUENTA</t>
   </si>
@@ -179,12 +179,6 @@
     <t>BORRAR INGREDIENTES</t>
   </si>
   <si>
-    <t>Crear una opción en el menú para que el usuario borre ingredientes de su inventario</t>
-  </si>
-  <si>
-    <t>Crear la consulta sql para borrar un ingrediente introducido por el usuario</t>
-  </si>
-  <si>
     <t>Validar que las consultas salen por pantalla</t>
   </si>
   <si>
@@ -320,9 +314,6 @@
     <t>FECHA ENTREGA</t>
   </si>
   <si>
-    <t>Aprender a utilizar las herramientas de testing en Go (setup y teardown)</t>
-  </si>
-  <si>
     <t>Validar que un usuario que ha accedido a la aplicación puede añadir ingredientes a su inventario</t>
   </si>
   <si>
@@ -384,15 +375,31 @@
   </si>
   <si>
     <t>No permitir introducir el mismo ingrediente más de una vez a un usuario</t>
+  </si>
+  <si>
+    <t>Crear el código necesario para que se pueda borrar un ingrediente</t>
+  </si>
+  <si>
+    <t>Validar que se pueda borrar un ingrediente introducido por el usuario</t>
+  </si>
+  <si>
+    <t>Crear pantalla para borrar los ingredientes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -505,6 +512,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -601,106 +616,109 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="17" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1015,25 +1033,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66436974-768D-9A40-9A43-2F0986DDE03B}">
-  <dimension ref="A1:G136"/>
+  <dimension ref="A1:G137"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D92" sqref="D92"/>
+    <sheetView tabSelected="1" topLeftCell="D82" zoomScale="112" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G93" sqref="G93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="25"/>
-    <col min="2" max="2" width="116.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="11"/>
-    <col min="4" max="4" width="36.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.69921875" style="25"/>
+    <col min="2" max="2" width="116.19921875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.796875" style="11"/>
+    <col min="4" max="4" width="36.19921875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.19921875" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="11"/>
+    <col min="7" max="7" width="15.19921875" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.796875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
@@ -1053,27 +1071,27 @@
         <v>45</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42">
-        <v>1</v>
-      </c>
-      <c r="B2" s="43" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="41">
+        <v>1</v>
+      </c>
+      <c r="B2" s="42" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="45">
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="44">
         <v>44155</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="12"/>
       <c r="B3" s="13" t="s">
         <v>1</v>
@@ -1089,7 +1107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="12"/>
       <c r="B4" s="13" t="s">
         <v>1</v>
@@ -1105,7 +1123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
       <c r="B5" s="13" t="s">
         <v>1</v>
@@ -1121,7 +1139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="12"/>
       <c r="B6" s="13" t="s">
         <v>1</v>
@@ -1137,7 +1155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="12"/>
       <c r="B7" s="13" t="s">
         <v>31</v>
@@ -1153,7 +1171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="12"/>
       <c r="B8" s="13" t="s">
         <v>31</v>
@@ -1169,7 +1187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
       <c r="B9" s="13" t="s">
         <v>31</v>
@@ -1185,7 +1203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="12"/>
       <c r="B10" s="13" t="s">
         <v>31</v>
@@ -1201,7 +1219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="12"/>
       <c r="B11" s="13" t="s">
         <v>31</v>
@@ -1217,7 +1235,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="12"/>
       <c r="B12" s="13" t="s">
         <v>2</v>
@@ -1233,7 +1251,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="12"/>
       <c r="B13" s="13" t="s">
         <v>29</v>
@@ -1249,7 +1267,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
       <c r="B14" s="13" t="s">
         <v>29</v>
@@ -1265,7 +1283,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="12"/>
       <c r="B15" s="17" t="s">
         <v>30</v>
@@ -1281,7 +1299,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="12"/>
       <c r="B16" s="13" t="s">
         <v>32</v>
@@ -1297,7 +1315,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="12"/>
       <c r="B17" s="13" t="s">
         <v>36</v>
@@ -1313,7 +1331,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="12"/>
       <c r="B18" s="13" t="s">
         <v>36</v>
@@ -1329,7 +1347,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="12"/>
       <c r="B19" s="18" t="s">
         <v>3</v>
@@ -1345,25 +1363,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="42">
-        <v>1</v>
-      </c>
-      <c r="B20" s="43" t="s">
+    <row r="20" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="41">
+        <v>1</v>
+      </c>
+      <c r="B20" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="44"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="45">
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="44">
         <v>44155</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="19"/>
       <c r="B21" s="20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C21" s="21"/>
       <c r="D21" s="22" t="s">
@@ -1373,7 +1391,7 @@
       <c r="F21" s="21"/>
       <c r="G21" s="23"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="12"/>
       <c r="B22" s="13" t="s">
         <v>40</v>
@@ -1387,7 +1405,7 @@
       </c>
       <c r="F22" s="15"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="12"/>
       <c r="B23" s="13" t="s">
         <v>39</v>
@@ -1401,10 +1419,10 @@
       </c>
       <c r="F23" s="15"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="12"/>
       <c r="B24" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C24" s="21"/>
       <c r="D24" s="15" t="s">
@@ -1415,9 +1433,9 @@
       </c>
       <c r="F24" s="15"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B25" s="26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D25" s="27" t="s">
         <v>34</v>
@@ -1426,24 +1444,24 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="42">
-        <v>1</v>
-      </c>
-      <c r="B26" s="43" t="s">
+    <row r="26" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="41">
+        <v>1</v>
+      </c>
+      <c r="B26" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="63" t="s">
+      <c r="C26" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="44"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="44"/>
-      <c r="G26" s="45">
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="44">
         <v>44155</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="12"/>
       <c r="B27" s="15" t="s">
         <v>5</v>
@@ -1459,7 +1477,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="12"/>
       <c r="B28" s="15" t="s">
         <v>5</v>
@@ -1475,7 +1493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="12"/>
       <c r="B29" s="15" t="s">
         <v>6</v>
@@ -1491,7 +1509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="12"/>
       <c r="B30" s="15" t="s">
         <v>7</v>
@@ -1507,7 +1525,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="12"/>
       <c r="B31" s="15" t="s">
         <v>8</v>
@@ -1523,10 +1541,10 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="12"/>
       <c r="B32" s="28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C32" s="14"/>
       <c r="D32" s="27" t="s">
@@ -1539,14 +1557,14 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="12"/>
-      <c r="B33" s="54" t="s">
-        <v>107</v>
+      <c r="B33" s="53" t="s">
+        <v>104</v>
       </c>
       <c r="C33" s="14"/>
-      <c r="D33" s="53" t="s">
-        <v>108</v>
+      <c r="D33" s="52" t="s">
+        <v>105</v>
       </c>
       <c r="E33" s="15">
         <v>0.5</v>
@@ -1555,7 +1573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="12"/>
       <c r="B34" s="18" t="s">
         <v>37</v>
@@ -1571,7 +1589,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="12"/>
       <c r="B35" s="18" t="s">
         <v>37</v>
@@ -1587,10 +1605,10 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="12"/>
       <c r="B36" s="26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C36" s="14"/>
       <c r="D36" s="27" t="s">
@@ -1603,24 +1621,24 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="42">
-        <v>1</v>
-      </c>
-      <c r="B37" s="43" t="s">
+    <row r="37" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="41">
+        <v>1</v>
+      </c>
+      <c r="B37" s="42" t="s">
         <v>9</v>
       </c>
       <c r="C37" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D37" s="44"/>
-      <c r="E37" s="44"/>
-      <c r="F37" s="44"/>
-      <c r="G37" s="45">
+      <c r="D37" s="43"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="43"/>
+      <c r="G37" s="44">
         <v>44155</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="12"/>
       <c r="B38" s="15" t="s">
         <v>10</v>
@@ -1636,7 +1654,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="12"/>
       <c r="B39" s="15" t="s">
         <v>42</v>
@@ -1652,7 +1670,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="12"/>
       <c r="B40" s="15" t="s">
         <v>42</v>
@@ -1668,7 +1686,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="12"/>
       <c r="B41" s="15" t="s">
         <v>36</v>
@@ -1684,7 +1702,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="12"/>
       <c r="B42" s="15" t="s">
         <v>36</v>
@@ -1700,7 +1718,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="12"/>
       <c r="B43" s="15" t="s">
         <v>21</v>
@@ -1716,24 +1734,24 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="42">
-        <v>1</v>
-      </c>
-      <c r="B44" s="43" t="s">
-        <v>61</v>
+    <row r="44" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="41">
+        <v>1</v>
+      </c>
+      <c r="B44" s="42" t="s">
+        <v>59</v>
       </c>
       <c r="C44" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D44" s="44"/>
-      <c r="E44" s="44"/>
-      <c r="F44" s="44"/>
-      <c r="G44" s="45">
+      <c r="D44" s="43"/>
+      <c r="E44" s="43"/>
+      <c r="F44" s="43"/>
+      <c r="G44" s="44">
         <v>44155</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="12"/>
       <c r="B45" s="15" t="s">
         <v>22</v>
@@ -1749,7 +1767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="12"/>
       <c r="B46" s="15" t="s">
         <v>23</v>
@@ -1765,10 +1783,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="12"/>
-      <c r="B47" s="41" t="s">
-        <v>96</v>
+      <c r="B47" s="40" t="s">
+        <v>93</v>
       </c>
       <c r="C47" s="14"/>
       <c r="D47" s="15" t="s">
@@ -1781,24 +1799,24 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="42">
-        <v>1</v>
-      </c>
-      <c r="B48" s="43" t="s">
+    <row r="48" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="41">
+        <v>1</v>
+      </c>
+      <c r="B48" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="C48" s="66" t="s">
+      <c r="C48" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="D48" s="44"/>
-      <c r="E48" s="44"/>
-      <c r="F48" s="44"/>
-      <c r="G48" s="45">
+      <c r="D48" s="43"/>
+      <c r="E48" s="43"/>
+      <c r="F48" s="43"/>
+      <c r="G48" s="44">
         <v>44155</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="12"/>
       <c r="B49" s="15" t="s">
         <v>12</v>
@@ -1814,7 +1832,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="12"/>
       <c r="B50" s="15" t="s">
         <v>43</v>
@@ -1830,7 +1848,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="12"/>
       <c r="B51" s="15" t="s">
         <v>36</v>
@@ -1846,7 +1864,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="12"/>
       <c r="B52" s="15" t="s">
         <v>36</v>
@@ -1862,7 +1880,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="12"/>
       <c r="B53" s="15" t="s">
         <v>36</v>
@@ -1878,7 +1896,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="12"/>
       <c r="B54" s="15" t="s">
         <v>11</v>
@@ -1894,10 +1912,10 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="55" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="19"/>
       <c r="B55" s="28" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C55" s="14"/>
       <c r="D55" s="21" t="s">
@@ -1911,7 +1929,7 @@
       </c>
       <c r="G55" s="23"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="12"/>
       <c r="B56" s="15" t="s">
         <v>38</v>
@@ -1927,27 +1945,27 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="57" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="42">
-        <v>1</v>
-      </c>
-      <c r="B57" s="43" t="s">
-        <v>54</v>
+    <row r="57" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="41">
+        <v>1</v>
+      </c>
+      <c r="B57" s="42" t="s">
+        <v>52</v>
       </c>
       <c r="C57" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D57" s="44"/>
-      <c r="E57" s="44"/>
-      <c r="F57" s="44"/>
-      <c r="G57" s="45">
+      <c r="D57" s="43"/>
+      <c r="E57" s="43"/>
+      <c r="F57" s="43"/>
+      <c r="G57" s="44">
         <v>44155</v>
       </c>
     </row>
-    <row r="58" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="19"/>
       <c r="B58" s="22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C58" s="14"/>
       <c r="D58" s="21" t="s">
@@ -1961,10 +1979,10 @@
       </c>
       <c r="G58" s="23"/>
     </row>
-    <row r="59" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="19"/>
       <c r="B59" s="30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C59" s="14"/>
       <c r="D59" s="22" t="s">
@@ -1978,10 +1996,10 @@
       </c>
       <c r="G59" s="23"/>
     </row>
-    <row r="60" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="19"/>
       <c r="B60" s="30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C60" s="14"/>
       <c r="D60" s="22" t="s">
@@ -1995,7 +2013,7 @@
       </c>
       <c r="G60" s="23"/>
     </row>
-    <row r="61" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="19"/>
       <c r="B61" s="15" t="s">
         <v>14</v>
@@ -2012,7 +2030,7 @@
       </c>
       <c r="G61" s="23"/>
     </row>
-    <row r="62" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="19"/>
       <c r="B62" s="15" t="s">
         <v>14</v>
@@ -2029,10 +2047,10 @@
       </c>
       <c r="G62" s="23"/>
     </row>
-    <row r="63" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="19"/>
       <c r="B63" s="30" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C63" s="14"/>
       <c r="D63" s="29" t="s">
@@ -2047,12 +2065,12 @@
       </c>
       <c r="G63" s="23"/>
     </row>
-    <row r="64" spans="1:7" s="27" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" s="27" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A64" s="32"/>
       <c r="B64" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="C64" s="63"/>
+        <v>60</v>
+      </c>
+      <c r="C64" s="62"/>
       <c r="D64" s="27" t="s">
         <v>34</v>
       </c>
@@ -2064,24 +2082,24 @@
       </c>
       <c r="G64" s="33"/>
     </row>
-    <row r="65" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="42">
-        <v>1</v>
-      </c>
-      <c r="B65" s="43" t="s">
+    <row r="65" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="41">
+        <v>1</v>
+      </c>
+      <c r="B65" s="42" t="s">
         <v>24</v>
       </c>
       <c r="C65" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D65" s="44"/>
-      <c r="E65" s="44"/>
-      <c r="F65" s="44"/>
-      <c r="G65" s="45">
+      <c r="D65" s="43"/>
+      <c r="E65" s="43"/>
+      <c r="F65" s="43"/>
+      <c r="G65" s="44">
         <v>44155</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="12"/>
       <c r="B66" s="15" t="s">
         <v>26</v>
@@ -2097,7 +2115,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="12"/>
       <c r="B67" s="15" t="s">
         <v>35</v>
@@ -2114,7 +2132,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="12"/>
       <c r="B68" s="15" t="s">
         <v>25</v>
@@ -2131,7 +2149,7 @@
         <v>5.25</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="12"/>
       <c r="B69" s="15" t="s">
         <v>25</v>
@@ -2147,10 +2165,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="12"/>
       <c r="B70" s="35" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C70" s="14"/>
       <c r="D70" s="15" t="s">
@@ -2163,10 +2181,10 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="12"/>
       <c r="B71" s="35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C71" s="14"/>
       <c r="D71" s="15" t="s">
@@ -2177,10 +2195,10 @@
       </c>
       <c r="F71" s="15"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="12"/>
       <c r="B72" s="15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C72" s="14"/>
       <c r="D72" s="15" t="s">
@@ -2193,10 +2211,10 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="12"/>
       <c r="B73" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C73" s="14"/>
       <c r="D73" s="15" t="s">
@@ -2209,7 +2227,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="12"/>
       <c r="B74" s="18" t="s">
         <v>46</v>
@@ -2225,44 +2243,45 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="75" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="42">
+    <row r="75" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="41">
         <v>2</v>
       </c>
-      <c r="B75" s="43" t="s">
+      <c r="B75" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="C75" s="44"/>
-      <c r="D75" s="44"/>
-      <c r="E75" s="44"/>
-      <c r="F75" s="44"/>
-      <c r="G75" s="45">
+      <c r="C75" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="D75" s="43"/>
+      <c r="E75" s="43"/>
+      <c r="F75" s="43"/>
+      <c r="G75" s="44">
         <v>44155</v>
       </c>
     </row>
-    <row r="76" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="19"/>
-      <c r="B76" s="39" t="s">
-        <v>95</v>
-      </c>
-      <c r="C76" s="21"/>
-      <c r="D76" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="E76" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="F76" s="21">
-        <v>2</v>
-      </c>
-      <c r="G76" s="23"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A76" s="12"/>
+      <c r="B76" s="66" t="s">
+        <v>114</v>
+      </c>
+      <c r="C76" s="14"/>
+      <c r="D76" s="66" t="s">
+        <v>34</v>
+      </c>
+      <c r="E76" s="15">
+        <v>1</v>
+      </c>
+      <c r="F76" s="15">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="12"/>
-      <c r="B77" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C77" s="15"/>
+      <c r="B77" s="66" t="s">
+        <v>114</v>
+      </c>
+      <c r="C77" s="14"/>
       <c r="D77" s="15" t="s">
         <v>20</v>
       </c>
@@ -2273,14 +2292,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="12"/>
-      <c r="B78" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="C78" s="15"/>
-      <c r="D78" s="15" t="s">
-        <v>20</v>
+      <c r="B78" s="66" t="s">
+        <v>115</v>
+      </c>
+      <c r="C78" s="14"/>
+      <c r="D78" s="66" t="s">
+        <v>34</v>
       </c>
       <c r="E78" s="15">
         <v>0.1</v>
@@ -2289,28 +2308,30 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="79" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="42">
-        <v>1</v>
-      </c>
-      <c r="B79" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="C79" s="44"/>
-      <c r="D79" s="44"/>
-      <c r="E79" s="44"/>
-      <c r="F79" s="44"/>
-      <c r="G79" s="45">
+    <row r="79" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="41">
+        <v>1</v>
+      </c>
+      <c r="B79" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="C79" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="D79" s="43"/>
+      <c r="E79" s="43"/>
+      <c r="F79" s="43"/>
+      <c r="G79" s="44">
         <v>44155</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="12"/>
-      <c r="B80" s="64" t="s">
-        <v>116</v>
+      <c r="B80" s="63" t="s">
+        <v>113</v>
       </c>
       <c r="C80" s="14"/>
-      <c r="D80" s="65" t="s">
+      <c r="D80" s="64" t="s">
         <v>20</v>
       </c>
       <c r="E80" s="15">
@@ -2320,12 +2341,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="12"/>
       <c r="B81" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="C81" s="15"/>
+        <v>57</v>
+      </c>
+      <c r="C81" s="14"/>
       <c r="D81" s="27" t="s">
         <v>34</v>
       </c>
@@ -2334,30 +2355,30 @@
       </c>
       <c r="F81" s="15"/>
     </row>
-    <row r="82" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="42">
-        <v>1</v>
-      </c>
-      <c r="B82" s="43" t="s">
-        <v>55</v>
+    <row r="82" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="41">
+        <v>1</v>
+      </c>
+      <c r="B82" s="42" t="s">
+        <v>53</v>
       </c>
       <c r="C82" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D82" s="44"/>
-      <c r="E82" s="44"/>
-      <c r="F82" s="44"/>
-      <c r="G82" s="45">
+      <c r="D82" s="43"/>
+      <c r="E82" s="43"/>
+      <c r="F82" s="43"/>
+      <c r="G82" s="44">
         <v>44155</v>
       </c>
     </row>
-    <row r="83" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="36"/>
-      <c r="B83" s="40" t="s">
-        <v>103</v>
+      <c r="B83" s="39" t="s">
+        <v>100</v>
       </c>
       <c r="C83" s="14"/>
-      <c r="D83" s="40" t="s">
+      <c r="D83" s="39" t="s">
         <v>20</v>
       </c>
       <c r="E83" s="31">
@@ -2368,13 +2389,13 @@
       </c>
       <c r="G83" s="37"/>
     </row>
-    <row r="84" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="36"/>
-      <c r="B84" s="52" t="s">
-        <v>106</v>
+      <c r="B84" s="51" t="s">
+        <v>103</v>
       </c>
       <c r="C84" s="14"/>
-      <c r="D84" s="52" t="s">
+      <c r="D84" s="51" t="s">
         <v>20</v>
       </c>
       <c r="E84" s="31">
@@ -2385,13 +2406,13 @@
       </c>
       <c r="G84" s="37"/>
     </row>
-    <row r="85" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="36"/>
-      <c r="B85" s="40" t="s">
-        <v>97</v>
+      <c r="B85" s="39" t="s">
+        <v>94</v>
       </c>
       <c r="C85" s="14"/>
-      <c r="D85" s="40" t="s">
+      <c r="D85" s="39" t="s">
         <v>27</v>
       </c>
       <c r="E85" s="31">
@@ -2400,13 +2421,13 @@
       <c r="F85" s="31"/>
       <c r="G85" s="37"/>
     </row>
-    <row r="86" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="36"/>
-      <c r="B86" s="40" t="s">
-        <v>97</v>
+      <c r="B86" s="39" t="s">
+        <v>94</v>
       </c>
       <c r="C86" s="14"/>
-      <c r="D86" s="52" t="s">
+      <c r="D86" s="51" t="s">
         <v>20</v>
       </c>
       <c r="E86" s="31">
@@ -2417,13 +2438,13 @@
       </c>
       <c r="G86" s="37"/>
     </row>
-    <row r="87" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="36"/>
-      <c r="B87" s="40" t="s">
-        <v>99</v>
+      <c r="B87" s="39" t="s">
+        <v>96</v>
       </c>
       <c r="C87" s="14"/>
-      <c r="D87" s="52" t="s">
+      <c r="D87" s="51" t="s">
         <v>27</v>
       </c>
       <c r="E87" s="31">
@@ -2434,13 +2455,13 @@
       </c>
       <c r="G87" s="37"/>
     </row>
-    <row r="88" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="36"/>
-      <c r="B88" s="52" t="s">
-        <v>104</v>
+      <c r="B88" s="51" t="s">
+        <v>101</v>
       </c>
       <c r="C88" s="14"/>
-      <c r="D88" s="52" t="s">
+      <c r="D88" s="51" t="s">
         <v>20</v>
       </c>
       <c r="E88" s="31">
@@ -2451,13 +2472,13 @@
       </c>
       <c r="G88" s="37"/>
     </row>
-    <row r="89" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="36"/>
-      <c r="B89" s="55" t="s">
-        <v>98</v>
+      <c r="B89" s="54" t="s">
+        <v>95</v>
       </c>
       <c r="C89" s="14"/>
-      <c r="D89" s="59" t="s">
+      <c r="D89" s="58" t="s">
         <v>27</v>
       </c>
       <c r="E89" s="31">
@@ -2468,13 +2489,13 @@
       </c>
       <c r="G89" s="37"/>
     </row>
-    <row r="90" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="36"/>
-      <c r="B90" s="55" t="s">
-        <v>109</v>
+      <c r="B90" s="54" t="s">
+        <v>106</v>
       </c>
       <c r="C90" s="14"/>
-      <c r="D90" s="55" t="s">
+      <c r="D90" s="54" t="s">
         <v>20</v>
       </c>
       <c r="E90" s="31">
@@ -2485,13 +2506,13 @@
       </c>
       <c r="G90" s="37"/>
     </row>
-    <row r="91" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="36"/>
-      <c r="B91" s="56" t="s">
-        <v>110</v>
+      <c r="B91" s="55" t="s">
+        <v>107</v>
       </c>
       <c r="C91" s="14"/>
-      <c r="D91" s="56" t="s">
+      <c r="D91" s="55" t="s">
         <v>27</v>
       </c>
       <c r="E91" s="31">
@@ -2502,13 +2523,13 @@
       </c>
       <c r="G91" s="37"/>
     </row>
-    <row r="92" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="36"/>
-      <c r="B92" s="52" t="s">
-        <v>105</v>
+      <c r="B92" s="51" t="s">
+        <v>102</v>
       </c>
       <c r="C92" s="14"/>
-      <c r="D92" s="52" t="s">
+      <c r="D92" s="51" t="s">
         <v>20</v>
       </c>
       <c r="E92" s="31">
@@ -2519,13 +2540,13 @@
       </c>
       <c r="G92" s="37"/>
     </row>
-    <row r="93" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="36"/>
-      <c r="B93" s="59" t="s">
-        <v>111</v>
+      <c r="B93" s="58" t="s">
+        <v>108</v>
       </c>
       <c r="C93" s="14"/>
-      <c r="D93" s="59" t="s">
+      <c r="D93" s="58" t="s">
         <v>34</v>
       </c>
       <c r="E93" s="31">
@@ -2535,352 +2556,369 @@
         <f>0.4+0.2</f>
         <v>0.60000000000000009</v>
       </c>
-      <c r="G93" s="37"/>
-    </row>
-    <row r="94" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G93" s="69"/>
+    </row>
+    <row r="94" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="36"/>
-      <c r="B94" s="59" t="s">
+      <c r="B94" s="58" t="s">
+        <v>109</v>
+      </c>
+      <c r="C94" s="14"/>
+      <c r="D94" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="E94" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="F94" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="G94" s="37"/>
+    </row>
+    <row r="95" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="36"/>
+      <c r="B95" s="68" t="s">
+        <v>116</v>
+      </c>
+      <c r="C95" s="14"/>
+      <c r="D95" s="68" t="s">
+        <v>34</v>
+      </c>
+      <c r="E95" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="F95" s="31">
+        <v>0.2</v>
+      </c>
+      <c r="G95" s="37"/>
+    </row>
+    <row r="96" spans="1:7" s="50" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="49">
+        <v>2</v>
+      </c>
+      <c r="B96" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="C96" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G96" s="44">
+        <v>44187</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="56"/>
+      <c r="B97" s="59" t="s">
+        <v>110</v>
+      </c>
+      <c r="C97" s="61"/>
+      <c r="D97" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="E97" s="59">
+        <v>0.5</v>
+      </c>
+      <c r="F97" s="60">
+        <v>1.5</v>
+      </c>
+      <c r="G97" s="23"/>
+    </row>
+    <row r="98" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="56"/>
+      <c r="B98" s="59" t="s">
+        <v>111</v>
+      </c>
+      <c r="C98" s="61"/>
+      <c r="D98" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="E98" s="59">
+        <v>0.5</v>
+      </c>
+      <c r="F98" s="60">
+        <v>1</v>
+      </c>
+      <c r="G98" s="23"/>
+    </row>
+    <row r="99" spans="1:7" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="56"/>
+      <c r="B99" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="C94" s="14"/>
-      <c r="D94" s="59" t="s">
+      <c r="C99" s="61"/>
+      <c r="D99" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="E94" s="31">
-        <v>0.1</v>
-      </c>
-      <c r="F94" s="31">
-        <v>0.5</v>
-      </c>
-      <c r="G94" s="37"/>
-    </row>
-    <row r="95" spans="1:7" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="50">
+      <c r="E99" s="59">
+        <v>0.1</v>
+      </c>
+      <c r="F99" s="60">
+        <v>0.1</v>
+      </c>
+      <c r="G99" s="23"/>
+    </row>
+    <row r="100" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="41">
         <v>2</v>
       </c>
-      <c r="B95" s="48" t="s">
-        <v>101</v>
-      </c>
-      <c r="C95" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G95" s="45">
+      <c r="B100" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="C100" s="43"/>
+      <c r="D100" s="48"/>
+      <c r="E100" s="43"/>
+      <c r="F100" s="43"/>
+      <c r="G100" s="44">
         <v>44187</v>
       </c>
     </row>
-    <row r="96" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="57"/>
-      <c r="B96" s="60" t="s">
-        <v>113</v>
-      </c>
-      <c r="C96" s="62"/>
-      <c r="D96" s="60" t="s">
-        <v>34</v>
-      </c>
-      <c r="E96" s="60">
-        <v>0.5</v>
-      </c>
-      <c r="F96" s="61">
-        <v>1.5</v>
-      </c>
-      <c r="G96" s="23"/>
-    </row>
-    <row r="97" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="57"/>
-      <c r="B97" s="60" t="s">
-        <v>114</v>
-      </c>
-      <c r="C97" s="62"/>
-      <c r="D97" s="60" t="s">
-        <v>34</v>
-      </c>
-      <c r="E97" s="60">
-        <v>0.5</v>
-      </c>
-      <c r="F97" s="61">
-        <v>1</v>
-      </c>
-      <c r="G97" s="23"/>
-    </row>
-    <row r="98" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="57"/>
-      <c r="B98" s="60" t="s">
-        <v>115</v>
-      </c>
-      <c r="C98" s="62"/>
-      <c r="D98" s="60" t="s">
-        <v>34</v>
-      </c>
-      <c r="E98" s="60">
-        <v>0.1</v>
-      </c>
-      <c r="F98" s="61">
-        <v>0.1</v>
-      </c>
-      <c r="G98" s="23"/>
-    </row>
-    <row r="99" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="42">
+    <row r="101" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="46">
         <v>2</v>
       </c>
-      <c r="B99" s="48" t="s">
-        <v>100</v>
-      </c>
-      <c r="C99" s="44"/>
-      <c r="D99" s="49"/>
-      <c r="E99" s="44"/>
-      <c r="F99" s="44"/>
-      <c r="G99" s="45">
+      <c r="B101" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="G101" s="44">
         <v>44187</v>
       </c>
     </row>
-    <row r="100" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="47">
+    <row r="102" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="46">
         <v>2</v>
       </c>
-      <c r="B100" s="48" t="s">
-        <v>75</v>
-      </c>
-      <c r="G100" s="45">
+      <c r="B102" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="G102" s="44">
         <v>44187</v>
       </c>
     </row>
-    <row r="101" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="47">
+    <row r="103" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="46">
         <v>2</v>
       </c>
-      <c r="B101" s="48" t="s">
-        <v>76</v>
-      </c>
-      <c r="G101" s="45">
+      <c r="B103" s="47" t="s">
+        <v>99</v>
+      </c>
+      <c r="G103" s="44">
         <v>44187</v>
       </c>
     </row>
-    <row r="102" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="47">
+    <row r="104" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="46">
         <v>2</v>
       </c>
-      <c r="B102" s="48" t="s">
-        <v>102</v>
-      </c>
-      <c r="G102" s="45">
+      <c r="B104" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="G104" s="44">
         <v>44187</v>
       </c>
     </row>
-    <row r="103" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="47">
-        <v>2</v>
-      </c>
-      <c r="B103" s="48" t="s">
-        <v>69</v>
-      </c>
-      <c r="G103" s="45">
+    <row r="105" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="46">
+        <v>3</v>
+      </c>
+      <c r="B105" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="G105" s="44">
         <v>44187</v>
       </c>
     </row>
-    <row r="104" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="47">
+    <row r="106" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="46">
         <v>3</v>
       </c>
-      <c r="B104" s="48" t="s">
-        <v>74</v>
-      </c>
-      <c r="G104" s="45">
+      <c r="B106" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="G106" s="44">
         <v>44187</v>
       </c>
     </row>
-    <row r="105" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="47">
+    <row r="107" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="46">
         <v>3</v>
       </c>
-      <c r="B105" s="48" t="s">
-        <v>89</v>
-      </c>
-      <c r="G105" s="45">
+      <c r="B107" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="G107" s="44">
         <v>44187</v>
       </c>
     </row>
-    <row r="106" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="47">
-        <v>3</v>
-      </c>
-      <c r="B106" s="48" t="s">
-        <v>80</v>
-      </c>
-      <c r="G106" s="45">
-        <v>44187</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="3">
-        <v>2</v>
-      </c>
-      <c r="B118" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G118" s="1"/>
-    </row>
-    <row r="119" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A119" s="3">
         <v>2</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G119" s="1"/>
     </row>
-    <row r="120" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A120" s="3">
         <v>2</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G120" s="1"/>
     </row>
-    <row r="121" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A121" s="3">
         <v>2</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G121" s="1"/>
     </row>
-    <row r="122" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A122" s="3">
         <v>2</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G122" s="1"/>
     </row>
-    <row r="123" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A123" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G123" s="1"/>
     </row>
-    <row r="124" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A124" s="3">
         <v>3</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G124" s="1"/>
     </row>
-    <row r="125" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A125" s="3">
         <v>3</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G125" s="1"/>
     </row>
-    <row r="126" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A126" s="3">
         <v>3</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G126" s="1"/>
     </row>
-    <row r="127" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A127" s="3">
         <v>3</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G127" s="1"/>
     </row>
-    <row r="128" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A128" s="3">
         <v>3</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G128" s="1"/>
     </row>
-    <row r="129" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A129" s="3">
         <v>3</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G129" s="1"/>
     </row>
-    <row r="130" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A130" s="3">
         <v>3</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G130" s="1"/>
     </row>
-    <row r="131" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A131" s="3">
         <v>3</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G131" s="1"/>
     </row>
-    <row r="132" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A132" s="3">
         <v>3</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G132" s="1"/>
     </row>
-    <row r="133" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A133" s="3">
         <v>3</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G133" s="1"/>
     </row>
-    <row r="134" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A134" s="3">
         <v>3</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G134" s="1"/>
     </row>
-    <row r="135" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A135" s="3">
         <v>3</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G135" s="1"/>
     </row>
-    <row r="136" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A136" s="3">
         <v>3</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G136" s="1"/>
+    </row>
+    <row r="137" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="3">
+        <v>3</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G137" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>